<commit_message>
add rules and words
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2482D5C8-EDC4-4AC4-BFF8-93BFD36C9927}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E907DB6-52D3-489A-BBB1-F2FC5994B50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="697">
   <si>
     <t>stage</t>
   </si>
@@ -2059,6 +2059,66 @@
   </si>
   <si>
     <t>빌려</t>
+  </si>
+  <si>
+    <t>외모</t>
+  </si>
+  <si>
+    <t>예쁘다</t>
+  </si>
+  <si>
+    <t>귀엽다</t>
+  </si>
+  <si>
+    <t>날씬하다</t>
+  </si>
+  <si>
+    <t>머있다</t>
+  </si>
+  <si>
+    <t>뚱뚱하다</t>
+  </si>
+  <si>
+    <t>잘생기다</t>
+  </si>
+  <si>
+    <t>머리가 길다 / 짧다</t>
+  </si>
+  <si>
+    <t>마르다</t>
+  </si>
+  <si>
+    <t>тощий</t>
+  </si>
+  <si>
+    <t>волосы длинные / короткие</t>
+  </si>
+  <si>
+    <t>красивый</t>
+  </si>
+  <si>
+    <t>толстый</t>
+  </si>
+  <si>
+    <t>внешность</t>
+  </si>
+  <si>
+    <t>милый</t>
+  </si>
+  <si>
+    <t>стройный</t>
+  </si>
+  <si>
+    <t>рост высокий / низкий</t>
+  </si>
+  <si>
+    <t>키가 크다 / 작다</t>
+  </si>
+  <si>
+    <t>красивый (хорошо появился)</t>
+  </si>
+  <si>
+    <t>look</t>
   </si>
 </sst>
 </file>
@@ -2419,11 +2479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:K284"/>
+  <dimension ref="A1:K294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G274" sqref="G274"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J286" sqref="J286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9015,6 +9075,206 @@
         <v>2</v>
       </c>
     </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>677</v>
+      </c>
+      <c r="B285" t="s">
+        <v>690</v>
+      </c>
+      <c r="D285" t="s">
+        <v>696</v>
+      </c>
+      <c r="E285" t="s">
+        <v>690</v>
+      </c>
+      <c r="J285" t="s">
+        <v>64</v>
+      </c>
+      <c r="K285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>678</v>
+      </c>
+      <c r="B286" t="s">
+        <v>688</v>
+      </c>
+      <c r="D286" t="s">
+        <v>696</v>
+      </c>
+      <c r="E286" t="s">
+        <v>690</v>
+      </c>
+      <c r="J286" t="s">
+        <v>302</v>
+      </c>
+      <c r="K286">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>679</v>
+      </c>
+      <c r="B287" t="s">
+        <v>691</v>
+      </c>
+      <c r="D287" t="s">
+        <v>696</v>
+      </c>
+      <c r="E287" t="s">
+        <v>690</v>
+      </c>
+      <c r="J287" t="s">
+        <v>302</v>
+      </c>
+      <c r="K287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>680</v>
+      </c>
+      <c r="B288" t="s">
+        <v>692</v>
+      </c>
+      <c r="D288" t="s">
+        <v>696</v>
+      </c>
+      <c r="E288" t="s">
+        <v>690</v>
+      </c>
+      <c r="J288" t="s">
+        <v>302</v>
+      </c>
+      <c r="K288">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>681</v>
+      </c>
+      <c r="B289" t="s">
+        <v>688</v>
+      </c>
+      <c r="D289" t="s">
+        <v>696</v>
+      </c>
+      <c r="E289" t="s">
+        <v>690</v>
+      </c>
+      <c r="J289" t="s">
+        <v>302</v>
+      </c>
+      <c r="K289">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>694</v>
+      </c>
+      <c r="B290" t="s">
+        <v>693</v>
+      </c>
+      <c r="D290" t="s">
+        <v>696</v>
+      </c>
+      <c r="E290" t="s">
+        <v>690</v>
+      </c>
+      <c r="J290" t="s">
+        <v>302</v>
+      </c>
+      <c r="K290">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>682</v>
+      </c>
+      <c r="B291" t="s">
+        <v>689</v>
+      </c>
+      <c r="D291" t="s">
+        <v>696</v>
+      </c>
+      <c r="E291" t="s">
+        <v>690</v>
+      </c>
+      <c r="J291" t="s">
+        <v>302</v>
+      </c>
+      <c r="K291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>683</v>
+      </c>
+      <c r="B292" t="s">
+        <v>695</v>
+      </c>
+      <c r="D292" t="s">
+        <v>696</v>
+      </c>
+      <c r="E292" t="s">
+        <v>690</v>
+      </c>
+      <c r="J292" t="s">
+        <v>302</v>
+      </c>
+      <c r="K292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>684</v>
+      </c>
+      <c r="B293" t="s">
+        <v>687</v>
+      </c>
+      <c r="D293" t="s">
+        <v>696</v>
+      </c>
+      <c r="E293" t="s">
+        <v>690</v>
+      </c>
+      <c r="J293" t="s">
+        <v>302</v>
+      </c>
+      <c r="K293">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>685</v>
+      </c>
+      <c r="B294" t="s">
+        <v>686</v>
+      </c>
+      <c r="D294" t="s">
+        <v>696</v>
+      </c>
+      <c r="E294" t="s">
+        <v>690</v>
+      </c>
+      <c r="J294" t="s">
+        <v>302</v>
+      </c>
+      <c r="K294">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K204" xr:uid="{D8E1E4CA-BFBB-4D1E-A8FB-B1C7C7615718}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new word and padez
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A5F3D9-B704-4C5D-809F-E1F6F45611C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C518F389-7BED-4C1E-B9C7-EF5DE1E321D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2301" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="812">
   <si>
     <t>stage</t>
   </si>
@@ -2380,6 +2380,90 @@
   </si>
   <si>
     <t>цвет</t>
+  </si>
+  <si>
+    <t>입다</t>
+  </si>
+  <si>
+    <t>надевать (брюки, юбку...)</t>
+  </si>
+  <si>
+    <t>들다</t>
+  </si>
+  <si>
+    <t>держать (сумку)</t>
+  </si>
+  <si>
+    <t>넥타이를 매다</t>
+  </si>
+  <si>
+    <t>носить галстук</t>
+  </si>
+  <si>
+    <t>목도리를 하다</t>
+  </si>
+  <si>
+    <t>завязывать шарф</t>
+  </si>
+  <si>
+    <t>가족</t>
+  </si>
+  <si>
+    <t>дедушка</t>
+  </si>
+  <si>
+    <t>сестра для девушка</t>
+  </si>
+  <si>
+    <t>сестро для мальчика</t>
+  </si>
+  <si>
+    <t>бабушка</t>
+  </si>
+  <si>
+    <t>старший брат для девушка</t>
+  </si>
+  <si>
+    <t>младший брат или сетсра</t>
+  </si>
+  <si>
+    <t>старший брат для мальчика</t>
+  </si>
+  <si>
+    <t>младший брат</t>
+  </si>
+  <si>
+    <t>младшая сестра</t>
+  </si>
+  <si>
+    <t>할아버지</t>
+  </si>
+  <si>
+    <t>언니</t>
+  </si>
+  <si>
+    <t>누나</t>
+  </si>
+  <si>
+    <t>할머니</t>
+  </si>
+  <si>
+    <t>오빠</t>
+  </si>
+  <si>
+    <t>형</t>
+  </si>
+  <si>
+    <t>아버지</t>
+  </si>
+  <si>
+    <t>동생</t>
+  </si>
+  <si>
+    <t>여동생</t>
+  </si>
+  <si>
+    <t>남동생</t>
   </si>
 </sst>
 </file>
@@ -2740,11 +2824,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M331"/>
+  <dimension ref="A1:M346"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B338" sqref="B338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11717,6 +11801,486 @@
         <v>758</v>
       </c>
     </row>
+    <row r="332" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>784</v>
+      </c>
+      <c r="B332" t="s">
+        <v>785</v>
+      </c>
+      <c r="D332" t="s">
+        <v>54</v>
+      </c>
+      <c r="E332" t="s">
+        <v>567</v>
+      </c>
+      <c r="F332" t="s">
+        <v>127</v>
+      </c>
+      <c r="G332" t="s">
+        <v>570</v>
+      </c>
+      <c r="J332" t="s">
+        <v>55</v>
+      </c>
+      <c r="K332">
+        <v>2</v>
+      </c>
+      <c r="L332">
+        <v>7</v>
+      </c>
+      <c r="M332" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="333" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>786</v>
+      </c>
+      <c r="B333" t="s">
+        <v>787</v>
+      </c>
+      <c r="D333" t="s">
+        <v>54</v>
+      </c>
+      <c r="E333" t="s">
+        <v>567</v>
+      </c>
+      <c r="F333" t="s">
+        <v>128</v>
+      </c>
+      <c r="G333" t="s">
+        <v>571</v>
+      </c>
+      <c r="J333" t="s">
+        <v>55</v>
+      </c>
+      <c r="K333">
+        <v>2</v>
+      </c>
+      <c r="L333">
+        <v>7</v>
+      </c>
+      <c r="M333" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="334" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>788</v>
+      </c>
+      <c r="B334" t="s">
+        <v>789</v>
+      </c>
+      <c r="D334" t="s">
+        <v>54</v>
+      </c>
+      <c r="E334" t="s">
+        <v>567</v>
+      </c>
+      <c r="F334" t="s">
+        <v>127</v>
+      </c>
+      <c r="G334" t="s">
+        <v>570</v>
+      </c>
+      <c r="J334" t="s">
+        <v>55</v>
+      </c>
+      <c r="K334">
+        <v>2</v>
+      </c>
+      <c r="L334">
+        <v>7</v>
+      </c>
+      <c r="M334" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>790</v>
+      </c>
+      <c r="B335" t="s">
+        <v>791</v>
+      </c>
+      <c r="D335" t="s">
+        <v>54</v>
+      </c>
+      <c r="E335" t="s">
+        <v>567</v>
+      </c>
+      <c r="F335" t="s">
+        <v>127</v>
+      </c>
+      <c r="G335" t="s">
+        <v>570</v>
+      </c>
+      <c r="J335" t="s">
+        <v>55</v>
+      </c>
+      <c r="K335">
+        <v>2</v>
+      </c>
+      <c r="L335">
+        <v>7</v>
+      </c>
+      <c r="M335" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>792</v>
+      </c>
+      <c r="B336" t="s">
+        <v>591</v>
+      </c>
+      <c r="D336" t="s">
+        <v>589</v>
+      </c>
+      <c r="E336" t="s">
+        <v>588</v>
+      </c>
+      <c r="F336" t="s">
+        <v>590</v>
+      </c>
+      <c r="G336" t="s">
+        <v>591</v>
+      </c>
+      <c r="J336" t="s">
+        <v>64</v>
+      </c>
+      <c r="K336">
+        <v>2</v>
+      </c>
+      <c r="L336">
+        <v>8</v>
+      </c>
+      <c r="M336" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>802</v>
+      </c>
+      <c r="B337" t="s">
+        <v>793</v>
+      </c>
+      <c r="D337" t="s">
+        <v>589</v>
+      </c>
+      <c r="E337" t="s">
+        <v>588</v>
+      </c>
+      <c r="F337" t="s">
+        <v>590</v>
+      </c>
+      <c r="G337" t="s">
+        <v>591</v>
+      </c>
+      <c r="J337" t="s">
+        <v>64</v>
+      </c>
+      <c r="K337">
+        <v>2</v>
+      </c>
+      <c r="L337">
+        <v>8</v>
+      </c>
+      <c r="M337" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>803</v>
+      </c>
+      <c r="B338" t="s">
+        <v>794</v>
+      </c>
+      <c r="D338" t="s">
+        <v>589</v>
+      </c>
+      <c r="E338" t="s">
+        <v>588</v>
+      </c>
+      <c r="F338" t="s">
+        <v>590</v>
+      </c>
+      <c r="G338" t="s">
+        <v>591</v>
+      </c>
+      <c r="J338" t="s">
+        <v>64</v>
+      </c>
+      <c r="K338">
+        <v>2</v>
+      </c>
+      <c r="L338">
+        <v>8</v>
+      </c>
+      <c r="M338" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>804</v>
+      </c>
+      <c r="B339" t="s">
+        <v>795</v>
+      </c>
+      <c r="D339" t="s">
+        <v>589</v>
+      </c>
+      <c r="E339" t="s">
+        <v>588</v>
+      </c>
+      <c r="F339" t="s">
+        <v>590</v>
+      </c>
+      <c r="G339" t="s">
+        <v>591</v>
+      </c>
+      <c r="J339" t="s">
+        <v>64</v>
+      </c>
+      <c r="K339">
+        <v>2</v>
+      </c>
+      <c r="L339">
+        <v>8</v>
+      </c>
+      <c r="M339" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>805</v>
+      </c>
+      <c r="B340" t="s">
+        <v>796</v>
+      </c>
+      <c r="D340" t="s">
+        <v>589</v>
+      </c>
+      <c r="E340" t="s">
+        <v>588</v>
+      </c>
+      <c r="F340" t="s">
+        <v>590</v>
+      </c>
+      <c r="G340" t="s">
+        <v>591</v>
+      </c>
+      <c r="J340" t="s">
+        <v>64</v>
+      </c>
+      <c r="K340">
+        <v>2</v>
+      </c>
+      <c r="L340">
+        <v>8</v>
+      </c>
+      <c r="M340" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>806</v>
+      </c>
+      <c r="B341" t="s">
+        <v>797</v>
+      </c>
+      <c r="D341" t="s">
+        <v>589</v>
+      </c>
+      <c r="E341" t="s">
+        <v>588</v>
+      </c>
+      <c r="F341" t="s">
+        <v>590</v>
+      </c>
+      <c r="G341" t="s">
+        <v>591</v>
+      </c>
+      <c r="J341" t="s">
+        <v>64</v>
+      </c>
+      <c r="K341">
+        <v>2</v>
+      </c>
+      <c r="L341">
+        <v>8</v>
+      </c>
+      <c r="M341" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>807</v>
+      </c>
+      <c r="B342" t="s">
+        <v>799</v>
+      </c>
+      <c r="D342" t="s">
+        <v>589</v>
+      </c>
+      <c r="E342" t="s">
+        <v>588</v>
+      </c>
+      <c r="F342" t="s">
+        <v>590</v>
+      </c>
+      <c r="G342" t="s">
+        <v>591</v>
+      </c>
+      <c r="J342" t="s">
+        <v>64</v>
+      </c>
+      <c r="K342">
+        <v>2</v>
+      </c>
+      <c r="L342">
+        <v>8</v>
+      </c>
+      <c r="M342" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>808</v>
+      </c>
+      <c r="B343" t="s">
+        <v>793</v>
+      </c>
+      <c r="D343" t="s">
+        <v>589</v>
+      </c>
+      <c r="E343" t="s">
+        <v>588</v>
+      </c>
+      <c r="F343" t="s">
+        <v>590</v>
+      </c>
+      <c r="G343" t="s">
+        <v>591</v>
+      </c>
+      <c r="J343" t="s">
+        <v>64</v>
+      </c>
+      <c r="K343">
+        <v>2</v>
+      </c>
+      <c r="L343">
+        <v>8</v>
+      </c>
+      <c r="M343" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>809</v>
+      </c>
+      <c r="B344" t="s">
+        <v>798</v>
+      </c>
+      <c r="D344" t="s">
+        <v>589</v>
+      </c>
+      <c r="E344" t="s">
+        <v>588</v>
+      </c>
+      <c r="F344" t="s">
+        <v>590</v>
+      </c>
+      <c r="G344" t="s">
+        <v>591</v>
+      </c>
+      <c r="J344" t="s">
+        <v>64</v>
+      </c>
+      <c r="K344">
+        <v>2</v>
+      </c>
+      <c r="L344">
+        <v>8</v>
+      </c>
+      <c r="M344" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>810</v>
+      </c>
+      <c r="B345" t="s">
+        <v>800</v>
+      </c>
+      <c r="D345" t="s">
+        <v>589</v>
+      </c>
+      <c r="E345" t="s">
+        <v>588</v>
+      </c>
+      <c r="F345" t="s">
+        <v>590</v>
+      </c>
+      <c r="G345" t="s">
+        <v>591</v>
+      </c>
+      <c r="J345" t="s">
+        <v>64</v>
+      </c>
+      <c r="K345">
+        <v>2</v>
+      </c>
+      <c r="L345">
+        <v>8</v>
+      </c>
+      <c r="M345" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>811</v>
+      </c>
+      <c r="B346" t="s">
+        <v>801</v>
+      </c>
+      <c r="D346" t="s">
+        <v>589</v>
+      </c>
+      <c r="E346" t="s">
+        <v>588</v>
+      </c>
+      <c r="F346" t="s">
+        <v>590</v>
+      </c>
+      <c r="G346" t="s">
+        <v>591</v>
+      </c>
+      <c r="J346" t="s">
+        <v>64</v>
+      </c>
+      <c r="K346">
+        <v>2</v>
+      </c>
+      <c r="L346">
+        <v>8</v>
+      </c>
+      <c r="M346" t="s">
+        <v>758</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M321" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new words and rules
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C518F389-7BED-4C1E-B9C7-EF5DE1E321D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DBC71F-A6E3-40C9-B969-0DD7BA47D9D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="869">
   <si>
     <t>stage</t>
   </si>
@@ -2304,9 +2304,6 @@
     <t>words</t>
   </si>
   <si>
-    <t>word</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -2464,6 +2461,180 @@
   </si>
   <si>
     <t>남동생</t>
+  </si>
+  <si>
+    <t>있다</t>
+  </si>
+  <si>
+    <t>계시다</t>
+  </si>
+  <si>
+    <t>말씀하시다</t>
+  </si>
+  <si>
+    <t>드시다</t>
+  </si>
+  <si>
+    <t>돌아가시다</t>
+  </si>
+  <si>
+    <t>주무시다</t>
+  </si>
+  <si>
+    <t>편찮으시다</t>
+  </si>
+  <si>
+    <t>умирать (вежливо)</t>
+  </si>
+  <si>
+    <t>быть (вежливо)</t>
+  </si>
+  <si>
+    <t>говорит (вежливо)</t>
+  </si>
+  <si>
+    <t>есть (вежливо)</t>
+  </si>
+  <si>
+    <t>быть</t>
+  </si>
+  <si>
+    <t>спать (вежливо)</t>
+  </si>
+  <si>
+    <t>нормальный (вежливо)</t>
+  </si>
+  <si>
+    <t>아름답다</t>
+  </si>
+  <si>
+    <t>경치가 좋다</t>
+  </si>
+  <si>
+    <t>사람들이 친절하다</t>
+  </si>
+  <si>
+    <t>교통이 편리하다</t>
+  </si>
+  <si>
+    <t>교통이 불편하다</t>
+  </si>
+  <si>
+    <t>유명하다</t>
+  </si>
+  <si>
+    <t>공기가 맑다</t>
+  </si>
+  <si>
+    <t>транспорт неудобный</t>
+  </si>
+  <si>
+    <t>транспорт удобный</t>
+  </si>
+  <si>
+    <t>люди вежливые</t>
+  </si>
+  <si>
+    <t>хороший вид (пейзаж)</t>
+  </si>
+  <si>
+    <t>красивый</t>
+  </si>
+  <si>
+    <t>известный</t>
+  </si>
+  <si>
+    <t>воздух свежий</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>강</t>
+  </si>
+  <si>
+    <t>온천</t>
+  </si>
+  <si>
+    <t>민속촌</t>
+  </si>
+  <si>
+    <t>섬</t>
+  </si>
+  <si>
+    <t>폭포</t>
+  </si>
+  <si>
+    <t>호수</t>
+  </si>
+  <si>
+    <t>유적지</t>
+  </si>
+  <si>
+    <t>드라마 촬영지</t>
+  </si>
+  <si>
+    <t>река</t>
+  </si>
+  <si>
+    <t>горячие источники</t>
+  </si>
+  <si>
+    <t>национальная деревня</t>
+  </si>
+  <si>
+    <t>остров</t>
+  </si>
+  <si>
+    <t>водопад</t>
+  </si>
+  <si>
+    <t>озеро</t>
+  </si>
+  <si>
+    <t>исторический памятник</t>
+  </si>
+  <si>
+    <t>место съемок сериала</t>
+  </si>
+  <si>
+    <t>하지만</t>
+  </si>
+  <si>
+    <t>но</t>
+  </si>
+  <si>
+    <t>놀이공원</t>
+  </si>
+  <si>
+    <t>парк развлечений</t>
+  </si>
+  <si>
+    <t>특히</t>
+  </si>
+  <si>
+    <t>особенно</t>
+  </si>
+  <si>
+    <t>글쎄요</t>
+  </si>
+  <si>
+    <t>ну / ммм / что ж</t>
+  </si>
+  <si>
+    <t>곳</t>
+  </si>
+  <si>
+    <t>드라마</t>
+  </si>
+  <si>
+    <t>сериал</t>
+  </si>
+  <si>
+    <t>관심</t>
+  </si>
+  <si>
+    <t>интерес</t>
   </si>
 </sst>
 </file>
@@ -2824,11 +2995,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M346"/>
+  <dimension ref="A1:M375"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A334" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B338" sqref="B338"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2845,7 +3016,7 @@
     <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2888,7 +3059,7 @@
         <v>689</v>
       </c>
       <c r="M1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -5381,7 +5552,7 @@
         <v>1</v>
       </c>
       <c r="M97" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
@@ -10610,7 +10781,7 @@
         <v>6</v>
       </c>
       <c r="M286" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.3">
@@ -10636,7 +10807,7 @@
         <v>6</v>
       </c>
       <c r="M287" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.3">
@@ -10662,7 +10833,7 @@
         <v>6</v>
       </c>
       <c r="M288" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.3">
@@ -10688,7 +10859,7 @@
         <v>6</v>
       </c>
       <c r="M289" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.3">
@@ -10714,7 +10885,7 @@
         <v>6</v>
       </c>
       <c r="M290" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.3">
@@ -10740,7 +10911,7 @@
         <v>6</v>
       </c>
       <c r="M291" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.3">
@@ -10766,7 +10937,7 @@
         <v>6</v>
       </c>
       <c r="M292" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.3">
@@ -10792,7 +10963,7 @@
         <v>6</v>
       </c>
       <c r="M293" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.3">
@@ -10818,7 +10989,7 @@
         <v>6</v>
       </c>
       <c r="M294" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="295" spans="1:13" x14ac:dyDescent="0.3">
@@ -10847,7 +11018,7 @@
         <v>6</v>
       </c>
       <c r="M295" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="296" spans="1:13" x14ac:dyDescent="0.3">
@@ -10873,7 +11044,7 @@
         <v>7</v>
       </c>
       <c r="M296" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="297" spans="1:13" x14ac:dyDescent="0.3">
@@ -10899,7 +11070,7 @@
         <v>6</v>
       </c>
       <c r="M297" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="298" spans="1:13" x14ac:dyDescent="0.3">
@@ -10925,7 +11096,7 @@
         <v>6</v>
       </c>
       <c r="M298" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="299" spans="1:13" x14ac:dyDescent="0.3">
@@ -10951,7 +11122,7 @@
         <v>6</v>
       </c>
       <c r="M299" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="300" spans="1:13" x14ac:dyDescent="0.3">
@@ -10977,7 +11148,7 @@
         <v>6</v>
       </c>
       <c r="M300" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="301" spans="1:13" x14ac:dyDescent="0.3">
@@ -11003,7 +11174,7 @@
         <v>6</v>
       </c>
       <c r="M301" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.3">
@@ -11029,7 +11200,7 @@
         <v>7</v>
       </c>
       <c r="M302" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="303" spans="1:13" x14ac:dyDescent="0.3">
@@ -11037,7 +11208,7 @@
         <v>667</v>
       </c>
       <c r="B303" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C303" t="s">
         <v>685</v>
@@ -11058,7 +11229,7 @@
         <v>7</v>
       </c>
       <c r="M303" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="304" spans="1:13" x14ac:dyDescent="0.3">
@@ -11084,7 +11255,7 @@
         <v>7</v>
       </c>
       <c r="M304" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.3">
@@ -11110,7 +11281,7 @@
         <v>7</v>
       </c>
       <c r="M305" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.3">
@@ -11118,7 +11289,7 @@
         <v>670</v>
       </c>
       <c r="B306" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D306" t="s">
         <v>684</v>
@@ -11136,7 +11307,7 @@
         <v>7</v>
       </c>
       <c r="M306" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.3">
@@ -11162,7 +11333,7 @@
         <v>7</v>
       </c>
       <c r="M307" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.3">
@@ -11188,7 +11359,7 @@
         <v>7</v>
       </c>
       <c r="M308" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.3">
@@ -11214,7 +11385,7 @@
         <v>7</v>
       </c>
       <c r="M309" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.3">
@@ -11240,7 +11411,7 @@
         <v>7</v>
       </c>
       <c r="M310" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.3">
@@ -11266,7 +11437,7 @@
         <v>7</v>
       </c>
       <c r="M311" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.3">
@@ -11292,7 +11463,7 @@
         <v>2</v>
       </c>
       <c r="M312" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.3">
@@ -11318,7 +11489,7 @@
         <v>2</v>
       </c>
       <c r="M313" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.3">
@@ -11344,7 +11515,7 @@
         <v>2</v>
       </c>
       <c r="M314" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.3">
@@ -11370,7 +11541,7 @@
         <v>2</v>
       </c>
       <c r="M315" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.3">
@@ -11396,7 +11567,7 @@
         <v>2</v>
       </c>
       <c r="M316" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="317" spans="1:13" x14ac:dyDescent="0.3">
@@ -11422,7 +11593,7 @@
         <v>2</v>
       </c>
       <c r="M317" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="318" spans="1:13" x14ac:dyDescent="0.3">
@@ -11448,7 +11619,7 @@
         <v>2</v>
       </c>
       <c r="M318" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="319" spans="1:13" x14ac:dyDescent="0.3">
@@ -11480,7 +11651,7 @@
         <v>2</v>
       </c>
       <c r="M319" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="320" spans="1:13" x14ac:dyDescent="0.3">
@@ -11506,7 +11677,7 @@
         <v>2</v>
       </c>
       <c r="M320" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="321" spans="1:13" x14ac:dyDescent="0.3">
@@ -11538,15 +11709,15 @@
         <v>2</v>
       </c>
       <c r="M321" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B322" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D322" t="s">
         <v>54</v>
@@ -11564,21 +11735,21 @@
         <v>7</v>
       </c>
       <c r="M322" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="323" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B323" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D323" t="s">
+        <v>781</v>
+      </c>
+      <c r="E323" t="s">
         <v>782</v>
-      </c>
-      <c r="E323" t="s">
-        <v>783</v>
       </c>
       <c r="J323" t="s">
         <v>64</v>
@@ -11590,21 +11761,21 @@
         <v>7</v>
       </c>
       <c r="M323" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="324" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B324" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D324" t="s">
+        <v>781</v>
+      </c>
+      <c r="E324" t="s">
         <v>782</v>
-      </c>
-      <c r="E324" t="s">
-        <v>783</v>
       </c>
       <c r="J324" t="s">
         <v>64</v>
@@ -11616,15 +11787,15 @@
         <v>7</v>
       </c>
       <c r="M324" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="325" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B325" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D325" t="s">
         <v>127</v>
@@ -11642,15 +11813,15 @@
         <v>7</v>
       </c>
       <c r="M325" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="326" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B326" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D326" t="s">
         <v>96</v>
@@ -11668,15 +11839,15 @@
         <v>7</v>
       </c>
       <c r="M326" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B327" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D327" t="s">
         <v>589</v>
@@ -11694,15 +11865,15 @@
         <v>7</v>
       </c>
       <c r="M327" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="328" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B328" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D328" t="s">
         <v>300</v>
@@ -11720,21 +11891,21 @@
         <v>7</v>
       </c>
       <c r="M328" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B329" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D329" t="s">
+        <v>781</v>
+      </c>
+      <c r="E329" t="s">
         <v>782</v>
-      </c>
-      <c r="E329" t="s">
-        <v>783</v>
       </c>
       <c r="J329" t="s">
         <v>64</v>
@@ -11746,21 +11917,21 @@
         <v>7</v>
       </c>
       <c r="M329" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B330" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D330" t="s">
+        <v>781</v>
+      </c>
+      <c r="E330" t="s">
         <v>782</v>
-      </c>
-      <c r="E330" t="s">
-        <v>783</v>
       </c>
       <c r="J330" t="s">
         <v>64</v>
@@ -11772,15 +11943,15 @@
         <v>7</v>
       </c>
       <c r="M330" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="331" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
+        <v>770</v>
+      </c>
+      <c r="B331" t="s">
         <v>771</v>
-      </c>
-      <c r="B331" t="s">
-        <v>772</v>
       </c>
       <c r="D331" t="s">
         <v>54</v>
@@ -11798,15 +11969,15 @@
         <v>7</v>
       </c>
       <c r="M331" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="332" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
+        <v>783</v>
+      </c>
+      <c r="B332" t="s">
         <v>784</v>
-      </c>
-      <c r="B332" t="s">
-        <v>785</v>
       </c>
       <c r="D332" t="s">
         <v>54</v>
@@ -11830,15 +12001,15 @@
         <v>7</v>
       </c>
       <c r="M332" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
+        <v>785</v>
+      </c>
+      <c r="B333" t="s">
         <v>786</v>
-      </c>
-      <c r="B333" t="s">
-        <v>787</v>
       </c>
       <c r="D333" t="s">
         <v>54</v>
@@ -11862,15 +12033,15 @@
         <v>7</v>
       </c>
       <c r="M333" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>787</v>
+      </c>
+      <c r="B334" t="s">
         <v>788</v>
-      </c>
-      <c r="B334" t="s">
-        <v>789</v>
       </c>
       <c r="D334" t="s">
         <v>54</v>
@@ -11894,15 +12065,15 @@
         <v>7</v>
       </c>
       <c r="M334" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="335" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
+        <v>789</v>
+      </c>
+      <c r="B335" t="s">
         <v>790</v>
-      </c>
-      <c r="B335" t="s">
-        <v>791</v>
       </c>
       <c r="D335" t="s">
         <v>54</v>
@@ -11926,12 +12097,12 @@
         <v>7</v>
       </c>
       <c r="M335" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="336" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B336" t="s">
         <v>591</v>
@@ -11958,15 +12129,15 @@
         <v>8</v>
       </c>
       <c r="M336" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B337" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D337" t="s">
         <v>589</v>
@@ -11990,15 +12161,15 @@
         <v>8</v>
       </c>
       <c r="M337" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B338" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D338" t="s">
         <v>589</v>
@@ -12022,15 +12193,15 @@
         <v>8</v>
       </c>
       <c r="M338" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B339" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D339" t="s">
         <v>589</v>
@@ -12054,15 +12225,15 @@
         <v>8</v>
       </c>
       <c r="M339" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B340" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D340" t="s">
         <v>589</v>
@@ -12086,15 +12257,15 @@
         <v>8</v>
       </c>
       <c r="M340" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B341" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D341" t="s">
         <v>589</v>
@@ -12118,15 +12289,15 @@
         <v>8</v>
       </c>
       <c r="M341" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B342" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D342" t="s">
         <v>589</v>
@@ -12150,15 +12321,15 @@
         <v>8</v>
       </c>
       <c r="M342" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B343" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D343" t="s">
         <v>589</v>
@@ -12182,15 +12353,15 @@
         <v>8</v>
       </c>
       <c r="M343" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B344" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D344" t="s">
         <v>589</v>
@@ -12214,15 +12385,15 @@
         <v>8</v>
       </c>
       <c r="M344" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B345" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D345" t="s">
         <v>589</v>
@@ -12246,15 +12417,15 @@
         <v>8</v>
       </c>
       <c r="M345" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B346" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D346" t="s">
         <v>589</v>
@@ -12278,7 +12449,761 @@
         <v>8</v>
       </c>
       <c r="M346" t="s">
-        <v>758</v>
+        <v>757</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>811</v>
+      </c>
+      <c r="B347" t="s">
+        <v>822</v>
+      </c>
+      <c r="D347" t="s">
+        <v>300</v>
+      </c>
+      <c r="E347" t="s">
+        <v>578</v>
+      </c>
+      <c r="J347" t="s">
+        <v>55</v>
+      </c>
+      <c r="K347">
+        <v>1</v>
+      </c>
+      <c r="L347">
+        <v>1</v>
+      </c>
+      <c r="M347" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>812</v>
+      </c>
+      <c r="B348" t="s">
+        <v>819</v>
+      </c>
+      <c r="D348" t="s">
+        <v>300</v>
+      </c>
+      <c r="E348" t="s">
+        <v>578</v>
+      </c>
+      <c r="J348" t="s">
+        <v>55</v>
+      </c>
+      <c r="K348">
+        <v>2</v>
+      </c>
+      <c r="L348">
+        <v>8</v>
+      </c>
+      <c r="M348" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>813</v>
+      </c>
+      <c r="B349" t="s">
+        <v>820</v>
+      </c>
+      <c r="D349" t="s">
+        <v>752</v>
+      </c>
+      <c r="E349" t="s">
+        <v>753</v>
+      </c>
+      <c r="J349" t="s">
+        <v>55</v>
+      </c>
+      <c r="K349">
+        <v>2</v>
+      </c>
+      <c r="L349">
+        <v>8</v>
+      </c>
+      <c r="M349" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>814</v>
+      </c>
+      <c r="B350" t="s">
+        <v>821</v>
+      </c>
+      <c r="D350" t="s">
+        <v>54</v>
+      </c>
+      <c r="E350" t="s">
+        <v>567</v>
+      </c>
+      <c r="J350" t="s">
+        <v>55</v>
+      </c>
+      <c r="K350">
+        <v>2</v>
+      </c>
+      <c r="L350">
+        <v>8</v>
+      </c>
+      <c r="M350" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>815</v>
+      </c>
+      <c r="B351" t="s">
+        <v>818</v>
+      </c>
+      <c r="D351" t="s">
+        <v>54</v>
+      </c>
+      <c r="E351" t="s">
+        <v>567</v>
+      </c>
+      <c r="J351" t="s">
+        <v>55</v>
+      </c>
+      <c r="K351">
+        <v>2</v>
+      </c>
+      <c r="L351">
+        <v>8</v>
+      </c>
+      <c r="M351" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>816</v>
+      </c>
+      <c r="B352" t="s">
+        <v>823</v>
+      </c>
+      <c r="D352" t="s">
+        <v>54</v>
+      </c>
+      <c r="E352" t="s">
+        <v>567</v>
+      </c>
+      <c r="J352" t="s">
+        <v>55</v>
+      </c>
+      <c r="K352">
+        <v>2</v>
+      </c>
+      <c r="L352">
+        <v>8</v>
+      </c>
+      <c r="M352" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>817</v>
+      </c>
+      <c r="B353" t="s">
+        <v>824</v>
+      </c>
+      <c r="D353" t="s">
+        <v>300</v>
+      </c>
+      <c r="E353" t="s">
+        <v>578</v>
+      </c>
+      <c r="J353" t="s">
+        <v>301</v>
+      </c>
+      <c r="K353">
+        <v>2</v>
+      </c>
+      <c r="L353">
+        <v>8</v>
+      </c>
+      <c r="M353" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>825</v>
+      </c>
+      <c r="B354" t="s">
+        <v>836</v>
+      </c>
+      <c r="D354" t="s">
+        <v>300</v>
+      </c>
+      <c r="E354" t="s">
+        <v>578</v>
+      </c>
+      <c r="J354" t="s">
+        <v>301</v>
+      </c>
+      <c r="K354">
+        <v>2</v>
+      </c>
+      <c r="L354">
+        <v>9</v>
+      </c>
+      <c r="M354" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>826</v>
+      </c>
+      <c r="B355" t="s">
+        <v>835</v>
+      </c>
+      <c r="D355" t="s">
+        <v>300</v>
+      </c>
+      <c r="E355" t="s">
+        <v>578</v>
+      </c>
+      <c r="J355" t="s">
+        <v>301</v>
+      </c>
+      <c r="K355">
+        <v>2</v>
+      </c>
+      <c r="L355">
+        <v>9</v>
+      </c>
+      <c r="M355" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>827</v>
+      </c>
+      <c r="B356" t="s">
+        <v>834</v>
+      </c>
+      <c r="D356" t="s">
+        <v>589</v>
+      </c>
+      <c r="E356" t="s">
+        <v>588</v>
+      </c>
+      <c r="J356" t="s">
+        <v>301</v>
+      </c>
+      <c r="K356">
+        <v>2</v>
+      </c>
+      <c r="L356">
+        <v>9</v>
+      </c>
+      <c r="M356" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>828</v>
+      </c>
+      <c r="B357" t="s">
+        <v>833</v>
+      </c>
+      <c r="D357" t="s">
+        <v>401</v>
+      </c>
+      <c r="E357" t="s">
+        <v>577</v>
+      </c>
+      <c r="J357" t="s">
+        <v>301</v>
+      </c>
+      <c r="K357">
+        <v>2</v>
+      </c>
+      <c r="L357">
+        <v>9</v>
+      </c>
+      <c r="M357" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>829</v>
+      </c>
+      <c r="B358" t="s">
+        <v>832</v>
+      </c>
+      <c r="D358" t="s">
+        <v>401</v>
+      </c>
+      <c r="E358" t="s">
+        <v>577</v>
+      </c>
+      <c r="J358" t="s">
+        <v>301</v>
+      </c>
+      <c r="K358">
+        <v>2</v>
+      </c>
+      <c r="L358">
+        <v>9</v>
+      </c>
+      <c r="M358" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>830</v>
+      </c>
+      <c r="B359" t="s">
+        <v>837</v>
+      </c>
+      <c r="D359" t="s">
+        <v>300</v>
+      </c>
+      <c r="E359" t="s">
+        <v>578</v>
+      </c>
+      <c r="J359" t="s">
+        <v>301</v>
+      </c>
+      <c r="K359">
+        <v>2</v>
+      </c>
+      <c r="L359">
+        <v>9</v>
+      </c>
+      <c r="M359" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>831</v>
+      </c>
+      <c r="B360" t="s">
+        <v>838</v>
+      </c>
+      <c r="D360" t="s">
+        <v>300</v>
+      </c>
+      <c r="E360" t="s">
+        <v>578</v>
+      </c>
+      <c r="J360" t="s">
+        <v>301</v>
+      </c>
+      <c r="K360">
+        <v>2</v>
+      </c>
+      <c r="L360">
+        <v>9</v>
+      </c>
+      <c r="M360" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>840</v>
+      </c>
+      <c r="B361" t="s">
+        <v>848</v>
+      </c>
+      <c r="D361" t="s">
+        <v>96</v>
+      </c>
+      <c r="E361" t="s">
+        <v>569</v>
+      </c>
+      <c r="J361" t="s">
+        <v>64</v>
+      </c>
+      <c r="K361">
+        <v>2</v>
+      </c>
+      <c r="L361">
+        <v>9</v>
+      </c>
+      <c r="M361" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>841</v>
+      </c>
+      <c r="B362" t="s">
+        <v>849</v>
+      </c>
+      <c r="D362" t="s">
+        <v>96</v>
+      </c>
+      <c r="E362" t="s">
+        <v>569</v>
+      </c>
+      <c r="J362" t="s">
+        <v>301</v>
+      </c>
+      <c r="K362">
+        <v>2</v>
+      </c>
+      <c r="L362">
+        <v>9</v>
+      </c>
+      <c r="M362" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="363" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>842</v>
+      </c>
+      <c r="B363" t="s">
+        <v>850</v>
+      </c>
+      <c r="D363" t="s">
+        <v>96</v>
+      </c>
+      <c r="E363" t="s">
+        <v>569</v>
+      </c>
+      <c r="J363" t="s">
+        <v>64</v>
+      </c>
+      <c r="K363">
+        <v>2</v>
+      </c>
+      <c r="L363">
+        <v>9</v>
+      </c>
+      <c r="M363" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>843</v>
+      </c>
+      <c r="B364" t="s">
+        <v>851</v>
+      </c>
+      <c r="D364" t="s">
+        <v>96</v>
+      </c>
+      <c r="E364" t="s">
+        <v>569</v>
+      </c>
+      <c r="J364" t="s">
+        <v>64</v>
+      </c>
+      <c r="K364">
+        <v>2</v>
+      </c>
+      <c r="L364">
+        <v>9</v>
+      </c>
+      <c r="M364" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>844</v>
+      </c>
+      <c r="B365" t="s">
+        <v>852</v>
+      </c>
+      <c r="D365" t="s">
+        <v>96</v>
+      </c>
+      <c r="E365" t="s">
+        <v>569</v>
+      </c>
+      <c r="J365" t="s">
+        <v>64</v>
+      </c>
+      <c r="K365">
+        <v>2</v>
+      </c>
+      <c r="L365">
+        <v>9</v>
+      </c>
+      <c r="M365" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>845</v>
+      </c>
+      <c r="B366" t="s">
+        <v>853</v>
+      </c>
+      <c r="D366" t="s">
+        <v>96</v>
+      </c>
+      <c r="E366" t="s">
+        <v>569</v>
+      </c>
+      <c r="J366" t="s">
+        <v>64</v>
+      </c>
+      <c r="K366">
+        <v>2</v>
+      </c>
+      <c r="L366">
+        <v>9</v>
+      </c>
+      <c r="M366" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="367" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>846</v>
+      </c>
+      <c r="B367" t="s">
+        <v>854</v>
+      </c>
+      <c r="D367" t="s">
+        <v>96</v>
+      </c>
+      <c r="E367" t="s">
+        <v>569</v>
+      </c>
+      <c r="J367" t="s">
+        <v>64</v>
+      </c>
+      <c r="K367">
+        <v>2</v>
+      </c>
+      <c r="L367">
+        <v>9</v>
+      </c>
+      <c r="M367" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>847</v>
+      </c>
+      <c r="B368" t="s">
+        <v>855</v>
+      </c>
+      <c r="D368" t="s">
+        <v>96</v>
+      </c>
+      <c r="E368" t="s">
+        <v>569</v>
+      </c>
+      <c r="J368" t="s">
+        <v>64</v>
+      </c>
+      <c r="K368">
+        <v>2</v>
+      </c>
+      <c r="L368">
+        <v>9</v>
+      </c>
+      <c r="M368" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>856</v>
+      </c>
+      <c r="B369" t="s">
+        <v>857</v>
+      </c>
+      <c r="D369" t="s">
+        <v>174</v>
+      </c>
+      <c r="E369" t="s">
+        <v>574</v>
+      </c>
+      <c r="J369" t="s">
+        <v>302</v>
+      </c>
+      <c r="K369">
+        <v>2</v>
+      </c>
+      <c r="L369">
+        <v>9</v>
+      </c>
+      <c r="M369" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>858</v>
+      </c>
+      <c r="B370" t="s">
+        <v>859</v>
+      </c>
+      <c r="D370" t="s">
+        <v>96</v>
+      </c>
+      <c r="E370" t="s">
+        <v>569</v>
+      </c>
+      <c r="J370" t="s">
+        <v>64</v>
+      </c>
+      <c r="K370">
+        <v>2</v>
+      </c>
+      <c r="L370">
+        <v>9</v>
+      </c>
+      <c r="M370" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>860</v>
+      </c>
+      <c r="B371" t="s">
+        <v>861</v>
+      </c>
+      <c r="D371" t="s">
+        <v>174</v>
+      </c>
+      <c r="E371" t="s">
+        <v>574</v>
+      </c>
+      <c r="J371" t="s">
+        <v>302</v>
+      </c>
+      <c r="K371">
+        <v>2</v>
+      </c>
+      <c r="L371">
+        <v>9</v>
+      </c>
+      <c r="M371" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>862</v>
+      </c>
+      <c r="B372" t="s">
+        <v>863</v>
+      </c>
+      <c r="D372" t="s">
+        <v>300</v>
+      </c>
+      <c r="E372" t="s">
+        <v>578</v>
+      </c>
+      <c r="J372" t="s">
+        <v>302</v>
+      </c>
+      <c r="K372">
+        <v>2</v>
+      </c>
+      <c r="L372">
+        <v>9</v>
+      </c>
+      <c r="M372" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="373" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>864</v>
+      </c>
+      <c r="B373" t="s">
+        <v>569</v>
+      </c>
+      <c r="D373" t="s">
+        <v>96</v>
+      </c>
+      <c r="E373" t="s">
+        <v>569</v>
+      </c>
+      <c r="J373" t="s">
+        <v>64</v>
+      </c>
+      <c r="K373">
+        <v>2</v>
+      </c>
+      <c r="L373">
+        <v>9</v>
+      </c>
+      <c r="M373" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="374" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>865</v>
+      </c>
+      <c r="B374" t="s">
+        <v>866</v>
+      </c>
+      <c r="D374" t="s">
+        <v>300</v>
+      </c>
+      <c r="E374" t="s">
+        <v>578</v>
+      </c>
+      <c r="J374" t="s">
+        <v>64</v>
+      </c>
+      <c r="K374">
+        <v>2</v>
+      </c>
+      <c r="L374">
+        <v>9</v>
+      </c>
+      <c r="M374" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="375" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>867</v>
+      </c>
+      <c r="B375" t="s">
+        <v>868</v>
+      </c>
+      <c r="D375" t="s">
+        <v>300</v>
+      </c>
+      <c r="E375" t="s">
+        <v>578</v>
+      </c>
+      <c r="J375" t="s">
+        <v>64</v>
+      </c>
+      <c r="K375">
+        <v>2</v>
+      </c>
+      <c r="L375">
+        <v>9</v>
+      </c>
+      <c r="M375" t="s">
+        <v>757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new word and rules 12 les
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0063696-0F36-41A7-98BE-F01C358F9305}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA05358-D8CC-4624-87D4-4BC7D98402CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="1050">
   <si>
     <t>stage</t>
   </si>
@@ -2845,6 +2845,339 @@
   </si>
   <si>
     <t>annother</t>
+  </si>
+  <si>
+    <t>산물</t>
+  </si>
+  <si>
+    <t>케이크</t>
+  </si>
+  <si>
+    <t>꽃</t>
+  </si>
+  <si>
+    <t>풍선</t>
+  </si>
+  <si>
+    <t>음료수</t>
+  </si>
+  <si>
+    <t>사진기</t>
+  </si>
+  <si>
+    <t>초대장</t>
+  </si>
+  <si>
+    <t>подарок</t>
+  </si>
+  <si>
+    <t>торт</t>
+  </si>
+  <si>
+    <t>цветы</t>
+  </si>
+  <si>
+    <t>воздушный шар</t>
+  </si>
+  <si>
+    <t>напитки</t>
+  </si>
+  <si>
+    <t>фотоаппарат</t>
+  </si>
+  <si>
+    <t>приглашение</t>
+  </si>
+  <si>
+    <t>техника</t>
+  </si>
+  <si>
+    <t>technics</t>
+  </si>
+  <si>
+    <t>모임을 준비하다</t>
+  </si>
+  <si>
+    <t>장소를 예악하다</t>
+  </si>
+  <si>
+    <t>연락을 하다</t>
+  </si>
+  <si>
+    <t>사람들을 초대하다</t>
+  </si>
+  <si>
+    <t>회비를 모으다</t>
+  </si>
+  <si>
+    <t>готовиться к встречи</t>
+  </si>
+  <si>
+    <t>резервировать место</t>
+  </si>
+  <si>
+    <t>связываться (по тел., интернету и т.п.)</t>
+  </si>
+  <si>
+    <t>приглашать людей</t>
+  </si>
+  <si>
+    <t>시간을 정하다</t>
+  </si>
+  <si>
+    <t>определять время</t>
+  </si>
+  <si>
+    <t>собирать взнос</t>
+  </si>
+  <si>
+    <t>празднование дня рождения</t>
+  </si>
+  <si>
+    <t>заканчиваться</t>
+  </si>
+  <si>
+    <t>собираться</t>
+  </si>
+  <si>
+    <t>помогать</t>
+  </si>
+  <si>
+    <t>презентация/творческий вечер</t>
+  </si>
+  <si>
+    <t>сладости</t>
+  </si>
+  <si>
+    <t>уборка</t>
+  </si>
+  <si>
+    <t>один раз</t>
+  </si>
+  <si>
+    <t>мысль</t>
+  </si>
+  <si>
+    <t>конец семестра</t>
+  </si>
+  <si>
+    <t>порядок</t>
+  </si>
+  <si>
+    <t>спортивные соревнования</t>
+  </si>
+  <si>
+    <t>생일 파티</t>
+  </si>
+  <si>
+    <t>끝나다</t>
+  </si>
+  <si>
+    <t>모이다</t>
+  </si>
+  <si>
+    <t>도와주다</t>
+  </si>
+  <si>
+    <t>발표회</t>
+  </si>
+  <si>
+    <t>과자</t>
+  </si>
+  <si>
+    <t>청소</t>
+  </si>
+  <si>
+    <t>한번</t>
+  </si>
+  <si>
+    <t>생각</t>
+  </si>
+  <si>
+    <t>학기 말</t>
+  </si>
+  <si>
+    <t>순서</t>
+  </si>
+  <si>
+    <t>체육 대회</t>
+  </si>
+  <si>
+    <t>크다</t>
+  </si>
+  <si>
+    <t>작다</t>
+  </si>
+  <si>
+    <t>복잡하다</t>
+  </si>
+  <si>
+    <t>단순하다</t>
+  </si>
+  <si>
+    <t>넓다</t>
+  </si>
+  <si>
+    <t>좁다</t>
+  </si>
+  <si>
+    <t>조용하다</t>
+  </si>
+  <si>
+    <t>시끄럽다</t>
+  </si>
+  <si>
+    <t>깨끗하다</t>
+  </si>
+  <si>
+    <t>더럽다</t>
+  </si>
+  <si>
+    <t>большой</t>
+  </si>
+  <si>
+    <t>маленький</t>
+  </si>
+  <si>
+    <t>далекий</t>
+  </si>
+  <si>
+    <t>близкий</t>
+  </si>
+  <si>
+    <t>запутанный</t>
+  </si>
+  <si>
+    <t>простой</t>
+  </si>
+  <si>
+    <t>широкий</t>
+  </si>
+  <si>
+    <t>узкий</t>
+  </si>
+  <si>
+    <t>тихий</t>
+  </si>
+  <si>
+    <t>шумный</t>
+  </si>
+  <si>
+    <t>чистый</t>
+  </si>
+  <si>
+    <t>грязный</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>описание</t>
+  </si>
+  <si>
+    <t>살기 좋다</t>
+  </si>
+  <si>
+    <t>높은 건물이 많다</t>
+  </si>
+  <si>
+    <t>현대적인 도시다</t>
+  </si>
+  <si>
+    <t>분위기가 좋다</t>
+  </si>
+  <si>
+    <t>전통적인 도시다</t>
+  </si>
+  <si>
+    <t>인기가 많다</t>
+  </si>
+  <si>
+    <t>большая популярность</t>
+  </si>
+  <si>
+    <t>это традиционный город</t>
+  </si>
+  <si>
+    <t>хорошая атмосфера</t>
+  </si>
+  <si>
+    <t>это современный город</t>
+  </si>
+  <si>
+    <t>много высоких зданий</t>
+  </si>
+  <si>
+    <t>удобный для проживания</t>
+  </si>
+  <si>
+    <t>시골</t>
+  </si>
+  <si>
+    <t>다르다</t>
+  </si>
+  <si>
+    <t>제일</t>
+  </si>
+  <si>
+    <t>더</t>
+  </si>
+  <si>
+    <t>마을</t>
+  </si>
+  <si>
+    <t>비슷하다</t>
+  </si>
+  <si>
+    <t>뉴스</t>
+  </si>
+  <si>
+    <t>남쪽</t>
+  </si>
+  <si>
+    <t>대도시</t>
+  </si>
+  <si>
+    <t>축제</t>
+  </si>
+  <si>
+    <t>более</t>
+  </si>
+  <si>
+    <t>самый</t>
+  </si>
+  <si>
+    <t>непохожий</t>
+  </si>
+  <si>
+    <t>село</t>
+  </si>
+  <si>
+    <t>деревня</t>
+  </si>
+  <si>
+    <t>похожий</t>
+  </si>
+  <si>
+    <t>новости</t>
+  </si>
+  <si>
+    <t>юг</t>
+  </si>
+  <si>
+    <t>из (среди нескольких)</t>
+  </si>
+  <si>
+    <t>крупный город</t>
+  </si>
+  <si>
+    <t>фестиваль</t>
+  </si>
+  <si>
+    <t>적다</t>
+  </si>
+  <si>
+    <t>мало</t>
   </si>
 </sst>
 </file>
@@ -3205,11 +3538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M411"/>
+  <dimension ref="A1:M467"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="1" topLeftCell="A451" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E464" sqref="E464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14472,6 +14805,1519 @@
         <v>757</v>
       </c>
     </row>
+    <row r="412" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>939</v>
+      </c>
+      <c r="B412" t="s">
+        <v>946</v>
+      </c>
+      <c r="D412" t="s">
+        <v>128</v>
+      </c>
+      <c r="E412" t="s">
+        <v>571</v>
+      </c>
+      <c r="J412" t="s">
+        <v>64</v>
+      </c>
+      <c r="K412">
+        <v>2</v>
+      </c>
+      <c r="L412">
+        <v>11</v>
+      </c>
+      <c r="M412" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="413" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>940</v>
+      </c>
+      <c r="B413" t="s">
+        <v>947</v>
+      </c>
+      <c r="D413" t="s">
+        <v>150</v>
+      </c>
+      <c r="E413" t="s">
+        <v>572</v>
+      </c>
+      <c r="J413" t="s">
+        <v>64</v>
+      </c>
+      <c r="K413">
+        <v>2</v>
+      </c>
+      <c r="L413">
+        <v>11</v>
+      </c>
+      <c r="M413" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="414" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>941</v>
+      </c>
+      <c r="B414" t="s">
+        <v>948</v>
+      </c>
+      <c r="D414" t="s">
+        <v>128</v>
+      </c>
+      <c r="E414" t="s">
+        <v>571</v>
+      </c>
+      <c r="J414" t="s">
+        <v>64</v>
+      </c>
+      <c r="K414">
+        <v>2</v>
+      </c>
+      <c r="L414">
+        <v>11</v>
+      </c>
+      <c r="M414" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="415" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>942</v>
+      </c>
+      <c r="B415" t="s">
+        <v>949</v>
+      </c>
+      <c r="D415" t="s">
+        <v>128</v>
+      </c>
+      <c r="E415" t="s">
+        <v>571</v>
+      </c>
+      <c r="J415" t="s">
+        <v>64</v>
+      </c>
+      <c r="K415">
+        <v>2</v>
+      </c>
+      <c r="L415">
+        <v>11</v>
+      </c>
+      <c r="M415" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="416" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>694</v>
+      </c>
+      <c r="B416" t="s">
+        <v>695</v>
+      </c>
+      <c r="D416" t="s">
+        <v>150</v>
+      </c>
+      <c r="E416" t="s">
+        <v>572</v>
+      </c>
+      <c r="J416" t="s">
+        <v>64</v>
+      </c>
+      <c r="K416">
+        <v>2</v>
+      </c>
+      <c r="L416">
+        <v>11</v>
+      </c>
+      <c r="M416" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="417" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>943</v>
+      </c>
+      <c r="B417" t="s">
+        <v>950</v>
+      </c>
+      <c r="D417" t="s">
+        <v>150</v>
+      </c>
+      <c r="E417" t="s">
+        <v>572</v>
+      </c>
+      <c r="J417" t="s">
+        <v>64</v>
+      </c>
+      <c r="K417">
+        <v>2</v>
+      </c>
+      <c r="L417">
+        <v>11</v>
+      </c>
+      <c r="M417" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="418" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>944</v>
+      </c>
+      <c r="B418" t="s">
+        <v>951</v>
+      </c>
+      <c r="D418" t="s">
+        <v>954</v>
+      </c>
+      <c r="E418" t="s">
+        <v>953</v>
+      </c>
+      <c r="J418" t="s">
+        <v>64</v>
+      </c>
+      <c r="K418">
+        <v>2</v>
+      </c>
+      <c r="L418">
+        <v>11</v>
+      </c>
+      <c r="M418" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="419" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>945</v>
+      </c>
+      <c r="B419" t="s">
+        <v>952</v>
+      </c>
+      <c r="D419" t="s">
+        <v>128</v>
+      </c>
+      <c r="E419" t="s">
+        <v>571</v>
+      </c>
+      <c r="J419" t="s">
+        <v>64</v>
+      </c>
+      <c r="K419">
+        <v>2</v>
+      </c>
+      <c r="L419">
+        <v>11</v>
+      </c>
+      <c r="M419" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="420" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>955</v>
+      </c>
+      <c r="B420" t="s">
+        <v>960</v>
+      </c>
+      <c r="D420" t="s">
+        <v>54</v>
+      </c>
+      <c r="E420" t="s">
+        <v>567</v>
+      </c>
+      <c r="K420">
+        <v>2</v>
+      </c>
+      <c r="L420">
+        <v>11</v>
+      </c>
+      <c r="M420" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="421" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>956</v>
+      </c>
+      <c r="B421" t="s">
+        <v>961</v>
+      </c>
+      <c r="D421" t="s">
+        <v>54</v>
+      </c>
+      <c r="E421" t="s">
+        <v>567</v>
+      </c>
+      <c r="K421">
+        <v>2</v>
+      </c>
+      <c r="L421">
+        <v>11</v>
+      </c>
+      <c r="M421" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="422" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>957</v>
+      </c>
+      <c r="B422" t="s">
+        <v>962</v>
+      </c>
+      <c r="D422" t="s">
+        <v>54</v>
+      </c>
+      <c r="E422" t="s">
+        <v>567</v>
+      </c>
+      <c r="K422">
+        <v>2</v>
+      </c>
+      <c r="L422">
+        <v>11</v>
+      </c>
+      <c r="M422" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="423" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>958</v>
+      </c>
+      <c r="B423" t="s">
+        <v>963</v>
+      </c>
+      <c r="D423" t="s">
+        <v>54</v>
+      </c>
+      <c r="E423" t="s">
+        <v>567</v>
+      </c>
+      <c r="K423">
+        <v>2</v>
+      </c>
+      <c r="L423">
+        <v>11</v>
+      </c>
+      <c r="M423" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="424" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>964</v>
+      </c>
+      <c r="B424" t="s">
+        <v>965</v>
+      </c>
+      <c r="D424" t="s">
+        <v>54</v>
+      </c>
+      <c r="E424" t="s">
+        <v>567</v>
+      </c>
+      <c r="K424">
+        <v>2</v>
+      </c>
+      <c r="L424">
+        <v>11</v>
+      </c>
+      <c r="M424" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="425" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>959</v>
+      </c>
+      <c r="B425" t="s">
+        <v>966</v>
+      </c>
+      <c r="D425" t="s">
+        <v>54</v>
+      </c>
+      <c r="E425" t="s">
+        <v>567</v>
+      </c>
+      <c r="K425">
+        <v>2</v>
+      </c>
+      <c r="L425">
+        <v>11</v>
+      </c>
+      <c r="M425" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="426" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>979</v>
+      </c>
+      <c r="B426" t="s">
+        <v>967</v>
+      </c>
+      <c r="D426" t="s">
+        <v>54</v>
+      </c>
+      <c r="E426" t="s">
+        <v>567</v>
+      </c>
+      <c r="K426">
+        <v>2</v>
+      </c>
+      <c r="L426">
+        <v>11</v>
+      </c>
+      <c r="M426" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="427" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>980</v>
+      </c>
+      <c r="B427" t="s">
+        <v>968</v>
+      </c>
+      <c r="D427" t="s">
+        <v>300</v>
+      </c>
+      <c r="E427" t="s">
+        <v>578</v>
+      </c>
+      <c r="J427" t="s">
+        <v>55</v>
+      </c>
+      <c r="K427">
+        <v>2</v>
+      </c>
+      <c r="L427">
+        <v>11</v>
+      </c>
+      <c r="M427" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="428" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>981</v>
+      </c>
+      <c r="B428" t="s">
+        <v>969</v>
+      </c>
+      <c r="D428" t="s">
+        <v>54</v>
+      </c>
+      <c r="E428" t="s">
+        <v>567</v>
+      </c>
+      <c r="J428" t="s">
+        <v>55</v>
+      </c>
+      <c r="K428">
+        <v>2</v>
+      </c>
+      <c r="L428">
+        <v>11</v>
+      </c>
+      <c r="M428" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="429" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>982</v>
+      </c>
+      <c r="B429" t="s">
+        <v>970</v>
+      </c>
+      <c r="D429" t="s">
+        <v>54</v>
+      </c>
+      <c r="E429" t="s">
+        <v>567</v>
+      </c>
+      <c r="J429" t="s">
+        <v>55</v>
+      </c>
+      <c r="K429">
+        <v>2</v>
+      </c>
+      <c r="L429">
+        <v>11</v>
+      </c>
+      <c r="M429" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="430" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>983</v>
+      </c>
+      <c r="B430" t="s">
+        <v>971</v>
+      </c>
+      <c r="D430" t="s">
+        <v>300</v>
+      </c>
+      <c r="E430" t="s">
+        <v>578</v>
+      </c>
+      <c r="K430">
+        <v>2</v>
+      </c>
+      <c r="L430">
+        <v>11</v>
+      </c>
+      <c r="M430" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="431" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>984</v>
+      </c>
+      <c r="B431" t="s">
+        <v>972</v>
+      </c>
+      <c r="D431" t="s">
+        <v>150</v>
+      </c>
+      <c r="E431" t="s">
+        <v>572</v>
+      </c>
+      <c r="J431" t="s">
+        <v>64</v>
+      </c>
+      <c r="K431">
+        <v>2</v>
+      </c>
+      <c r="L431">
+        <v>11</v>
+      </c>
+      <c r="M431" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="432" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>985</v>
+      </c>
+      <c r="B432" t="s">
+        <v>973</v>
+      </c>
+      <c r="D432" t="s">
+        <v>54</v>
+      </c>
+      <c r="E432" t="s">
+        <v>567</v>
+      </c>
+      <c r="J432" t="s">
+        <v>64</v>
+      </c>
+      <c r="K432">
+        <v>2</v>
+      </c>
+      <c r="L432">
+        <v>11</v>
+      </c>
+      <c r="M432" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="433" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>986</v>
+      </c>
+      <c r="B433" t="s">
+        <v>974</v>
+      </c>
+      <c r="D433" t="s">
+        <v>586</v>
+      </c>
+      <c r="E433" t="s">
+        <v>587</v>
+      </c>
+      <c r="K433">
+        <v>2</v>
+      </c>
+      <c r="L433">
+        <v>11</v>
+      </c>
+      <c r="M433" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="434" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>987</v>
+      </c>
+      <c r="B434" t="s">
+        <v>975</v>
+      </c>
+      <c r="D434" t="s">
+        <v>300</v>
+      </c>
+      <c r="E434" t="s">
+        <v>578</v>
+      </c>
+      <c r="J434" t="s">
+        <v>64</v>
+      </c>
+      <c r="K434">
+        <v>2</v>
+      </c>
+      <c r="L434">
+        <v>11</v>
+      </c>
+      <c r="M434" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="435" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>988</v>
+      </c>
+      <c r="B435" t="s">
+        <v>976</v>
+      </c>
+      <c r="D435" t="s">
+        <v>332</v>
+      </c>
+      <c r="E435" t="s">
+        <v>575</v>
+      </c>
+      <c r="K435">
+        <v>2</v>
+      </c>
+      <c r="L435">
+        <v>11</v>
+      </c>
+      <c r="M435" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="436" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>989</v>
+      </c>
+      <c r="B436" t="s">
+        <v>977</v>
+      </c>
+      <c r="D436" t="s">
+        <v>300</v>
+      </c>
+      <c r="E436" t="s">
+        <v>578</v>
+      </c>
+      <c r="J436" t="s">
+        <v>64</v>
+      </c>
+      <c r="K436">
+        <v>2</v>
+      </c>
+      <c r="L436">
+        <v>11</v>
+      </c>
+      <c r="M436" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="437" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>990</v>
+      </c>
+      <c r="B437" t="s">
+        <v>978</v>
+      </c>
+      <c r="D437" t="s">
+        <v>54</v>
+      </c>
+      <c r="E437" t="s">
+        <v>567</v>
+      </c>
+      <c r="K437">
+        <v>2</v>
+      </c>
+      <c r="L437">
+        <v>11</v>
+      </c>
+      <c r="M437" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="438" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>991</v>
+      </c>
+      <c r="B438" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D438" t="s">
+        <v>96</v>
+      </c>
+      <c r="E438" t="s">
+        <v>569</v>
+      </c>
+      <c r="F438" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G438" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J438" t="s">
+        <v>301</v>
+      </c>
+      <c r="K438">
+        <v>2</v>
+      </c>
+      <c r="L438">
+        <v>12</v>
+      </c>
+      <c r="M438" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="439" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>992</v>
+      </c>
+      <c r="B439" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D439" t="s">
+        <v>96</v>
+      </c>
+      <c r="E439" t="s">
+        <v>569</v>
+      </c>
+      <c r="F439" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G439" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J439" t="s">
+        <v>301</v>
+      </c>
+      <c r="K439">
+        <v>2</v>
+      </c>
+      <c r="L439">
+        <v>12</v>
+      </c>
+      <c r="M439" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="440" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>619</v>
+      </c>
+      <c r="B440" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D440" t="s">
+        <v>96</v>
+      </c>
+      <c r="E440" t="s">
+        <v>569</v>
+      </c>
+      <c r="F440" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G440" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J440" t="s">
+        <v>301</v>
+      </c>
+      <c r="K440">
+        <v>2</v>
+      </c>
+      <c r="L440">
+        <v>12</v>
+      </c>
+      <c r="M440" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>603</v>
+      </c>
+      <c r="B441" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D441" t="s">
+        <v>96</v>
+      </c>
+      <c r="E441" t="s">
+        <v>569</v>
+      </c>
+      <c r="F441" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G441" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J441" t="s">
+        <v>301</v>
+      </c>
+      <c r="K441">
+        <v>2</v>
+      </c>
+      <c r="L441">
+        <v>12</v>
+      </c>
+      <c r="M441" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="442" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>993</v>
+      </c>
+      <c r="B442" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D442" t="s">
+        <v>96</v>
+      </c>
+      <c r="E442" t="s">
+        <v>569</v>
+      </c>
+      <c r="F442" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G442" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J442" t="s">
+        <v>301</v>
+      </c>
+      <c r="K442">
+        <v>2</v>
+      </c>
+      <c r="L442">
+        <v>12</v>
+      </c>
+      <c r="M442" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="443" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>994</v>
+      </c>
+      <c r="B443" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D443" t="s">
+        <v>96</v>
+      </c>
+      <c r="E443" t="s">
+        <v>569</v>
+      </c>
+      <c r="F443" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G443" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J443" t="s">
+        <v>301</v>
+      </c>
+      <c r="K443">
+        <v>2</v>
+      </c>
+      <c r="L443">
+        <v>12</v>
+      </c>
+      <c r="M443" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="444" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>995</v>
+      </c>
+      <c r="B444" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D444" t="s">
+        <v>96</v>
+      </c>
+      <c r="E444" t="s">
+        <v>569</v>
+      </c>
+      <c r="F444" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G444" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J444" t="s">
+        <v>301</v>
+      </c>
+      <c r="K444">
+        <v>2</v>
+      </c>
+      <c r="L444">
+        <v>12</v>
+      </c>
+      <c r="M444" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="445" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>996</v>
+      </c>
+      <c r="B445" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D445" t="s">
+        <v>96</v>
+      </c>
+      <c r="E445" t="s">
+        <v>569</v>
+      </c>
+      <c r="F445" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G445" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J445" t="s">
+        <v>301</v>
+      </c>
+      <c r="K445">
+        <v>2</v>
+      </c>
+      <c r="L445">
+        <v>12</v>
+      </c>
+      <c r="M445" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="446" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>997</v>
+      </c>
+      <c r="B446" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D446" t="s">
+        <v>96</v>
+      </c>
+      <c r="E446" t="s">
+        <v>569</v>
+      </c>
+      <c r="F446" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G446" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J446" t="s">
+        <v>301</v>
+      </c>
+      <c r="K446">
+        <v>2</v>
+      </c>
+      <c r="L446">
+        <v>12</v>
+      </c>
+      <c r="M446" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="447" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>998</v>
+      </c>
+      <c r="B447" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D447" t="s">
+        <v>96</v>
+      </c>
+      <c r="E447" t="s">
+        <v>569</v>
+      </c>
+      <c r="F447" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G447" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J447" t="s">
+        <v>301</v>
+      </c>
+      <c r="K447">
+        <v>2</v>
+      </c>
+      <c r="L447">
+        <v>12</v>
+      </c>
+      <c r="M447" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="448" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>999</v>
+      </c>
+      <c r="B448" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D448" t="s">
+        <v>96</v>
+      </c>
+      <c r="E448" t="s">
+        <v>569</v>
+      </c>
+      <c r="F448" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G448" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J448" t="s">
+        <v>301</v>
+      </c>
+      <c r="K448">
+        <v>2</v>
+      </c>
+      <c r="L448">
+        <v>12</v>
+      </c>
+      <c r="M448" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="449" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B449" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D449" t="s">
+        <v>96</v>
+      </c>
+      <c r="E449" t="s">
+        <v>569</v>
+      </c>
+      <c r="F449" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G449" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J449" t="s">
+        <v>301</v>
+      </c>
+      <c r="K449">
+        <v>2</v>
+      </c>
+      <c r="L449">
+        <v>12</v>
+      </c>
+      <c r="M449" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="450" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B450" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D450" t="s">
+        <v>96</v>
+      </c>
+      <c r="E450" t="s">
+        <v>569</v>
+      </c>
+      <c r="F450" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G450" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K450">
+        <v>2</v>
+      </c>
+      <c r="L450">
+        <v>12</v>
+      </c>
+      <c r="M450" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="451" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B451" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D451" t="s">
+        <v>96</v>
+      </c>
+      <c r="E451" t="s">
+        <v>569</v>
+      </c>
+      <c r="F451" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G451" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K451">
+        <v>2</v>
+      </c>
+      <c r="L451">
+        <v>12</v>
+      </c>
+      <c r="M451" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="452" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B452" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D452" t="s">
+        <v>96</v>
+      </c>
+      <c r="E452" t="s">
+        <v>569</v>
+      </c>
+      <c r="F452" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G452" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K452">
+        <v>2</v>
+      </c>
+      <c r="L452">
+        <v>12</v>
+      </c>
+      <c r="M452" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="453" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B453" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D453" t="s">
+        <v>96</v>
+      </c>
+      <c r="E453" t="s">
+        <v>569</v>
+      </c>
+      <c r="F453" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G453" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K453">
+        <v>2</v>
+      </c>
+      <c r="L453">
+        <v>12</v>
+      </c>
+      <c r="M453" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="454" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B454" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D454" t="s">
+        <v>96</v>
+      </c>
+      <c r="E454" t="s">
+        <v>569</v>
+      </c>
+      <c r="F454" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G454" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K454">
+        <v>2</v>
+      </c>
+      <c r="L454">
+        <v>12</v>
+      </c>
+      <c r="M454" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="455" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B455" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D455" t="s">
+        <v>96</v>
+      </c>
+      <c r="E455" t="s">
+        <v>569</v>
+      </c>
+      <c r="F455" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G455" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K455">
+        <v>2</v>
+      </c>
+      <c r="L455">
+        <v>12</v>
+      </c>
+      <c r="M455" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="456" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D456" t="s">
+        <v>96</v>
+      </c>
+      <c r="E456" t="s">
+        <v>569</v>
+      </c>
+      <c r="J456" t="s">
+        <v>64</v>
+      </c>
+      <c r="K456">
+        <v>2</v>
+      </c>
+      <c r="L456">
+        <v>12</v>
+      </c>
+      <c r="M456" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="457" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B457" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D457" t="s">
+        <v>300</v>
+      </c>
+      <c r="E457" t="s">
+        <v>578</v>
+      </c>
+      <c r="J457" t="s">
+        <v>301</v>
+      </c>
+      <c r="K457">
+        <v>2</v>
+      </c>
+      <c r="L457">
+        <v>12</v>
+      </c>
+      <c r="M457" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="458" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B458" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D458" t="s">
+        <v>300</v>
+      </c>
+      <c r="E458" t="s">
+        <v>578</v>
+      </c>
+      <c r="J458" t="s">
+        <v>301</v>
+      </c>
+      <c r="K458">
+        <v>2</v>
+      </c>
+      <c r="L458">
+        <v>12</v>
+      </c>
+      <c r="M458" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="459" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B459" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D459" t="s">
+        <v>300</v>
+      </c>
+      <c r="E459" t="s">
+        <v>578</v>
+      </c>
+      <c r="J459" t="s">
+        <v>302</v>
+      </c>
+      <c r="K459">
+        <v>2</v>
+      </c>
+      <c r="L459">
+        <v>12</v>
+      </c>
+      <c r="M459" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="460" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B460" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D460" t="s">
+        <v>96</v>
+      </c>
+      <c r="E460" t="s">
+        <v>569</v>
+      </c>
+      <c r="J460" t="s">
+        <v>64</v>
+      </c>
+      <c r="K460">
+        <v>2</v>
+      </c>
+      <c r="L460">
+        <v>12</v>
+      </c>
+      <c r="M460" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="461" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B461" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D461" t="s">
+        <v>300</v>
+      </c>
+      <c r="E461" t="s">
+        <v>578</v>
+      </c>
+      <c r="J461" t="s">
+        <v>301</v>
+      </c>
+      <c r="K461">
+        <v>2</v>
+      </c>
+      <c r="L461">
+        <v>12</v>
+      </c>
+      <c r="M461" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="462" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A462" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B462" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D462" t="s">
+        <v>300</v>
+      </c>
+      <c r="E462" t="s">
+        <v>578</v>
+      </c>
+      <c r="J462" t="s">
+        <v>64</v>
+      </c>
+      <c r="K462">
+        <v>2</v>
+      </c>
+      <c r="L462">
+        <v>12</v>
+      </c>
+      <c r="M462" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="463" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A463" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B463" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D463" t="s">
+        <v>167</v>
+      </c>
+      <c r="E463" t="s">
+        <v>573</v>
+      </c>
+      <c r="J463" t="s">
+        <v>64</v>
+      </c>
+      <c r="K463">
+        <v>2</v>
+      </c>
+      <c r="L463">
+        <v>12</v>
+      </c>
+      <c r="M463" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="464" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A464" t="s">
+        <v>213</v>
+      </c>
+      <c r="B464" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D464" t="s">
+        <v>300</v>
+      </c>
+      <c r="E464" t="s">
+        <v>578</v>
+      </c>
+      <c r="J464" t="s">
+        <v>302</v>
+      </c>
+      <c r="K464">
+        <v>2</v>
+      </c>
+      <c r="L464">
+        <v>12</v>
+      </c>
+      <c r="M464" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="465" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A465" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B465" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D465" t="s">
+        <v>96</v>
+      </c>
+      <c r="E465" t="s">
+        <v>569</v>
+      </c>
+      <c r="J465" t="s">
+        <v>64</v>
+      </c>
+      <c r="K465">
+        <v>2</v>
+      </c>
+      <c r="L465">
+        <v>12</v>
+      </c>
+      <c r="M465" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="466" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A466" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D466" t="s">
+        <v>96</v>
+      </c>
+      <c r="E466" t="s">
+        <v>569</v>
+      </c>
+      <c r="J466" t="s">
+        <v>64</v>
+      </c>
+      <c r="K466">
+        <v>2</v>
+      </c>
+      <c r="L466">
+        <v>12</v>
+      </c>
+      <c r="M466" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="467" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A467" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B467" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D467" t="s">
+        <v>300</v>
+      </c>
+      <c r="E467" t="s">
+        <v>578</v>
+      </c>
+      <c r="J467" t="s">
+        <v>302</v>
+      </c>
+      <c r="K467">
+        <v>2</v>
+      </c>
+      <c r="L467">
+        <v>12</v>
+      </c>
+      <c r="M467" t="s">
+        <v>757</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M411" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new word and rules 14 end season
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B254BB-A288-407F-ABB1-AA317F2FAA94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8924B124-A170-43EB-89EA-25B59AA789C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="1157">
   <si>
     <t>stage</t>
   </si>
@@ -3325,6 +3325,180 @@
   </si>
   <si>
     <t>связываться (по тел., интернету и т.п. вежливая форма)</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>будущее</t>
+  </si>
+  <si>
+    <t>한국 진구를 라귀다</t>
+  </si>
+  <si>
+    <t>한국으로 여행을 가다</t>
+  </si>
+  <si>
+    <t>한국 회사에 쥐직하다</t>
+  </si>
+  <si>
+    <t>한국 문화에 관심이 있다</t>
+  </si>
+  <si>
+    <t>한국과 무역을 하다</t>
+  </si>
+  <si>
+    <t>한국으로 유학을 가다</t>
+  </si>
+  <si>
+    <t>통역사가 되다</t>
+  </si>
+  <si>
+    <t>번역가가 되다</t>
+  </si>
+  <si>
+    <t>становиться письменным переводчиком</t>
+  </si>
+  <si>
+    <t>встречаться с корейскими друзьями</t>
+  </si>
+  <si>
+    <t>отправляться в путешествие в Корею</t>
+  </si>
+  <si>
+    <t>устраиваться на работу в Корейскую компанию</t>
+  </si>
+  <si>
+    <t>заниматься торговлей с Кореей</t>
+  </si>
+  <si>
+    <t>интересоваться Корейской культурой</t>
+  </si>
+  <si>
+    <t>отправляться на стажировуц в Корею</t>
+  </si>
+  <si>
+    <t>становиться устным переводчиком</t>
+  </si>
+  <si>
+    <t>선생님이 되다</t>
+  </si>
+  <si>
+    <t>꿈을 이루다</t>
+  </si>
+  <si>
+    <t>좋은 사람과 결흔하다</t>
+  </si>
+  <si>
+    <t>성공하다</t>
+  </si>
+  <si>
+    <t>돈을 많이 벌다</t>
+  </si>
+  <si>
+    <t>외국 여행을 가다</t>
+  </si>
+  <si>
+    <t>зарабатывать много денег</t>
+  </si>
+  <si>
+    <t>становиться учителем</t>
+  </si>
+  <si>
+    <t>достигать мечту</t>
+  </si>
+  <si>
+    <t>играть свадьбу с хорошим человеком</t>
+  </si>
+  <si>
+    <t>добиваться успеха</t>
+  </si>
+  <si>
+    <t>отправляться в путешествие за границу</t>
+  </si>
+  <si>
+    <t>양복</t>
+  </si>
+  <si>
+    <t>사업을 하다</t>
+  </si>
+  <si>
+    <t>무역</t>
+  </si>
+  <si>
+    <t>한 살</t>
+  </si>
+  <si>
+    <t>신청하다</t>
+  </si>
+  <si>
+    <t>중급</t>
+  </si>
+  <si>
+    <t>가사</t>
+  </si>
+  <si>
+    <t>торговля</t>
+  </si>
+  <si>
+    <t>деловой костюм</t>
+  </si>
+  <si>
+    <t>заниматься предпринимательством</t>
+  </si>
+  <si>
+    <t>текст</t>
+  </si>
+  <si>
+    <t>средний уровень</t>
+  </si>
+  <si>
+    <t>앉다</t>
+  </si>
+  <si>
+    <t>아이들</t>
+  </si>
+  <si>
+    <t>부자</t>
+  </si>
+  <si>
+    <t>전 세계</t>
+  </si>
+  <si>
+    <t>초급</t>
+  </si>
+  <si>
+    <t>고급</t>
+  </si>
+  <si>
+    <t>весь мир</t>
+  </si>
+  <si>
+    <t>начальный уровень</t>
+  </si>
+  <si>
+    <t>высший уровень</t>
+  </si>
+  <si>
+    <t>один год</t>
+  </si>
+  <si>
+    <t>подавать заявку</t>
+  </si>
+  <si>
+    <t>садиться</t>
+  </si>
+  <si>
+    <t>дети</t>
+  </si>
+  <si>
+    <t>богатый человек</t>
+  </si>
+  <si>
+    <t>год</t>
+  </si>
+  <si>
+    <t>годы</t>
   </si>
 </sst>
 </file>
@@ -3685,17 +3859,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M492"/>
+  <dimension ref="A1:M520"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J492" sqref="J492"/>
+      <pane ySplit="1" topLeftCell="A487" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
@@ -8141,7 +8315,7 @@
         <v>352</v>
       </c>
       <c r="G166" t="s">
-        <v>352</v>
+        <v>1156</v>
       </c>
       <c r="J166" t="s">
         <v>301</v>
@@ -17140,6 +17314,683 @@
       </c>
       <c r="M492" t="s">
         <v>756</v>
+      </c>
+    </row>
+    <row r="493" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B493" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D493" t="s">
+        <v>332</v>
+      </c>
+      <c r="E493" t="s">
+        <v>574</v>
+      </c>
+      <c r="F493" t="s">
+        <v>476</v>
+      </c>
+      <c r="G493" t="s">
+        <v>578</v>
+      </c>
+      <c r="J493" t="s">
+        <v>64</v>
+      </c>
+      <c r="K493">
+        <v>2</v>
+      </c>
+      <c r="L493">
+        <v>14</v>
+      </c>
+      <c r="M493" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="494" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B494" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D494" t="s">
+        <v>300</v>
+      </c>
+      <c r="E494" t="s">
+        <v>577</v>
+      </c>
+      <c r="K494">
+        <v>2</v>
+      </c>
+      <c r="L494">
+        <v>14</v>
+      </c>
+      <c r="M494" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="495" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B495" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D495" t="s">
+        <v>300</v>
+      </c>
+      <c r="E495" t="s">
+        <v>577</v>
+      </c>
+      <c r="K495">
+        <v>2</v>
+      </c>
+      <c r="L495">
+        <v>14</v>
+      </c>
+      <c r="M495" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="496" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B496" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D496" t="s">
+        <v>300</v>
+      </c>
+      <c r="E496" t="s">
+        <v>577</v>
+      </c>
+      <c r="K496">
+        <v>2</v>
+      </c>
+      <c r="L496">
+        <v>14</v>
+      </c>
+      <c r="M496" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="497" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B497" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D497" t="s">
+        <v>300</v>
+      </c>
+      <c r="E497" t="s">
+        <v>577</v>
+      </c>
+      <c r="K497">
+        <v>2</v>
+      </c>
+      <c r="L497">
+        <v>14</v>
+      </c>
+      <c r="M497" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="498" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B498" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D498" t="s">
+        <v>300</v>
+      </c>
+      <c r="E498" t="s">
+        <v>577</v>
+      </c>
+      <c r="K498">
+        <v>2</v>
+      </c>
+      <c r="L498">
+        <v>14</v>
+      </c>
+      <c r="M498" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="499" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B499" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D499" t="s">
+        <v>300</v>
+      </c>
+      <c r="E499" t="s">
+        <v>577</v>
+      </c>
+      <c r="K499">
+        <v>2</v>
+      </c>
+      <c r="L499">
+        <v>14</v>
+      </c>
+      <c r="M499" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="500" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B500" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D500" t="s">
+        <v>300</v>
+      </c>
+      <c r="E500" t="s">
+        <v>577</v>
+      </c>
+      <c r="K500">
+        <v>2</v>
+      </c>
+      <c r="L500">
+        <v>14</v>
+      </c>
+      <c r="M500" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="501" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A501" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B501" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D501" t="s">
+        <v>300</v>
+      </c>
+      <c r="E501" t="s">
+        <v>577</v>
+      </c>
+      <c r="K501">
+        <v>2</v>
+      </c>
+      <c r="L501">
+        <v>14</v>
+      </c>
+      <c r="M501" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="502" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A502" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B502" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D502" t="s">
+        <v>300</v>
+      </c>
+      <c r="E502" t="s">
+        <v>577</v>
+      </c>
+      <c r="K502">
+        <v>2</v>
+      </c>
+      <c r="L502">
+        <v>14</v>
+      </c>
+      <c r="M502" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="503" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A503" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D503" t="s">
+        <v>300</v>
+      </c>
+      <c r="E503" t="s">
+        <v>577</v>
+      </c>
+      <c r="K503">
+        <v>2</v>
+      </c>
+      <c r="L503">
+        <v>14</v>
+      </c>
+      <c r="M503" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="504" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A504" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D504" t="s">
+        <v>300</v>
+      </c>
+      <c r="E504" t="s">
+        <v>577</v>
+      </c>
+      <c r="K504">
+        <v>2</v>
+      </c>
+      <c r="L504">
+        <v>14</v>
+      </c>
+      <c r="M504" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="505" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A505" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B505" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D505" t="s">
+        <v>300</v>
+      </c>
+      <c r="E505" t="s">
+        <v>577</v>
+      </c>
+      <c r="K505">
+        <v>2</v>
+      </c>
+      <c r="L505">
+        <v>14</v>
+      </c>
+      <c r="M505" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="506" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A506" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D506" t="s">
+        <v>300</v>
+      </c>
+      <c r="E506" t="s">
+        <v>577</v>
+      </c>
+      <c r="K506">
+        <v>2</v>
+      </c>
+      <c r="L506">
+        <v>14</v>
+      </c>
+      <c r="M506" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="507" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A507" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B507" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D507" t="s">
+        <v>300</v>
+      </c>
+      <c r="E507" t="s">
+        <v>577</v>
+      </c>
+      <c r="K507">
+        <v>2</v>
+      </c>
+      <c r="L507">
+        <v>14</v>
+      </c>
+      <c r="M507" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="508" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A508" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B508" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D508" t="s">
+        <v>54</v>
+      </c>
+      <c r="E508" t="s">
+        <v>566</v>
+      </c>
+      <c r="J508" t="s">
+        <v>64</v>
+      </c>
+      <c r="K508">
+        <v>2</v>
+      </c>
+      <c r="L508">
+        <v>14</v>
+      </c>
+      <c r="M508" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="509" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A509" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B509" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D509" t="s">
+        <v>127</v>
+      </c>
+      <c r="E509" t="s">
+        <v>569</v>
+      </c>
+      <c r="J509" t="s">
+        <v>64</v>
+      </c>
+      <c r="K509">
+        <v>2</v>
+      </c>
+      <c r="L509">
+        <v>14</v>
+      </c>
+      <c r="M509" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="510" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A510" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B510" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D510" t="s">
+        <v>54</v>
+      </c>
+      <c r="E510" t="s">
+        <v>566</v>
+      </c>
+      <c r="K510">
+        <v>2</v>
+      </c>
+      <c r="L510">
+        <v>14</v>
+      </c>
+      <c r="M510" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="511" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A511" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B511" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D511" t="s">
+        <v>332</v>
+      </c>
+      <c r="E511" t="s">
+        <v>574</v>
+      </c>
+      <c r="F511" t="s">
+        <v>352</v>
+      </c>
+      <c r="G511" t="s">
+        <v>1155</v>
+      </c>
+      <c r="K511">
+        <v>2</v>
+      </c>
+      <c r="L511">
+        <v>14</v>
+      </c>
+      <c r="M511" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="512" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A512" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B512" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D512" t="s">
+        <v>54</v>
+      </c>
+      <c r="E512" t="s">
+        <v>566</v>
+      </c>
+      <c r="K512">
+        <v>2</v>
+      </c>
+      <c r="L512">
+        <v>14</v>
+      </c>
+      <c r="M512" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="513" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A513" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B513" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D513" t="s">
+        <v>300</v>
+      </c>
+      <c r="E513" t="s">
+        <v>577</v>
+      </c>
+      <c r="J513" t="s">
+        <v>64</v>
+      </c>
+      <c r="K513">
+        <v>2</v>
+      </c>
+      <c r="L513">
+        <v>14</v>
+      </c>
+      <c r="M513" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="514" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A514" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D514" t="s">
+        <v>54</v>
+      </c>
+      <c r="E514" t="s">
+        <v>566</v>
+      </c>
+      <c r="J514" t="s">
+        <v>55</v>
+      </c>
+      <c r="K514">
+        <v>2</v>
+      </c>
+      <c r="L514">
+        <v>14</v>
+      </c>
+      <c r="M514" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="515" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A515" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D515" t="s">
+        <v>588</v>
+      </c>
+      <c r="E515" t="s">
+        <v>587</v>
+      </c>
+      <c r="J515" t="s">
+        <v>64</v>
+      </c>
+      <c r="K515">
+        <v>2</v>
+      </c>
+      <c r="L515">
+        <v>14</v>
+      </c>
+      <c r="M515" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="516" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A516" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B516" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D516" t="s">
+        <v>588</v>
+      </c>
+      <c r="E516" t="s">
+        <v>587</v>
+      </c>
+      <c r="J516" t="s">
+        <v>64</v>
+      </c>
+      <c r="K516">
+        <v>2</v>
+      </c>
+      <c r="L516">
+        <v>14</v>
+      </c>
+      <c r="M516" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="517" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A517" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B517" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D517" t="s">
+        <v>167</v>
+      </c>
+      <c r="E517" t="s">
+        <v>568</v>
+      </c>
+      <c r="K517">
+        <v>2</v>
+      </c>
+      <c r="L517">
+        <v>14</v>
+      </c>
+      <c r="M517" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="518" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A518" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B518" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D518" t="s">
+        <v>300</v>
+      </c>
+      <c r="E518" t="s">
+        <v>577</v>
+      </c>
+      <c r="K518">
+        <v>2</v>
+      </c>
+      <c r="L518">
+        <v>14</v>
+      </c>
+      <c r="M518" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="519" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A519" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B519" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D519" t="s">
+        <v>300</v>
+      </c>
+      <c r="E519" t="s">
+        <v>577</v>
+      </c>
+      <c r="K519">
+        <v>2</v>
+      </c>
+      <c r="L519">
+        <v>14</v>
+      </c>
+      <c r="M519" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="520" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A520" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B520" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D520" t="s">
+        <v>300</v>
+      </c>
+      <c r="E520" t="s">
+        <v>577</v>
+      </c>
+      <c r="K520">
+        <v>2</v>
+      </c>
+      <c r="L520">
+        <v>14</v>
+      </c>
+      <c r="M520" t="s">
+        <v>838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new word and rules
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EC7B8E-DE4C-4C5F-A545-2177747E972F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DBE1A1-F3CC-429F-A211-01CABA4FED65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист4" sheetId="4" r:id="rId3"/>
-    <sheet name="Лист5" sheetId="5" r:id="rId4"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId5"/>
+    <sheet name="Лист6" sheetId="6" r:id="rId3"/>
+    <sheet name="Лист4" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист5" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$M$474</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$M$544</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$M$520</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Лист4!$A$1:$E$442</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Лист4!$A$1:$E$442</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10329" uniqueCount="2396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10805" uniqueCount="2524">
   <si>
     <t>stage</t>
   </si>
@@ -7222,13 +7223,397 @@
   </si>
   <si>
     <t>profession</t>
+  </si>
+  <si>
+    <t>은행에/회사에 다니다</t>
+  </si>
+  <si>
+    <t>한국 요리를/구두를/가방을/옷을 만들다</t>
+  </si>
+  <si>
+    <t>대학교에서/대학원에서 한국어를/경영학을/교육학을/법학을 전공하다</t>
+  </si>
+  <si>
+    <t>초등학교에서/중학교에서/고등학교에서/대학교에서 영어를/수학을 가르치다</t>
+  </si>
+  <si>
+    <t>은행에서/회사에서 일하다</t>
+  </si>
+  <si>
+    <t>работать в банке</t>
+  </si>
+  <si>
+    <t>корейскую еду/обувь/сумку/одежду делать своими руками</t>
+  </si>
+  <si>
+    <t>만들다</t>
+  </si>
+  <si>
+    <t>경영하다</t>
+  </si>
+  <si>
+    <t>управлять</t>
+  </si>
+  <si>
+    <t>голова (волосы)</t>
+  </si>
+  <si>
+    <t>경영학</t>
+  </si>
+  <si>
+    <t>менеджмент</t>
+  </si>
+  <si>
+    <t>교육학</t>
+  </si>
+  <si>
+    <t>법학</t>
+  </si>
+  <si>
+    <t>юриспруденция</t>
+  </si>
+  <si>
+    <t>педагогика</t>
+  </si>
+  <si>
+    <t>специализация</t>
+  </si>
+  <si>
+    <t>specialization</t>
+  </si>
+  <si>
+    <t>закон</t>
+  </si>
+  <si>
+    <t>전공하다</t>
+  </si>
+  <si>
+    <t>в университете/в аспирантуре/менеджмент/педагогику/право специализация</t>
+  </si>
+  <si>
+    <t>преподавать</t>
+  </si>
+  <si>
+    <t>младшая школа/средняя школа/старшая школа/преподаю</t>
+  </si>
+  <si>
+    <t>초등학교</t>
+  </si>
+  <si>
+    <t>중학교</t>
+  </si>
+  <si>
+    <t>고등학교</t>
+  </si>
+  <si>
+    <t>старшая школа</t>
+  </si>
+  <si>
+    <t>младшая школа</t>
+  </si>
+  <si>
+    <t>средняя школа</t>
+  </si>
+  <si>
+    <t>학교</t>
+  </si>
+  <si>
+    <t>школа</t>
+  </si>
+  <si>
+    <t>방법</t>
+  </si>
+  <si>
+    <t>способ / метод</t>
+  </si>
+  <si>
+    <t>делать / делать руками</t>
+  </si>
+  <si>
+    <t>приветствовать</t>
+  </si>
+  <si>
+    <t>открывать компанию</t>
+  </si>
+  <si>
+    <t>переезжать</t>
+  </si>
+  <si>
+    <t>이사하다</t>
+  </si>
+  <si>
+    <t>돕다</t>
+  </si>
+  <si>
+    <t>처음</t>
+  </si>
+  <si>
+    <t>지난번</t>
+  </si>
+  <si>
+    <t>впервые</t>
+  </si>
+  <si>
+    <t>в прошлый раз</t>
+  </si>
+  <si>
+    <t>이번</t>
+  </si>
+  <si>
+    <t>в этот раз</t>
+  </si>
+  <si>
+    <t>помнить</t>
+  </si>
+  <si>
+    <t>импортировать</t>
+  </si>
+  <si>
+    <t>театр и кино</t>
+  </si>
+  <si>
+    <t>барабан</t>
+  </si>
+  <si>
+    <t>игра на инструментах</t>
+  </si>
+  <si>
+    <t>ответ на письмо / сообщение</t>
+  </si>
+  <si>
+    <t>기억하다</t>
+  </si>
+  <si>
+    <t>수출하다</t>
+  </si>
+  <si>
+    <t>잘 맞다</t>
+  </si>
+  <si>
+    <t>подходить / хорошо подходить</t>
+  </si>
+  <si>
+    <t>연극영화</t>
+  </si>
+  <si>
+    <t>가요</t>
+  </si>
+  <si>
+    <t>드럼</t>
+  </si>
+  <si>
+    <t>연주</t>
+  </si>
+  <si>
+    <t>답장</t>
+  </si>
+  <si>
+    <t>인사하다</t>
+  </si>
+  <si>
+    <t>회사를 세우다</t>
+  </si>
+  <si>
+    <t>подходить, хорошо подходить</t>
+  </si>
+  <si>
+    <t>ответ на письмо, сообщение</t>
+  </si>
+  <si>
+    <t>축구</t>
+  </si>
+  <si>
+    <t>야구</t>
+  </si>
+  <si>
+    <t>농구</t>
+  </si>
+  <si>
+    <t>배구</t>
+  </si>
+  <si>
+    <t>수영</t>
+  </si>
+  <si>
+    <t>조깅</t>
+  </si>
+  <si>
+    <t>태권도</t>
+  </si>
+  <si>
+    <t>탁구</t>
+  </si>
+  <si>
+    <t>футбол</t>
+  </si>
+  <si>
+    <t>бейсбол</t>
+  </si>
+  <si>
+    <t>плаванье</t>
+  </si>
+  <si>
+    <t>тхеквандо</t>
+  </si>
+  <si>
+    <t>баскетбол</t>
+  </si>
+  <si>
+    <t>волейбол</t>
+  </si>
+  <si>
+    <t>бег</t>
+  </si>
+  <si>
+    <t>пингпонг</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>спорт</t>
+  </si>
+  <si>
+    <t>주로</t>
+  </si>
+  <si>
+    <t>경기</t>
+  </si>
+  <si>
+    <t>싫어하다</t>
+  </si>
+  <si>
+    <t>필요하다</t>
+  </si>
+  <si>
+    <t>나라</t>
+  </si>
+  <si>
+    <t>치우다</t>
+  </si>
+  <si>
+    <t>밭</t>
+  </si>
+  <si>
+    <t>논</t>
+  </si>
+  <si>
+    <t>새롭다</t>
+  </si>
+  <si>
+    <t>목소리</t>
+  </si>
+  <si>
+    <t>соревнование</t>
+  </si>
+  <si>
+    <t>빠르다</t>
+  </si>
+  <si>
+    <t>친하다</t>
+  </si>
+  <si>
+    <t>모습</t>
+  </si>
+  <si>
+    <t>그러나</t>
+  </si>
+  <si>
+    <t>중요하다</t>
+  </si>
+  <si>
+    <t>необходим</t>
+  </si>
+  <si>
+    <t>не нравиться</t>
+  </si>
+  <si>
+    <t>в основном</t>
+  </si>
+  <si>
+    <t>страна</t>
+  </si>
+  <si>
+    <t>перемещать / переносить / убирать</t>
+  </si>
+  <si>
+    <t>annother</t>
+  </si>
+  <si>
+    <t>поле / рисовое поле</t>
+  </si>
+  <si>
+    <t>поле / суходольное поле</t>
+  </si>
+  <si>
+    <t>красивый голос</t>
+  </si>
+  <si>
+    <t>новый</t>
+  </si>
+  <si>
+    <t>закрыт</t>
+  </si>
+  <si>
+    <t>фигура</t>
+  </si>
+  <si>
+    <t>важно</t>
+  </si>
+  <si>
+    <t>встречаться с людьми</t>
+  </si>
+  <si>
+    <t>искать друзей</t>
+  </si>
+  <si>
+    <t>сидеть дома</t>
+  </si>
+  <si>
+    <t>читать книгу</t>
+  </si>
+  <si>
+    <t>общаться в компании людей</t>
+  </si>
+  <si>
+    <t>выходить на прогулку</t>
+  </si>
+  <si>
+    <t>사람을 만나다</t>
+  </si>
+  <si>
+    <t>친구를 사귀다</t>
+  </si>
+  <si>
+    <t>집에 있다</t>
+  </si>
+  <si>
+    <t>побыть одному</t>
+  </si>
+  <si>
+    <t>책을 읽다</t>
+  </si>
+  <si>
+    <t>петь</t>
+  </si>
+  <si>
+    <t>사람들과 어울리다</t>
+  </si>
+  <si>
+    <t>밖에 나가다</t>
+  </si>
+  <si>
+    <t>혼자 시간을 보내다</t>
+  </si>
+  <si>
+    <t>노래를 부르다</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7243,6 +7628,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7265,11 +7663,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -7584,70 +7990,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M528"/>
+  <dimension ref="A1:M592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A507" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H521" sqref="H521"/>
+      <pane ySplit="1" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B592" sqref="B592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="9" width="15.21875" customWidth="1"/>
+    <col min="10" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
     <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>564</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>565</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>757</v>
       </c>
     </row>
@@ -17862,7 +18262,7 @@
         <v>872</v>
       </c>
       <c r="B377" t="s">
-        <v>881</v>
+        <v>2406</v>
       </c>
       <c r="D377" t="s">
         <v>588</v>
@@ -21923,11 +22323,1548 @@
         <v>1</v>
       </c>
       <c r="M528" t="s">
-        <v>756</v>
+        <v>838</v>
+      </c>
+    </row>
+    <row r="529" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A529" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B529" t="s">
+        <v>2401</v>
+      </c>
+      <c r="K529">
+        <v>3</v>
+      </c>
+      <c r="L529">
+        <v>1</v>
+      </c>
+      <c r="M529" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="530" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A530" t="s">
+        <v>2400</v>
+      </c>
+      <c r="B530" t="s">
+        <v>2401</v>
+      </c>
+      <c r="K530">
+        <v>3</v>
+      </c>
+      <c r="L530">
+        <v>1</v>
+      </c>
+      <c r="M530" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="531" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A531" t="s">
+        <v>2397</v>
+      </c>
+      <c r="B531" t="s">
+        <v>2402</v>
+      </c>
+      <c r="K531">
+        <v>3</v>
+      </c>
+      <c r="L531">
+        <v>1</v>
+      </c>
+      <c r="M531" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="532" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A532" t="s">
+        <v>2398</v>
+      </c>
+      <c r="B532" t="s">
+        <v>2417</v>
+      </c>
+      <c r="K532">
+        <v>3</v>
+      </c>
+      <c r="L532">
+        <v>1</v>
+      </c>
+      <c r="M532" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="533" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A533" t="s">
+        <v>2399</v>
+      </c>
+      <c r="B533" t="s">
+        <v>2419</v>
+      </c>
+      <c r="K533">
+        <v>3</v>
+      </c>
+      <c r="L533">
+        <v>1</v>
+      </c>
+      <c r="M533" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="534" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A534" t="s">
+        <v>2403</v>
+      </c>
+      <c r="B534" t="s">
+        <v>2430</v>
+      </c>
+      <c r="D534" t="s">
+        <v>54</v>
+      </c>
+      <c r="E534" t="s">
+        <v>566</v>
+      </c>
+      <c r="J534" t="s">
+        <v>55</v>
+      </c>
+      <c r="K534">
+        <v>3</v>
+      </c>
+      <c r="L534">
+        <v>1</v>
+      </c>
+      <c r="M534" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="535" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A535" t="s">
+        <v>2404</v>
+      </c>
+      <c r="B535" t="s">
+        <v>2405</v>
+      </c>
+      <c r="D535" t="s">
+        <v>54</v>
+      </c>
+      <c r="E535" t="s">
+        <v>566</v>
+      </c>
+      <c r="J535" t="s">
+        <v>55</v>
+      </c>
+      <c r="K535">
+        <v>3</v>
+      </c>
+      <c r="L535">
+        <v>1</v>
+      </c>
+      <c r="M535" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="536" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A536" t="s">
+        <v>640</v>
+      </c>
+      <c r="B536" t="s">
+        <v>2418</v>
+      </c>
+      <c r="D536" t="s">
+        <v>54</v>
+      </c>
+      <c r="E536" t="s">
+        <v>566</v>
+      </c>
+      <c r="J536" t="s">
+        <v>55</v>
+      </c>
+      <c r="K536">
+        <v>3</v>
+      </c>
+      <c r="L536">
+        <v>1</v>
+      </c>
+      <c r="M536" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="537" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A537" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B537" t="s">
+        <v>2415</v>
+      </c>
+      <c r="D537" t="s">
+        <v>300</v>
+      </c>
+      <c r="E537" t="s">
+        <v>577</v>
+      </c>
+      <c r="J537" t="s">
+        <v>64</v>
+      </c>
+      <c r="K537">
+        <v>3</v>
+      </c>
+      <c r="L537">
+        <v>1</v>
+      </c>
+      <c r="M537" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="538" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A538" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B538" t="s">
+        <v>2413</v>
+      </c>
+      <c r="D538" t="s">
+        <v>2414</v>
+      </c>
+      <c r="E538" t="s">
+        <v>2413</v>
+      </c>
+      <c r="J538" t="s">
+        <v>64</v>
+      </c>
+      <c r="K538">
+        <v>3</v>
+      </c>
+      <c r="L538">
+        <v>1</v>
+      </c>
+      <c r="M538" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="539" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A539" t="s">
+        <v>2407</v>
+      </c>
+      <c r="B539" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D539" t="s">
+        <v>2414</v>
+      </c>
+      <c r="E539" t="s">
+        <v>2413</v>
+      </c>
+      <c r="J539" t="s">
+        <v>64</v>
+      </c>
+      <c r="K539">
+        <v>3</v>
+      </c>
+      <c r="L539">
+        <v>1</v>
+      </c>
+      <c r="M539" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="540" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A540" t="s">
+        <v>2409</v>
+      </c>
+      <c r="B540" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D540" t="s">
+        <v>2414</v>
+      </c>
+      <c r="E540" t="s">
+        <v>2413</v>
+      </c>
+      <c r="J540" t="s">
+        <v>64</v>
+      </c>
+      <c r="K540">
+        <v>3</v>
+      </c>
+      <c r="L540">
+        <v>1</v>
+      </c>
+      <c r="M540" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="541" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A541" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B541" t="s">
+        <v>2411</v>
+      </c>
+      <c r="D541" t="s">
+        <v>2414</v>
+      </c>
+      <c r="E541" t="s">
+        <v>2413</v>
+      </c>
+      <c r="J541" t="s">
+        <v>64</v>
+      </c>
+      <c r="K541">
+        <v>3</v>
+      </c>
+      <c r="L541">
+        <v>1</v>
+      </c>
+      <c r="M541" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="542" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A542" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B542" t="s">
+        <v>2424</v>
+      </c>
+      <c r="D542" t="s">
+        <v>96</v>
+      </c>
+      <c r="E542" t="s">
+        <v>568</v>
+      </c>
+      <c r="J542" t="s">
+        <v>64</v>
+      </c>
+      <c r="K542">
+        <v>3</v>
+      </c>
+      <c r="L542">
+        <v>1</v>
+      </c>
+      <c r="M542" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="543" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A543" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B543" t="s">
+        <v>2425</v>
+      </c>
+      <c r="D543" t="s">
+        <v>96</v>
+      </c>
+      <c r="E543" t="s">
+        <v>568</v>
+      </c>
+      <c r="J543" t="s">
+        <v>64</v>
+      </c>
+      <c r="K543">
+        <v>3</v>
+      </c>
+      <c r="L543">
+        <v>1</v>
+      </c>
+      <c r="M543" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="544" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A544" t="s">
+        <v>2422</v>
+      </c>
+      <c r="B544" t="s">
+        <v>2423</v>
+      </c>
+      <c r="D544" t="s">
+        <v>96</v>
+      </c>
+      <c r="E544" t="s">
+        <v>568</v>
+      </c>
+      <c r="J544" t="s">
+        <v>64</v>
+      </c>
+      <c r="K544">
+        <v>3</v>
+      </c>
+      <c r="L544">
+        <v>1</v>
+      </c>
+      <c r="M544" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="545" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A545" t="s">
+        <v>2426</v>
+      </c>
+      <c r="B545" t="s">
+        <v>2427</v>
+      </c>
+      <c r="D545" t="s">
+        <v>96</v>
+      </c>
+      <c r="E545" t="s">
+        <v>568</v>
+      </c>
+      <c r="J545" t="s">
+        <v>64</v>
+      </c>
+      <c r="K545">
+        <v>1</v>
+      </c>
+      <c r="M545" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="546" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A546" t="s">
+        <v>2428</v>
+      </c>
+      <c r="B546" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C546"/>
+      <c r="D546" t="s">
+        <v>54</v>
+      </c>
+      <c r="E546" t="s">
+        <v>566</v>
+      </c>
+      <c r="F546"/>
+      <c r="G546"/>
+      <c r="H546"/>
+      <c r="I546"/>
+      <c r="J546" t="s">
+        <v>55</v>
+      </c>
+      <c r="K546">
+        <v>3</v>
+      </c>
+      <c r="L546">
+        <v>1</v>
+      </c>
+      <c r="M546" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="547" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A547" t="s">
+        <v>2457</v>
+      </c>
+      <c r="B547" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D547" t="s">
+        <v>54</v>
+      </c>
+      <c r="E547" t="s">
+        <v>566</v>
+      </c>
+      <c r="J547" t="s">
+        <v>55</v>
+      </c>
+      <c r="K547">
+        <v>3</v>
+      </c>
+      <c r="L547">
+        <v>1</v>
+      </c>
+      <c r="M547" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="548" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A548" t="s">
+        <v>2458</v>
+      </c>
+      <c r="B548" t="s">
+        <v>2432</v>
+      </c>
+      <c r="D548" t="s">
+        <v>54</v>
+      </c>
+      <c r="E548" t="s">
+        <v>566</v>
+      </c>
+      <c r="J548" t="s">
+        <v>55</v>
+      </c>
+      <c r="K548">
+        <v>3</v>
+      </c>
+      <c r="L548">
+        <v>1</v>
+      </c>
+      <c r="M548" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="549" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A549" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B549" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D549" t="s">
+        <v>54</v>
+      </c>
+      <c r="E549" t="s">
+        <v>566</v>
+      </c>
+      <c r="J549" t="s">
+        <v>55</v>
+      </c>
+      <c r="K549">
+        <v>3</v>
+      </c>
+      <c r="L549">
+        <v>1</v>
+      </c>
+      <c r="M549" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="550" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A550" t="s">
+        <v>2435</v>
+      </c>
+      <c r="B550" t="s">
+        <v>968</v>
+      </c>
+      <c r="D550" t="s">
+        <v>54</v>
+      </c>
+      <c r="E550" t="s">
+        <v>566</v>
+      </c>
+      <c r="J550" t="s">
+        <v>55</v>
+      </c>
+      <c r="K550">
+        <v>3</v>
+      </c>
+      <c r="L550">
+        <v>1</v>
+      </c>
+      <c r="M550" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="551" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A551" t="s">
+        <v>2436</v>
+      </c>
+      <c r="B551" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D551" t="s">
+        <v>332</v>
+      </c>
+      <c r="E551" t="s">
+        <v>574</v>
+      </c>
+      <c r="F551" t="s">
+        <v>476</v>
+      </c>
+      <c r="G551" t="s">
+        <v>578</v>
+      </c>
+      <c r="J551" t="s">
+        <v>302</v>
+      </c>
+      <c r="K551">
+        <v>3</v>
+      </c>
+      <c r="L551">
+        <v>1</v>
+      </c>
+      <c r="M551" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="552" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A552" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B552" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D552" t="s">
+        <v>332</v>
+      </c>
+      <c r="E552" t="s">
+        <v>574</v>
+      </c>
+      <c r="F552" t="s">
+        <v>476</v>
+      </c>
+      <c r="G552" t="s">
+        <v>578</v>
+      </c>
+      <c r="J552" t="s">
+        <v>302</v>
+      </c>
+      <c r="K552">
+        <v>3</v>
+      </c>
+      <c r="L552">
+        <v>1</v>
+      </c>
+      <c r="M552" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="553" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A553" t="s">
+        <v>2440</v>
+      </c>
+      <c r="B553" t="s">
+        <v>2441</v>
+      </c>
+      <c r="D553" t="s">
+        <v>332</v>
+      </c>
+      <c r="E553" t="s">
+        <v>574</v>
+      </c>
+      <c r="F553" t="s">
+        <v>476</v>
+      </c>
+      <c r="G553" t="s">
+        <v>578</v>
+      </c>
+      <c r="J553" t="s">
+        <v>302</v>
+      </c>
+      <c r="K553">
+        <v>3</v>
+      </c>
+      <c r="L553">
+        <v>1</v>
+      </c>
+      <c r="M553" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="554" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A554" t="s">
+        <v>2448</v>
+      </c>
+      <c r="B554" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D554" t="s">
+        <v>54</v>
+      </c>
+      <c r="E554" t="s">
+        <v>566</v>
+      </c>
+      <c r="J554" t="s">
+        <v>55</v>
+      </c>
+      <c r="K554">
+        <v>3</v>
+      </c>
+      <c r="L554">
+        <v>1</v>
+      </c>
+      <c r="M554" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="555" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A555" t="s">
+        <v>2449</v>
+      </c>
+      <c r="B555" t="s">
+        <v>2443</v>
+      </c>
+      <c r="D555" t="s">
+        <v>54</v>
+      </c>
+      <c r="E555" t="s">
+        <v>566</v>
+      </c>
+      <c r="J555" t="s">
+        <v>55</v>
+      </c>
+      <c r="K555">
+        <v>3</v>
+      </c>
+      <c r="L555">
+        <v>1</v>
+      </c>
+      <c r="M555" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="556" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A556" t="s">
+        <v>2450</v>
+      </c>
+      <c r="B556" t="s">
+        <v>2451</v>
+      </c>
+      <c r="D556" t="s">
+        <v>300</v>
+      </c>
+      <c r="E556" t="s">
+        <v>577</v>
+      </c>
+      <c r="J556" t="s">
+        <v>302</v>
+      </c>
+      <c r="K556">
+        <v>3</v>
+      </c>
+      <c r="L556">
+        <v>1</v>
+      </c>
+      <c r="M556" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="557" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A557" t="s">
+        <v>2452</v>
+      </c>
+      <c r="B557" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D557" t="s">
+        <v>300</v>
+      </c>
+      <c r="E557" t="s">
+        <v>577</v>
+      </c>
+      <c r="J557" t="s">
+        <v>64</v>
+      </c>
+      <c r="K557">
+        <v>3</v>
+      </c>
+      <c r="L557">
+        <v>1</v>
+      </c>
+      <c r="M557" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="558" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A558" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D558" t="s">
+        <v>300</v>
+      </c>
+      <c r="E558" t="s">
+        <v>577</v>
+      </c>
+      <c r="J558" t="s">
+        <v>64</v>
+      </c>
+      <c r="K558">
+        <v>3</v>
+      </c>
+      <c r="L558">
+        <v>1</v>
+      </c>
+      <c r="M558" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="559" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A559" t="s">
+        <v>2454</v>
+      </c>
+      <c r="B559" t="s">
+        <v>2445</v>
+      </c>
+      <c r="D559" t="s">
+        <v>128</v>
+      </c>
+      <c r="E559" t="s">
+        <v>570</v>
+      </c>
+      <c r="J559" t="s">
+        <v>64</v>
+      </c>
+      <c r="K559">
+        <v>3</v>
+      </c>
+      <c r="L559">
+        <v>1</v>
+      </c>
+      <c r="M559" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="560" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A560" t="s">
+        <v>2455</v>
+      </c>
+      <c r="B560" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D560" t="s">
+        <v>54</v>
+      </c>
+      <c r="E560" t="s">
+        <v>566</v>
+      </c>
+      <c r="J560" t="s">
+        <v>55</v>
+      </c>
+      <c r="K560">
+        <v>3</v>
+      </c>
+      <c r="L560">
+        <v>1</v>
+      </c>
+      <c r="M560" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="561" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A561" t="s">
+        <v>2456</v>
+      </c>
+      <c r="B561" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D561" t="s">
+        <v>54</v>
+      </c>
+      <c r="E561" t="s">
+        <v>566</v>
+      </c>
+      <c r="J561" t="s">
+        <v>55</v>
+      </c>
+      <c r="K561">
+        <v>3</v>
+      </c>
+      <c r="L561">
+        <v>1</v>
+      </c>
+      <c r="M561" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="562" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A562" t="s">
+        <v>2461</v>
+      </c>
+      <c r="B562" t="s">
+        <v>2469</v>
+      </c>
+      <c r="D562" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E562" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J562" t="s">
+        <v>64</v>
+      </c>
+      <c r="K562">
+        <v>3</v>
+      </c>
+      <c r="L562">
+        <v>2</v>
+      </c>
+      <c r="M562" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="563" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A563" t="s">
+        <v>2462</v>
+      </c>
+      <c r="B563" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D563" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E563" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J563" t="s">
+        <v>64</v>
+      </c>
+      <c r="K563">
+        <v>3</v>
+      </c>
+      <c r="L563">
+        <v>2</v>
+      </c>
+      <c r="M563" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="564" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A564" t="s">
+        <v>2463</v>
+      </c>
+      <c r="B564" t="s">
+        <v>2473</v>
+      </c>
+      <c r="D564" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E564" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J564" t="s">
+        <v>64</v>
+      </c>
+      <c r="K564">
+        <v>3</v>
+      </c>
+      <c r="L564">
+        <v>2</v>
+      </c>
+      <c r="M564" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="565" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A565" t="s">
+        <v>2464</v>
+      </c>
+      <c r="B565" t="s">
+        <v>2474</v>
+      </c>
+      <c r="D565" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E565" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J565" t="s">
+        <v>64</v>
+      </c>
+      <c r="K565">
+        <v>3</v>
+      </c>
+      <c r="L565">
+        <v>2</v>
+      </c>
+      <c r="M565" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="566" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A566" t="s">
+        <v>2465</v>
+      </c>
+      <c r="B566" t="s">
+        <v>2471</v>
+      </c>
+      <c r="D566" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E566" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J566" t="s">
+        <v>64</v>
+      </c>
+      <c r="K566">
+        <v>3</v>
+      </c>
+      <c r="L566">
+        <v>2</v>
+      </c>
+      <c r="M566" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="567" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A567" t="s">
+        <v>2466</v>
+      </c>
+      <c r="B567" t="s">
+        <v>2475</v>
+      </c>
+      <c r="D567" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E567" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J567" t="s">
+        <v>64</v>
+      </c>
+      <c r="K567">
+        <v>3</v>
+      </c>
+      <c r="L567">
+        <v>2</v>
+      </c>
+      <c r="M567" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="568" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A568" t="s">
+        <v>2467</v>
+      </c>
+      <c r="B568" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D568" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E568" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J568" t="s">
+        <v>64</v>
+      </c>
+      <c r="K568">
+        <v>3</v>
+      </c>
+      <c r="L568">
+        <v>2</v>
+      </c>
+      <c r="M568" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="569" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A569" t="s">
+        <v>2468</v>
+      </c>
+      <c r="B569" t="s">
+        <v>2476</v>
+      </c>
+      <c r="D569" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E569" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J569" t="s">
+        <v>64</v>
+      </c>
+      <c r="K569">
+        <v>3</v>
+      </c>
+      <c r="L569">
+        <v>2</v>
+      </c>
+      <c r="M569" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="570" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A570" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B570" t="s">
+        <v>2497</v>
+      </c>
+      <c r="D570" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E570" t="s">
+        <v>577</v>
+      </c>
+      <c r="J570" t="s">
+        <v>302</v>
+      </c>
+      <c r="K570">
+        <v>3</v>
+      </c>
+      <c r="L570">
+        <v>2</v>
+      </c>
+      <c r="M570" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="571" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A571" t="s">
+        <v>2480</v>
+      </c>
+      <c r="B571" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D571" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E571" t="s">
+        <v>2478</v>
+      </c>
+      <c r="J571" t="s">
+        <v>64</v>
+      </c>
+      <c r="K571">
+        <v>3</v>
+      </c>
+      <c r="L571">
+        <v>2</v>
+      </c>
+      <c r="M571" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="572" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A572" t="s">
+        <v>2481</v>
+      </c>
+      <c r="B572" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D572" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E572" t="s">
+        <v>577</v>
+      </c>
+      <c r="J572" t="s">
+        <v>55</v>
+      </c>
+      <c r="K572">
+        <v>3</v>
+      </c>
+      <c r="L572">
+        <v>2</v>
+      </c>
+      <c r="M572" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="573" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A573" t="s">
+        <v>2482</v>
+      </c>
+      <c r="B573" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D573" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E573" t="s">
+        <v>577</v>
+      </c>
+      <c r="J573" t="s">
+        <v>302</v>
+      </c>
+      <c r="K573">
+        <v>3</v>
+      </c>
+      <c r="L573">
+        <v>2</v>
+      </c>
+      <c r="M573" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="574" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A574" t="s">
+        <v>2483</v>
+      </c>
+      <c r="B574" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D574" t="s">
+        <v>96</v>
+      </c>
+      <c r="E574" t="s">
+        <v>568</v>
+      </c>
+      <c r="J574" t="s">
+        <v>64</v>
+      </c>
+      <c r="K574">
+        <v>3</v>
+      </c>
+      <c r="L574">
+        <v>2</v>
+      </c>
+      <c r="M574" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="575" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A575" t="s">
+        <v>2484</v>
+      </c>
+      <c r="B575" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D575" t="s">
+        <v>54</v>
+      </c>
+      <c r="E575" t="s">
+        <v>566</v>
+      </c>
+      <c r="J575" t="s">
+        <v>302</v>
+      </c>
+      <c r="K575">
+        <v>3</v>
+      </c>
+      <c r="L575">
+        <v>2</v>
+      </c>
+      <c r="M575" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="576" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A576" t="s">
+        <v>2485</v>
+      </c>
+      <c r="B576" t="s">
+        <v>2502</v>
+      </c>
+      <c r="D576" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E576" t="s">
+        <v>577</v>
+      </c>
+      <c r="J576" t="s">
+        <v>64</v>
+      </c>
+      <c r="K576">
+        <v>3</v>
+      </c>
+      <c r="L576">
+        <v>2</v>
+      </c>
+      <c r="M576" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="577" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A577" t="s">
+        <v>2486</v>
+      </c>
+      <c r="B577" t="s">
+        <v>2501</v>
+      </c>
+      <c r="D577" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E577" t="s">
+        <v>577</v>
+      </c>
+      <c r="J577" t="s">
+        <v>64</v>
+      </c>
+      <c r="K577">
+        <v>3</v>
+      </c>
+      <c r="L577">
+        <v>2</v>
+      </c>
+      <c r="M577" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="578" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A578" t="s">
+        <v>2487</v>
+      </c>
+      <c r="B578" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D578" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E578" t="s">
+        <v>577</v>
+      </c>
+      <c r="J578" t="s">
+        <v>64</v>
+      </c>
+      <c r="K578">
+        <v>3</v>
+      </c>
+      <c r="L578">
+        <v>2</v>
+      </c>
+      <c r="M578" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="579" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A579" t="s">
+        <v>2488</v>
+      </c>
+      <c r="B579" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D579" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E579" t="s">
+        <v>577</v>
+      </c>
+      <c r="J579" t="s">
+        <v>301</v>
+      </c>
+      <c r="K579">
+        <v>3</v>
+      </c>
+      <c r="L579">
+        <v>2</v>
+      </c>
+      <c r="M579" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="580" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A580" t="s">
+        <v>2490</v>
+      </c>
+      <c r="B580" t="s">
+        <v>923</v>
+      </c>
+      <c r="D580" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E580" t="s">
+        <v>577</v>
+      </c>
+      <c r="J580" t="s">
+        <v>302</v>
+      </c>
+      <c r="K580">
+        <v>3</v>
+      </c>
+      <c r="L580">
+        <v>2</v>
+      </c>
+      <c r="M580" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="581" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A581" t="s">
+        <v>2491</v>
+      </c>
+      <c r="B581" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D581" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E581" t="s">
+        <v>577</v>
+      </c>
+      <c r="J581" t="s">
+        <v>301</v>
+      </c>
+      <c r="K581">
+        <v>3</v>
+      </c>
+      <c r="L581">
+        <v>2</v>
+      </c>
+      <c r="M581" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="582" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A582" t="s">
+        <v>2492</v>
+      </c>
+      <c r="B582" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D582" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E582" t="s">
+        <v>577</v>
+      </c>
+      <c r="J582" t="s">
+        <v>64</v>
+      </c>
+      <c r="K582">
+        <v>3</v>
+      </c>
+      <c r="L582">
+        <v>2</v>
+      </c>
+      <c r="M582" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="583" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A583" t="s">
+        <v>2493</v>
+      </c>
+      <c r="B583" t="s">
+        <v>856</v>
+      </c>
+      <c r="D583" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E583" t="s">
+        <v>577</v>
+      </c>
+      <c r="K583">
+        <v>3</v>
+      </c>
+      <c r="L583">
+        <v>2</v>
+      </c>
+      <c r="M583" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="584" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A584" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B584" t="s">
+        <v>2507</v>
+      </c>
+      <c r="D584" t="s">
+        <v>2500</v>
+      </c>
+      <c r="E584" t="s">
+        <v>577</v>
+      </c>
+      <c r="J584" t="s">
+        <v>302</v>
+      </c>
+      <c r="K584">
+        <v>3</v>
+      </c>
+      <c r="L584">
+        <v>2</v>
+      </c>
+      <c r="M584" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="585" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A585" t="s">
+        <v>2514</v>
+      </c>
+      <c r="B585" t="s">
+        <v>2508</v>
+      </c>
+      <c r="K585">
+        <v>3</v>
+      </c>
+      <c r="L585">
+        <v>2</v>
+      </c>
+      <c r="M585" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="586" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A586" t="s">
+        <v>2515</v>
+      </c>
+      <c r="B586" t="s">
+        <v>2509</v>
+      </c>
+      <c r="K586">
+        <v>3</v>
+      </c>
+      <c r="L586">
+        <v>2</v>
+      </c>
+      <c r="M586" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="587" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A587" t="s">
+        <v>2516</v>
+      </c>
+      <c r="B587" t="s">
+        <v>2510</v>
+      </c>
+      <c r="K587">
+        <v>3</v>
+      </c>
+      <c r="L587">
+        <v>2</v>
+      </c>
+      <c r="M587" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="588" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A588" t="s">
+        <v>2518</v>
+      </c>
+      <c r="B588" t="s">
+        <v>2511</v>
+      </c>
+      <c r="K588">
+        <v>3</v>
+      </c>
+      <c r="L588">
+        <v>2</v>
+      </c>
+      <c r="M588" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="589" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A589" t="s">
+        <v>2520</v>
+      </c>
+      <c r="B589" t="s">
+        <v>2512</v>
+      </c>
+      <c r="K589">
+        <v>3</v>
+      </c>
+      <c r="L589">
+        <v>2</v>
+      </c>
+      <c r="M589" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="590" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A590" t="s">
+        <v>2521</v>
+      </c>
+      <c r="B590" t="s">
+        <v>2513</v>
+      </c>
+    </row>
+    <row r="591" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A591" t="s">
+        <v>2522</v>
+      </c>
+      <c r="B591" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="592" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A592" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B592" t="s">
+        <v>2519</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M474" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}"/>
+  <autoFilter ref="A1:M544" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -36065,6 +38002,581 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D369D01-9764-417F-BDC6-1E0EEA4F2B74}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E1:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2479</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="D1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E1" s="6" t="str">
+        <f>"[['"&amp;A1&amp;"'], ['"&amp;B1&amp;"'], '"&amp;D1&amp;"', '3']"</f>
+        <v>[['주로'], ['в основном'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2480</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2478</v>
+      </c>
+      <c r="E2" s="6" t="str">
+        <f t="shared" ref="E2:E28" si="0">"[['"&amp;A2&amp;"'], ['"&amp;B2&amp;"'], '"&amp;D2&amp;"', '3']"</f>
+        <v>[['경기'], ['соревнование'], 'спорт', '3']</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2481</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D3" t="s">
+        <v>577</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['싫어하다'], ['не нравиться'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2482</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D4" t="s">
+        <v>577</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['필요하다'], ['необходим'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2483</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2498</v>
+      </c>
+      <c r="D5" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['나라'], ['страна'], 'место', '3']</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2484</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D6" t="s">
+        <v>566</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['치우다'], ['перемещать / переносить / убирать'], 'действие', '3']</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2485</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2502</v>
+      </c>
+      <c r="D7" t="s">
+        <v>577</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['밭'], ['поле / суходольное поле'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2486</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2501</v>
+      </c>
+      <c r="D8" t="s">
+        <v>577</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['논'], ['поле / рисовое поле'], 'другое', '3']</v>
+      </c>
+      <c r="J8" t="s">
+        <v>2479</v>
+      </c>
+      <c r="K8" t="s">
+        <v>2497</v>
+      </c>
+      <c r="M8" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2487</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D9" t="s">
+        <v>577</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['새롭다'], ['новый'], 'другое', '3']</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2480</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2489</v>
+      </c>
+      <c r="M9" t="s">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2488</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2503</v>
+      </c>
+      <c r="D10" t="s">
+        <v>577</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['목소리'], ['красивый голос'], 'другое', '3']</v>
+      </c>
+      <c r="J10" t="s">
+        <v>2481</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2496</v>
+      </c>
+      <c r="M10" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2490</v>
+      </c>
+      <c r="B11" t="s">
+        <v>923</v>
+      </c>
+      <c r="D11" t="s">
+        <v>577</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['빠르다'], ['быстро'], 'другое', '3']</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2482</v>
+      </c>
+      <c r="K11" t="s">
+        <v>2495</v>
+      </c>
+      <c r="M11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2491</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2505</v>
+      </c>
+      <c r="D12" t="s">
+        <v>577</v>
+      </c>
+      <c r="E12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['친하다'], ['закрыт'], 'другое', '3']</v>
+      </c>
+      <c r="J12" t="s">
+        <v>2483</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2498</v>
+      </c>
+      <c r="M12" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2492</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D13" t="s">
+        <v>577</v>
+      </c>
+      <c r="E13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['모습'], ['фигура'], 'другое', '3']</v>
+      </c>
+      <c r="J13" t="s">
+        <v>2484</v>
+      </c>
+      <c r="K13" t="s">
+        <v>2499</v>
+      </c>
+      <c r="M13" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2493</v>
+      </c>
+      <c r="B14" t="s">
+        <v>856</v>
+      </c>
+      <c r="D14" t="s">
+        <v>577</v>
+      </c>
+      <c r="E14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['그러나'], ['но'], 'другое', '3']</v>
+      </c>
+      <c r="J14" t="s">
+        <v>2485</v>
+      </c>
+      <c r="K14" t="s">
+        <v>2502</v>
+      </c>
+      <c r="M14" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2507</v>
+      </c>
+      <c r="D15" t="s">
+        <v>577</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['중요하다'], ['важно'], 'другое', '3']</v>
+      </c>
+      <c r="J15" t="s">
+        <v>2486</v>
+      </c>
+      <c r="K15" t="s">
+        <v>2501</v>
+      </c>
+      <c r="M15" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['이사하다'], ['переезжать'], 'действие', '3']</v>
+      </c>
+      <c r="J16" t="s">
+        <v>2487</v>
+      </c>
+      <c r="K16" t="s">
+        <v>2504</v>
+      </c>
+      <c r="M16" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2435</v>
+      </c>
+      <c r="B17" t="s">
+        <v>968</v>
+      </c>
+      <c r="D17" t="s">
+        <v>566</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['돕다'], ['помогать'], 'действие', '3']</v>
+      </c>
+      <c r="J17" t="s">
+        <v>2488</v>
+      </c>
+      <c r="K17" t="s">
+        <v>2503</v>
+      </c>
+      <c r="M17" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2436</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D18" t="s">
+        <v>574</v>
+      </c>
+      <c r="E18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['처음'], ['впервые'], 'время', '3']</v>
+      </c>
+      <c r="J18" t="s">
+        <v>2490</v>
+      </c>
+      <c r="K18" t="s">
+        <v>923</v>
+      </c>
+      <c r="M18" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D19" t="s">
+        <v>574</v>
+      </c>
+      <c r="E19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['지난번'], ['в прошлый раз'], 'время', '3']</v>
+      </c>
+      <c r="J19" t="s">
+        <v>2491</v>
+      </c>
+      <c r="K19" t="s">
+        <v>2505</v>
+      </c>
+      <c r="M19" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>2440</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2441</v>
+      </c>
+      <c r="D20" t="s">
+        <v>574</v>
+      </c>
+      <c r="E20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['이번'], ['в этот раз'], 'время', '3']</v>
+      </c>
+      <c r="J20" t="s">
+        <v>2492</v>
+      </c>
+      <c r="K20" t="s">
+        <v>2506</v>
+      </c>
+      <c r="M20" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2448</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D21" t="s">
+        <v>566</v>
+      </c>
+      <c r="E21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['기억하다'], ['помнить'], 'действие', '3']</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2493</v>
+      </c>
+      <c r="K21" t="s">
+        <v>856</v>
+      </c>
+      <c r="M21" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2449</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2443</v>
+      </c>
+      <c r="D22" t="s">
+        <v>566</v>
+      </c>
+      <c r="E22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['수출하다'], ['импортировать'], 'действие', '3']</v>
+      </c>
+      <c r="J22" t="s">
+        <v>2494</v>
+      </c>
+      <c r="K22" t="s">
+        <v>2507</v>
+      </c>
+      <c r="M22" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2450</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2459</v>
+      </c>
+      <c r="D23" t="s">
+        <v>577</v>
+      </c>
+      <c r="E23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['잘 맞다'], ['подходить, хорошо подходить'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2452</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D24" t="s">
+        <v>577</v>
+      </c>
+      <c r="E24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['연극영화'], ['театр и кино'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D25" t="s">
+        <v>577</v>
+      </c>
+      <c r="E25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['가요'], ['песня'], 'другое', '3']</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2454</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2445</v>
+      </c>
+      <c r="D26" t="s">
+        <v>570</v>
+      </c>
+      <c r="E26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['드럼'], ['барабан'], 'предметы', '3']</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2455</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2446</v>
+      </c>
+      <c r="D27" t="s">
+        <v>566</v>
+      </c>
+      <c r="E27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['연주'], ['игра на инструментах'], 'действие', '3']</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2456</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D28" t="s">
+        <v>566</v>
+      </c>
+      <c r="E28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['답장'], ['ответ на письмо, сообщение'], 'действие', '3']</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F582FB-FB24-4E4A-BE33-1C668F120252}">
   <dimension ref="A1:R442"/>
   <sheetViews>
@@ -48493,7 +51005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCB7588-90EC-49C9-B133-64FD3EA22B11}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -48536,7 +51048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E164134D-7990-49AA-80F1-4EC5269AFD3D}">
   <dimension ref="A1:B292"/>
   <sheetViews>

</xml_diff>

<commit_message>
new word and rules 3-5
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3E4106-2CA5-4904-B23C-E78AAC4FE89E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C7536E-2060-4A83-87ED-C1F5250F3992}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16329" uniqueCount="2777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16335" uniqueCount="2781">
   <si>
     <t>stage</t>
   </si>
@@ -8371,7 +8371,19 @@
     <t>[['활동'], ['деятельность ', 'активность ', 'занятие'], 'досуг', '3']</t>
   </si>
   <si>
-    <t>NULL</t>
+    <t>부모님</t>
+  </si>
+  <si>
+    <t>ролители</t>
+  </si>
+  <si>
+    <t>출장을 가다</t>
+  </si>
+  <si>
+    <t>시험공부를 하다</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -8454,67 +8466,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8550,6 +8502,36 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8863,11 +8845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M686"/>
+  <dimension ref="A1:M687"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A625" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J633" sqref="J633"/>
+      <pane ySplit="1" topLeftCell="A667" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J675" sqref="J675"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19546,8 +19528,8 @@
       <c r="E389" t="s">
         <v>871</v>
       </c>
-      <c r="J389" t="s">
-        <v>2776</v>
+      <c r="J389" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K389">
         <v>2</v>
@@ -19572,8 +19554,8 @@
       <c r="E390" t="s">
         <v>871</v>
       </c>
-      <c r="J390" t="s">
-        <v>2776</v>
+      <c r="J390" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K390">
         <v>2</v>
@@ -20144,8 +20126,8 @@
       <c r="E412" t="s">
         <v>566</v>
       </c>
-      <c r="J412" t="s">
-        <v>2776</v>
+      <c r="J412" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K412">
         <v>2</v>
@@ -20170,8 +20152,8 @@
       <c r="E413" t="s">
         <v>566</v>
       </c>
-      <c r="J413" t="s">
-        <v>2776</v>
+      <c r="J413" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K413">
         <v>2</v>
@@ -20196,8 +20178,8 @@
       <c r="E414" t="s">
         <v>566</v>
       </c>
-      <c r="J414" t="s">
-        <v>2776</v>
+      <c r="J414" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K414">
         <v>2</v>
@@ -20222,8 +20204,8 @@
       <c r="E415" t="s">
         <v>566</v>
       </c>
-      <c r="J415" t="s">
-        <v>2776</v>
+      <c r="J415" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K415">
         <v>2</v>
@@ -20248,8 +20230,8 @@
       <c r="E416" t="s">
         <v>566</v>
       </c>
-      <c r="J416" t="s">
-        <v>2776</v>
+      <c r="J416" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K416">
         <v>2</v>
@@ -20274,8 +20256,8 @@
       <c r="E417" t="s">
         <v>566</v>
       </c>
-      <c r="J417" t="s">
-        <v>2776</v>
+      <c r="J417" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K417">
         <v>2</v>
@@ -20300,8 +20282,8 @@
       <c r="E418" t="s">
         <v>566</v>
       </c>
-      <c r="J418" t="s">
-        <v>2776</v>
+      <c r="J418" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K418">
         <v>2</v>
@@ -20404,8 +20386,8 @@
       <c r="E422" t="s">
         <v>577</v>
       </c>
-      <c r="J422" t="s">
-        <v>2776</v>
+      <c r="J422" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K422">
         <v>2</v>
@@ -20482,8 +20464,8 @@
       <c r="E425" t="s">
         <v>586</v>
       </c>
-      <c r="J425" t="s">
-        <v>2776</v>
+      <c r="J425" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K425">
         <v>2</v>
@@ -20534,8 +20516,8 @@
       <c r="E427" t="s">
         <v>574</v>
       </c>
-      <c r="J427" t="s">
-        <v>2776</v>
+      <c r="J427" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K427">
         <v>2</v>
@@ -20586,8 +20568,8 @@
       <c r="E429" t="s">
         <v>566</v>
       </c>
-      <c r="J429" t="s">
-        <v>2776</v>
+      <c r="J429" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K429">
         <v>2</v>
@@ -20938,8 +20920,8 @@
       <c r="G440" t="s">
         <v>1012</v>
       </c>
-      <c r="J440" t="s">
-        <v>2776</v>
+      <c r="J440" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K440">
         <v>2</v>
@@ -20970,8 +20952,8 @@
       <c r="G441" t="s">
         <v>1012</v>
       </c>
-      <c r="J441" t="s">
-        <v>2776</v>
+      <c r="J441" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K441">
         <v>2</v>
@@ -21002,8 +20984,8 @@
       <c r="G442" t="s">
         <v>1012</v>
       </c>
-      <c r="J442" t="s">
-        <v>2776</v>
+      <c r="J442" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K442">
         <v>2</v>
@@ -21034,8 +21016,8 @@
       <c r="G443" t="s">
         <v>1012</v>
       </c>
-      <c r="J443" t="s">
-        <v>2776</v>
+      <c r="J443" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K443">
         <v>2</v>
@@ -21066,8 +21048,8 @@
       <c r="G444" t="s">
         <v>1012</v>
       </c>
-      <c r="J444" t="s">
-        <v>2776</v>
+      <c r="J444" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K444">
         <v>2</v>
@@ -21098,8 +21080,8 @@
       <c r="G445" t="s">
         <v>1012</v>
       </c>
-      <c r="J445" t="s">
-        <v>2776</v>
+      <c r="J445" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K445">
         <v>2</v>
@@ -21442,8 +21424,8 @@
       <c r="G458" t="s">
         <v>1063</v>
       </c>
-      <c r="J458" t="s">
-        <v>2776</v>
+      <c r="J458" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K458">
         <v>2</v>
@@ -21474,8 +21456,8 @@
       <c r="G459" t="s">
         <v>1063</v>
       </c>
-      <c r="J459" t="s">
-        <v>2776</v>
+      <c r="J459" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K459">
         <v>2</v>
@@ -21634,8 +21616,8 @@
       <c r="G464" t="s">
         <v>1063</v>
       </c>
-      <c r="J464" t="s">
-        <v>2776</v>
+      <c r="J464" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K464">
         <v>2</v>
@@ -21666,8 +21648,8 @@
       <c r="G465" t="s">
         <v>1063</v>
       </c>
-      <c r="J465" t="s">
-        <v>2776</v>
+      <c r="J465" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K465">
         <v>2</v>
@@ -21698,8 +21680,8 @@
       <c r="G466" t="s">
         <v>1063</v>
       </c>
-      <c r="J466" t="s">
-        <v>2776</v>
+      <c r="J466" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K466">
         <v>2</v>
@@ -21724,8 +21706,8 @@
       <c r="E467" t="s">
         <v>566</v>
       </c>
-      <c r="J467" t="s">
-        <v>2776</v>
+      <c r="J467" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K467">
         <v>2</v>
@@ -21750,8 +21732,8 @@
       <c r="E468" t="s">
         <v>566</v>
       </c>
-      <c r="J468" t="s">
-        <v>2776</v>
+      <c r="J468" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K468">
         <v>2</v>
@@ -21776,8 +21758,8 @@
       <c r="E469" t="s">
         <v>566</v>
       </c>
-      <c r="J469" t="s">
-        <v>2776</v>
+      <c r="J469" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K469">
         <v>2</v>
@@ -21802,8 +21784,8 @@
       <c r="E470" t="s">
         <v>566</v>
       </c>
-      <c r="J470" t="s">
-        <v>2776</v>
+      <c r="J470" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K470">
         <v>2</v>
@@ -21984,8 +21966,8 @@
       <c r="E477" t="s">
         <v>577</v>
       </c>
-      <c r="J477" t="s">
-        <v>2776</v>
+      <c r="J477" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K477">
         <v>2</v>
@@ -22048,8 +22030,8 @@
       <c r="G479" t="s">
         <v>1063</v>
       </c>
-      <c r="J479" t="s">
-        <v>2776</v>
+      <c r="J479" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K479">
         <v>2</v>
@@ -22074,8 +22056,8 @@
       <c r="E480" t="s">
         <v>577</v>
       </c>
-      <c r="J480" t="s">
-        <v>2776</v>
+      <c r="J480" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K480">
         <v>2</v>
@@ -22100,8 +22082,8 @@
       <c r="E481" t="s">
         <v>577</v>
       </c>
-      <c r="J481" t="s">
-        <v>2776</v>
+      <c r="J481" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K481">
         <v>2</v>
@@ -22184,8 +22166,8 @@
       <c r="E484" t="s">
         <v>577</v>
       </c>
-      <c r="J484" t="s">
-        <v>2776</v>
+      <c r="J484" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K484">
         <v>2</v>
@@ -22210,8 +22192,8 @@
       <c r="E485" t="s">
         <v>577</v>
       </c>
-      <c r="J485" t="s">
-        <v>2776</v>
+      <c r="J485" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K485">
         <v>2</v>
@@ -22236,8 +22218,8 @@
       <c r="E486" t="s">
         <v>577</v>
       </c>
-      <c r="J486" t="s">
-        <v>2776</v>
+      <c r="J486" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K486">
         <v>2</v>
@@ -22262,8 +22244,8 @@
       <c r="E487" t="s">
         <v>577</v>
       </c>
-      <c r="J487" t="s">
-        <v>2776</v>
+      <c r="J487" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K487">
         <v>2</v>
@@ -22288,8 +22270,8 @@
       <c r="E488" t="s">
         <v>577</v>
       </c>
-      <c r="J488" t="s">
-        <v>2776</v>
+      <c r="J488" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K488">
         <v>2</v>
@@ -22314,8 +22296,8 @@
       <c r="E489" t="s">
         <v>577</v>
       </c>
-      <c r="J489" t="s">
-        <v>2776</v>
+      <c r="J489" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K489">
         <v>2</v>
@@ -22340,8 +22322,8 @@
       <c r="E490" t="s">
         <v>577</v>
       </c>
-      <c r="J490" t="s">
-        <v>2776</v>
+      <c r="J490" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K490">
         <v>2</v>
@@ -22366,8 +22348,8 @@
       <c r="E491" t="s">
         <v>577</v>
       </c>
-      <c r="J491" t="s">
-        <v>2776</v>
+      <c r="J491" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K491">
         <v>2</v>
@@ -22392,8 +22374,8 @@
       <c r="E492" t="s">
         <v>577</v>
       </c>
-      <c r="J492" t="s">
-        <v>2776</v>
+      <c r="J492" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K492">
         <v>2</v>
@@ -22418,8 +22400,8 @@
       <c r="E493" t="s">
         <v>577</v>
       </c>
-      <c r="J493" t="s">
-        <v>2776</v>
+      <c r="J493" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K493">
         <v>2</v>
@@ -22444,8 +22426,8 @@
       <c r="E494" t="s">
         <v>577</v>
       </c>
-      <c r="J494" t="s">
-        <v>2776</v>
+      <c r="J494" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K494">
         <v>2</v>
@@ -22470,8 +22452,8 @@
       <c r="E495" t="s">
         <v>577</v>
       </c>
-      <c r="J495" t="s">
-        <v>2776</v>
+      <c r="J495" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K495">
         <v>2</v>
@@ -22496,8 +22478,8 @@
       <c r="E496" t="s">
         <v>577</v>
       </c>
-      <c r="J496" t="s">
-        <v>2776</v>
+      <c r="J496" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K496">
         <v>2</v>
@@ -22522,8 +22504,8 @@
       <c r="E497" t="s">
         <v>577</v>
       </c>
-      <c r="J497" t="s">
-        <v>2776</v>
+      <c r="J497" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K497">
         <v>2</v>
@@ -22600,8 +22582,8 @@
       <c r="E500" t="s">
         <v>566</v>
       </c>
-      <c r="J500" t="s">
-        <v>2776</v>
+      <c r="J500" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K500">
         <v>2</v>
@@ -22632,8 +22614,8 @@
       <c r="G501" t="s">
         <v>1155</v>
       </c>
-      <c r="J501" t="s">
-        <v>2776</v>
+      <c r="J501" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K501">
         <v>2</v>
@@ -22658,8 +22640,8 @@
       <c r="E502" t="s">
         <v>566</v>
       </c>
-      <c r="J502" t="s">
-        <v>2776</v>
+      <c r="J502" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K502">
         <v>2</v>
@@ -22788,8 +22770,8 @@
       <c r="E507" t="s">
         <v>568</v>
       </c>
-      <c r="J507" t="s">
-        <v>2776</v>
+      <c r="J507" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K507">
         <v>2</v>
@@ -22814,8 +22796,8 @@
       <c r="E508" t="s">
         <v>577</v>
       </c>
-      <c r="J508" t="s">
-        <v>2776</v>
+      <c r="J508" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K508">
         <v>2</v>
@@ -22840,8 +22822,8 @@
       <c r="E509" t="s">
         <v>577</v>
       </c>
-      <c r="J509" t="s">
-        <v>2776</v>
+      <c r="J509" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K509">
         <v>2</v>
@@ -22866,8 +22848,8 @@
       <c r="E510" t="s">
         <v>577</v>
       </c>
-      <c r="J510" t="s">
-        <v>2776</v>
+      <c r="J510" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K510">
         <v>2</v>
@@ -23100,8 +23082,8 @@
       <c r="E519" t="s">
         <v>2394</v>
       </c>
-      <c r="J519" t="s">
-        <v>2776</v>
+      <c r="J519" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K519">
         <v>3</v>
@@ -23126,8 +23108,8 @@
       <c r="E520" t="s">
         <v>2394</v>
       </c>
-      <c r="J520" t="s">
-        <v>2776</v>
+      <c r="J520" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K520">
         <v>3</v>
@@ -23152,8 +23134,8 @@
       <c r="E521" t="s">
         <v>2394</v>
       </c>
-      <c r="J521" t="s">
-        <v>2776</v>
+      <c r="J521" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K521">
         <v>3</v>
@@ -23178,8 +23160,8 @@
       <c r="E522" t="s">
         <v>2413</v>
       </c>
-      <c r="J522" t="s">
-        <v>2776</v>
+      <c r="J522" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K522">
         <v>3</v>
@@ -23204,8 +23186,8 @@
       <c r="E523" t="s">
         <v>2413</v>
       </c>
-      <c r="J523" t="s">
-        <v>2776</v>
+      <c r="J523" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K523">
         <v>3</v>
@@ -24573,8 +24555,8 @@
       <c r="E575" t="s">
         <v>587</v>
       </c>
-      <c r="J575" t="s">
-        <v>2776</v>
+      <c r="J575" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K575">
         <v>3</v>
@@ -24599,8 +24581,8 @@
       <c r="E576" t="s">
         <v>587</v>
       </c>
-      <c r="J576" t="s">
-        <v>2776</v>
+      <c r="J576" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K576">
         <v>3</v>
@@ -24625,8 +24607,8 @@
       <c r="E577" t="s">
         <v>566</v>
       </c>
-      <c r="J577" t="s">
-        <v>2776</v>
+      <c r="J577" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K577">
         <v>3</v>
@@ -24651,8 +24633,8 @@
       <c r="E578" t="s">
         <v>566</v>
       </c>
-      <c r="J578" t="s">
-        <v>2776</v>
+      <c r="J578" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K578">
         <v>3</v>
@@ -24677,8 +24659,8 @@
       <c r="E579" t="s">
         <v>587</v>
       </c>
-      <c r="J579" t="s">
-        <v>2776</v>
+      <c r="J579" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K579">
         <v>3</v>
@@ -24703,8 +24685,8 @@
       <c r="E580" t="s">
         <v>566</v>
       </c>
-      <c r="J580" t="s">
-        <v>2776</v>
+      <c r="J580" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K580">
         <v>3</v>
@@ -24729,8 +24711,8 @@
       <c r="E581" t="s">
         <v>871</v>
       </c>
-      <c r="J581" t="s">
-        <v>2776</v>
+      <c r="J581" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K581">
         <v>3</v>
@@ -24755,8 +24737,8 @@
       <c r="E582" t="s">
         <v>566</v>
       </c>
-      <c r="J582" t="s">
-        <v>2776</v>
+      <c r="J582" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K582">
         <v>3</v>
@@ -25460,8 +25442,8 @@
       <c r="E609" t="s">
         <v>2576</v>
       </c>
-      <c r="J609" t="s">
-        <v>2776</v>
+      <c r="J609" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K609">
         <v>3</v>
@@ -25486,8 +25468,8 @@
       <c r="E610" t="s">
         <v>2576</v>
       </c>
-      <c r="J610" t="s">
-        <v>2776</v>
+      <c r="J610" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K610">
         <v>3</v>
@@ -25512,8 +25494,8 @@
       <c r="E611" t="s">
         <v>566</v>
       </c>
-      <c r="J611" t="s">
-        <v>2776</v>
+      <c r="J611" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K611">
         <v>3</v>
@@ -25538,8 +25520,8 @@
       <c r="E612" t="s">
         <v>2576</v>
       </c>
-      <c r="J612" t="s">
-        <v>2776</v>
+      <c r="J612" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K612">
         <v>3</v>
@@ -25564,8 +25546,8 @@
       <c r="E613" t="s">
         <v>2576</v>
       </c>
-      <c r="J613" t="s">
-        <v>2776</v>
+      <c r="J613" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K613">
         <v>3</v>
@@ -25590,8 +25572,8 @@
       <c r="E614" t="s">
         <v>2576</v>
       </c>
-      <c r="J614" t="s">
-        <v>2776</v>
+      <c r="J614" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K614">
         <v>3</v>
@@ -25616,8 +25598,8 @@
       <c r="E615" t="s">
         <v>566</v>
       </c>
-      <c r="J615" t="s">
-        <v>2776</v>
+      <c r="J615" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K615">
         <v>3</v>
@@ -25642,8 +25624,8 @@
       <c r="E616" t="s">
         <v>2576</v>
       </c>
-      <c r="J616" t="s">
-        <v>2776</v>
+      <c r="J616" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K616">
         <v>3</v>
@@ -25746,8 +25728,8 @@
       <c r="E620" t="s">
         <v>566</v>
       </c>
-      <c r="J620" t="s">
-        <v>2776</v>
+      <c r="J620" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K620">
         <v>3</v>
@@ -25772,8 +25754,8 @@
       <c r="E621" t="s">
         <v>566</v>
       </c>
-      <c r="J621" t="s">
-        <v>2776</v>
+      <c r="J621" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K621">
         <v>3</v>
@@ -25798,8 +25780,8 @@
       <c r="E622" t="s">
         <v>566</v>
       </c>
-      <c r="J622" t="s">
-        <v>2776</v>
+      <c r="J622" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K622">
         <v>3</v>
@@ -25824,8 +25806,8 @@
       <c r="E623" t="s">
         <v>566</v>
       </c>
-      <c r="J623" t="s">
-        <v>2776</v>
+      <c r="J623" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K623">
         <v>3</v>
@@ -25850,8 +25832,8 @@
       <c r="E624" t="s">
         <v>566</v>
       </c>
-      <c r="J624" t="s">
-        <v>2776</v>
+      <c r="J624" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K624">
         <v>3</v>
@@ -25876,8 +25858,8 @@
       <c r="E625" t="s">
         <v>566</v>
       </c>
-      <c r="J625" t="s">
-        <v>2776</v>
+      <c r="J625" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K625">
         <v>3</v>
@@ -25902,8 +25884,8 @@
       <c r="E626" t="s">
         <v>569</v>
       </c>
-      <c r="J626" t="s">
-        <v>2776</v>
+      <c r="J626" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K626">
         <v>3</v>
@@ -25928,8 +25910,8 @@
       <c r="E627" t="s">
         <v>569</v>
       </c>
-      <c r="J627" t="s">
-        <v>2776</v>
+      <c r="J627" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K627">
         <v>3</v>
@@ -25954,8 +25936,8 @@
       <c r="E628" t="s">
         <v>566</v>
       </c>
-      <c r="J628" t="s">
-        <v>2776</v>
+      <c r="J628" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K628">
         <v>3</v>
@@ -25980,8 +25962,8 @@
       <c r="E629" t="s">
         <v>566</v>
       </c>
-      <c r="J629" t="s">
-        <v>2776</v>
+      <c r="J629" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K629">
         <v>3</v>
@@ -26006,8 +25988,8 @@
       <c r="E630" t="s">
         <v>566</v>
       </c>
-      <c r="J630" t="s">
-        <v>2776</v>
+      <c r="J630" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K630">
         <v>3</v>
@@ -26032,8 +26014,8 @@
       <c r="E631" t="s">
         <v>566</v>
       </c>
-      <c r="J631" t="s">
-        <v>2776</v>
+      <c r="J631" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K631">
         <v>3</v>
@@ -26110,8 +26092,8 @@
       <c r="E634" t="s">
         <v>569</v>
       </c>
-      <c r="J634" t="s">
-        <v>2776</v>
+      <c r="J634" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K634">
         <v>3</v>
@@ -26136,8 +26118,8 @@
       <c r="E635" t="s">
         <v>570</v>
       </c>
-      <c r="J635" t="s">
-        <v>2776</v>
+      <c r="J635" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K635">
         <v>3</v>
@@ -26214,8 +26196,8 @@
       <c r="E638" s="8" t="s">
         <v>2695</v>
       </c>
-      <c r="J638" t="s">
-        <v>2776</v>
+      <c r="J638" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K638">
         <v>3</v>
@@ -26240,8 +26222,8 @@
       <c r="E639" t="s">
         <v>2394</v>
       </c>
-      <c r="J639" t="s">
-        <v>2776</v>
+      <c r="J639" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K639">
         <v>3</v>
@@ -26255,7 +26237,7 @@
     </row>
     <row r="640" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A640" s="2" t="s">
-        <v>2635</v>
+        <v>2778</v>
       </c>
       <c r="B640" s="2" t="s">
         <v>2636</v>
@@ -26266,8 +26248,8 @@
       <c r="E640" t="s">
         <v>2394</v>
       </c>
-      <c r="J640" t="s">
-        <v>2776</v>
+      <c r="J640" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K640">
         <v>3</v>
@@ -26292,8 +26274,8 @@
       <c r="E641" s="8" t="s">
         <v>2695</v>
       </c>
-      <c r="J641" t="s">
-        <v>2776</v>
+      <c r="J641" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K641">
         <v>3</v>
@@ -26318,8 +26300,8 @@
       <c r="E642" t="s">
         <v>2394</v>
       </c>
-      <c r="J642" t="s">
-        <v>2776</v>
+      <c r="J642" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K642">
         <v>3</v>
@@ -26333,7 +26315,7 @@
     </row>
     <row r="643" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A643" s="2" t="s">
-        <v>2639</v>
+        <v>2779</v>
       </c>
       <c r="B643" s="2" t="s">
         <v>2640</v>
@@ -26344,8 +26326,8 @@
       <c r="E643" t="s">
         <v>2695</v>
       </c>
-      <c r="J643" t="s">
-        <v>2776</v>
+      <c r="J643" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K643">
         <v>3</v>
@@ -26942,8 +26924,8 @@
       <c r="E666" t="s">
         <v>590</v>
       </c>
-      <c r="J666" t="s">
-        <v>2776</v>
+      <c r="J666" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K666">
         <v>3</v>
@@ -26994,8 +26976,8 @@
       <c r="E668" t="s">
         <v>2739</v>
       </c>
-      <c r="J668" t="s">
-        <v>2776</v>
+      <c r="J668" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K668">
         <v>3</v>
@@ -27020,8 +27002,8 @@
       <c r="E669" t="s">
         <v>2739</v>
       </c>
-      <c r="J669" t="s">
-        <v>2776</v>
+      <c r="J669" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K669">
         <v>3</v>
@@ -27124,8 +27106,8 @@
       <c r="E673" t="s">
         <v>577</v>
       </c>
-      <c r="J673" t="s">
-        <v>2776</v>
+      <c r="J673" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K673">
         <v>3</v>
@@ -27150,8 +27132,8 @@
       <c r="E674" t="s">
         <v>2739</v>
       </c>
-      <c r="J674" t="s">
-        <v>2776</v>
+      <c r="J674" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K674">
         <v>3</v>
@@ -27228,8 +27210,8 @@
       <c r="E677" t="s">
         <v>2394</v>
       </c>
-      <c r="J677" t="s">
-        <v>2776</v>
+      <c r="J677" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K677">
         <v>3</v>
@@ -27254,8 +27236,8 @@
       <c r="E678" t="s">
         <v>590</v>
       </c>
-      <c r="J678" t="s">
-        <v>2776</v>
+      <c r="J678" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K678">
         <v>3</v>
@@ -27306,8 +27288,8 @@
       <c r="E680" t="s">
         <v>2740</v>
       </c>
-      <c r="J680" t="s">
-        <v>2776</v>
+      <c r="J680" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K680">
         <v>3</v>
@@ -27332,8 +27314,8 @@
       <c r="E681" t="s">
         <v>2740</v>
       </c>
-      <c r="J681" t="s">
-        <v>2776</v>
+      <c r="J681" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K681">
         <v>3</v>
@@ -27384,8 +27366,8 @@
       <c r="E683" t="s">
         <v>590</v>
       </c>
-      <c r="J683" t="s">
-        <v>2776</v>
+      <c r="J683" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K683">
         <v>3</v>
@@ -27410,8 +27392,8 @@
       <c r="E684" t="s">
         <v>2740</v>
       </c>
-      <c r="J684" t="s">
-        <v>2776</v>
+      <c r="J684" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K684">
         <v>3</v>
@@ -27462,8 +27444,8 @@
       <c r="E686" t="s">
         <v>2739</v>
       </c>
-      <c r="J686" t="s">
-        <v>2776</v>
+      <c r="J686" s="3" t="s">
+        <v>2780</v>
       </c>
       <c r="K686">
         <v>3</v>
@@ -27472,13 +27454,39 @@
         <v>5</v>
       </c>
       <c r="M686" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="687" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A687" t="s">
+        <v>2776</v>
+      </c>
+      <c r="B687" t="s">
+        <v>2777</v>
+      </c>
+      <c r="D687" t="s">
+        <v>589</v>
+      </c>
+      <c r="E687" t="s">
+        <v>590</v>
+      </c>
+      <c r="J687" t="s">
+        <v>64</v>
+      </c>
+      <c r="K687">
+        <v>3</v>
+      </c>
+      <c r="L687">
+        <v>5</v>
+      </c>
+      <c r="M687" t="s">
         <v>838</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M686" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}"/>
   <conditionalFormatting sqref="A620:A1048576 A1:A538 A540:A616">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -28873,7 +28881,7 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A67">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44744,7 +44752,7 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A614">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47847,11 +47855,11 @@
   </sheetData>
   <autoFilter ref="A1:A616" xr:uid="{CA85B85C-B632-4DE2-B59B-FD77C3B41E34}">
     <filterColumn colId="0">
-      <colorFilter dxfId="9"/>
+      <colorFilter dxfId="3"/>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -62014,7 +62022,7 @@
         <v>568</v>
       </c>
       <c r="E1" s="6" t="str">
-        <f>"[['"&amp;A1&amp;"'], ['"&amp;B1&amp;"'], '"&amp;D1&amp;"', '3']"</f>
+        <f t="shared" ref="E1:E32" si="0">"[['"&amp;A1&amp;"'], ['"&amp;B1&amp;"'], '"&amp;D1&amp;"', '3']"</f>
         <v>[['세탁소'], ['прачечная / химчистка'], 'место', '3']</v>
       </c>
       <c r="O1" t="s">
@@ -62041,7 +62049,7 @@
         <v>2394</v>
       </c>
       <c r="E2" s="6" t="str">
-        <f>"[['"&amp;A2&amp;"'], ['"&amp;B2&amp;"'], '"&amp;D2&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['발표'], ['презентация / доклад'], 'профессия', '3']</v>
       </c>
       <c r="O2" t="s">
@@ -62068,7 +62076,7 @@
         <v>871</v>
       </c>
       <c r="E3" s="6" t="str">
-        <f>"[['"&amp;A3&amp;"'], ['"&amp;B3&amp;"'], '"&amp;D3&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['걱정이다'], ['беспокоиться / беспокоиться о чем-то'], 'состояние', '3']</v>
       </c>
       <c r="O3" t="s">
@@ -62095,7 +62103,7 @@
         <v>871</v>
       </c>
       <c r="E4" s="6" t="str">
-        <f>"[['"&amp;A4&amp;"'], ['"&amp;B4&amp;"'], '"&amp;D4&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['걱정되다'], ['беспокоиться / волноваться'], 'состояние', '3']</v>
       </c>
       <c r="O4" t="s">
@@ -62122,7 +62130,7 @@
         <v>587</v>
       </c>
       <c r="E5" s="6" t="str">
-        <f>"[['"&amp;A5&amp;"'], ['"&amp;B5&amp;"'], '"&amp;D5&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['지저분하다'], ['грязный / неряшливый'], 'люди', '3']</v>
       </c>
       <c r="O5" t="s">
@@ -62149,7 +62157,7 @@
         <v>566</v>
       </c>
       <c r="E6" s="6" t="str">
-        <f>"[['"&amp;A6&amp;"'], ['"&amp;B6&amp;"'], '"&amp;D6&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['끝내다'], ['заканчивать / завершать'], 'действие', '3']</v>
       </c>
       <c r="O6" t="s">
@@ -62176,7 +62184,7 @@
         <v>577</v>
       </c>
       <c r="E7" s="6" t="str">
-        <f>"[['"&amp;A7&amp;"'], ['"&amp;B7&amp;"'], '"&amp;D7&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['여러 가지'], ['различный / разнообразный'], 'другое', '3']</v>
       </c>
       <c r="O7" t="s">
@@ -62203,7 +62211,7 @@
         <v>574</v>
       </c>
       <c r="E8" s="6" t="str">
-        <f>"[['"&amp;A8&amp;"'], ['"&amp;B8&amp;"'], '"&amp;D8&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['걸리다'], ['длиться (о времени) / занимать времени'], 'время', '3']</v>
       </c>
       <c r="J8" t="s">
@@ -62239,7 +62247,7 @@
         <v>568</v>
       </c>
       <c r="E9" s="6" t="str">
-        <f>"[['"&amp;A9&amp;"'], ['"&amp;B9&amp;"'], '"&amp;D9&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['부엌'], ['кухня (помещение)'], 'место', '3']</v>
       </c>
       <c r="J9" t="s">
@@ -62275,7 +62283,7 @@
         <v>574</v>
       </c>
       <c r="E10" s="6" t="str">
-        <f>"[['"&amp;A10&amp;"'], ['"&amp;B10&amp;"'], '"&amp;D10&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['아까'], ['ранее / недавно / только что'], 'время', '3']</v>
       </c>
       <c r="J10" t="s">
@@ -62311,7 +62319,7 @@
         <v>569</v>
       </c>
       <c r="E11" s="6" t="str">
-        <f>"[['"&amp;A11&amp;"'], ['"&amp;B11&amp;"'], '"&amp;D11&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['갈아입다'], ['переодеваться'], 'одежда', '3']</v>
       </c>
       <c r="J11" t="s">
@@ -62347,7 +62355,7 @@
         <v>566</v>
       </c>
       <c r="E12" s="6" t="str">
-        <f>"[['"&amp;A12&amp;"'], ['"&amp;B12&amp;"'], '"&amp;D12&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['무리'], ['сложно что-то сделать'], 'действие', '3']</v>
       </c>
       <c r="J12" t="s">
@@ -62383,7 +62391,7 @@
         <v>577</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f>"[['"&amp;A13&amp;"'], ['"&amp;B13&amp;"'], '"&amp;D13&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['싫다'], ['не хотеть / не нравиться'], 'другое', '3']</v>
       </c>
       <c r="J13" t="s">
@@ -62419,7 +62427,7 @@
         <v>574</v>
       </c>
       <c r="E14" s="6" t="str">
-        <f>"[['"&amp;A14&amp;"'], ['"&amp;B14&amp;"'], '"&amp;D14&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['일단'], ['сначала / сперва / в первую очередь'], 'время', '3']</v>
       </c>
       <c r="J14" t="s">
@@ -62455,7 +62463,7 @@
         <v>577</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f>"[['"&amp;A15&amp;"'], ['"&amp;B15&amp;"'], '"&amp;D15&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['또'], ['снова / опять / еще раз'], 'другое', '3']</v>
       </c>
       <c r="J15" t="s">
@@ -62491,7 +62499,7 @@
         <v>574</v>
       </c>
       <c r="E16" s="6" t="str">
-        <f>"[['"&amp;A16&amp;"'], ['"&amp;B16&amp;"'], '"&amp;D16&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['천천히'], ['медленно / неторопливо / потихоньку'], 'время', '3']</v>
       </c>
       <c r="J16" t="s">
@@ -62527,7 +62535,7 @@
         <v>574</v>
       </c>
       <c r="E17" s="6" t="str">
-        <f>"[['"&amp;A17&amp;"'], ['"&amp;B17&amp;"'], '"&amp;D17&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['새로'], ['вновь / заново'], 'время', '3']</v>
       </c>
       <c r="J17" t="s">
@@ -62563,7 +62571,7 @@
         <v>574</v>
       </c>
       <c r="E18" s="6" t="str">
-        <f>"[['"&amp;A18&amp;"'], ['"&amp;B18&amp;"'], '"&amp;D18&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['오래'], ['долго / давно'], 'время', '3']</v>
       </c>
       <c r="J18" t="s">
@@ -62599,7 +62607,7 @@
         <v>571</v>
       </c>
       <c r="E19" s="6" t="str">
-        <f>"[['"&amp;A19&amp;"'], ['"&amp;B19&amp;"'], '"&amp;D19&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['냄새'], ['запах / аромат / вонь'], 'продукты', '3']</v>
       </c>
       <c r="J19" t="s">
@@ -62635,7 +62643,7 @@
         <v>577</v>
       </c>
       <c r="E20" s="6" t="str">
-        <f>"[['"&amp;A20&amp;"'], ['"&amp;B20&amp;"'], '"&amp;D20&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['서류'], ['документ'], 'другое', '3']</v>
       </c>
       <c r="J20" t="s">
@@ -62671,7 +62679,7 @@
         <v>2695</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f>"[['"&amp;A21&amp;"'], ['"&amp;B21&amp;"'], '"&amp;D21&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['외국어'], ['иностранный язык'], 'образование', '3']</v>
       </c>
       <c r="J21" t="s">
@@ -62707,7 +62715,7 @@
         <v>2695</v>
       </c>
       <c r="E22" s="6" t="str">
-        <f>"[['"&amp;A22&amp;"'], ['"&amp;B22&amp;"'], '"&amp;D22&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['한국어능력시험'], ['экзамен ТОПИК'], 'образование', '3']</v>
       </c>
       <c r="J22" t="s">
@@ -62743,7 +62751,7 @@
         <v>2695</v>
       </c>
       <c r="E23" s="6" t="str">
-        <f>"[['"&amp;A23&amp;"'], ['"&amp;B23&amp;"'], '"&amp;D23&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['자격증'], ['диплом / сертификат / лицензия'], 'образование', '3']</v>
       </c>
       <c r="O23" t="s">
@@ -62770,7 +62778,7 @@
         <v>577</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f>"[['"&amp;A24&amp;"'], ['"&amp;B24&amp;"'], '"&amp;D24&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['계획'], ['планы / дела / проект'], 'другое', '3']</v>
       </c>
     </row>
@@ -62785,7 +62793,7 @@
         <v>577</v>
       </c>
       <c r="E25" s="6" t="str">
-        <f>"[['"&amp;A25&amp;"'], ['"&amp;B25&amp;"'], '"&amp;D25&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['내려가다'], ['спускаться'], 'другое', '3']</v>
       </c>
     </row>
@@ -62800,7 +62808,7 @@
         <v>566</v>
       </c>
       <c r="E26" s="6" t="str">
-        <f>"[['"&amp;A26&amp;"'], ['"&amp;B26&amp;"'], '"&amp;D26&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['돕다'], ['помогать / оказывать помощь'], 'действие', '3']</v>
       </c>
     </row>
@@ -62815,7 +62823,7 @@
         <v>577</v>
       </c>
       <c r="E27" s="6" t="str">
-        <f>"[['"&amp;A27&amp;"'], ['"&amp;B27&amp;"'], '"&amp;D27&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['밀리다'], ['скапливаться / накапливаться'], 'другое', '3']</v>
       </c>
     </row>
@@ -62830,7 +62838,7 @@
         <v>577</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f>"[['"&amp;A28&amp;"'], ['"&amp;B28&amp;"'], '"&amp;D28&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['방문하다'], ['посетить / прибыть с визитом / навещать'], 'другое', '3']</v>
       </c>
     </row>
@@ -62845,7 +62853,7 @@
         <v>2394</v>
       </c>
       <c r="E29" s="6" t="str">
-        <f>"[['"&amp;A29&amp;"'], ['"&amp;B29&amp;"'], '"&amp;D29&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['봉사'], ['волонтерство / обслуживание'], 'профессия', '3']</v>
       </c>
     </row>
@@ -62860,7 +62868,7 @@
         <v>577</v>
       </c>
       <c r="E30" s="6" t="str">
-        <f>"[['"&amp;A30&amp;"'], ['"&amp;B30&amp;"'], '"&amp;D30&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['실컷'], ['вдоволь / сколько угодно'], 'другое', '3']</v>
       </c>
     </row>
@@ -62875,7 +62883,7 @@
         <v>590</v>
       </c>
       <c r="E31" s="6" t="str">
-        <f>"[['"&amp;A31&amp;"'], ['"&amp;B31&amp;"'], '"&amp;D31&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['친척'], ['родственник / близкий родственник'], 'семья', '3']</v>
       </c>
     </row>
@@ -62890,217 +62898,217 @@
         <v>2740</v>
       </c>
       <c r="E32" s="6" t="str">
-        <f>"[['"&amp;A32&amp;"'], ['"&amp;B32&amp;"'], '"&amp;D32&amp;"', '3']"</f>
+        <f t="shared" si="0"/>
         <v>[['활동'], ['деятельность / активность / занятие'], 'досуг', '3']</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" s="6" t="str">
-        <f>"[['"&amp;A33&amp;"'], ['"&amp;B33&amp;"'], '"&amp;D33&amp;"', '3']"</f>
+        <f t="shared" ref="E33:E64" si="1">"[['"&amp;A33&amp;"'], ['"&amp;B33&amp;"'], '"&amp;D33&amp;"', '3']"</f>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E34" s="6" t="str">
-        <f>"[['"&amp;A34&amp;"'], ['"&amp;B34&amp;"'], '"&amp;D34&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="35" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E35" s="6" t="str">
-        <f>"[['"&amp;A35&amp;"'], ['"&amp;B35&amp;"'], '"&amp;D35&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="36" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E36" s="6" t="str">
-        <f>"[['"&amp;A36&amp;"'], ['"&amp;B36&amp;"'], '"&amp;D36&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E37" s="6" t="str">
-        <f>"[['"&amp;A37&amp;"'], ['"&amp;B37&amp;"'], '"&amp;D37&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E38" s="6" t="str">
-        <f>"[['"&amp;A38&amp;"'], ['"&amp;B38&amp;"'], '"&amp;D38&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="39" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E39" s="6" t="str">
-        <f>"[['"&amp;A39&amp;"'], ['"&amp;B39&amp;"'], '"&amp;D39&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="40" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E40" s="6" t="str">
-        <f>"[['"&amp;A40&amp;"'], ['"&amp;B40&amp;"'], '"&amp;D40&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="41" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E41" s="6" t="str">
-        <f>"[['"&amp;A41&amp;"'], ['"&amp;B41&amp;"'], '"&amp;D41&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="42" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E42" s="6" t="str">
-        <f>"[['"&amp;A42&amp;"'], ['"&amp;B42&amp;"'], '"&amp;D42&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="43" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E43" s="6" t="str">
-        <f>"[['"&amp;A43&amp;"'], ['"&amp;B43&amp;"'], '"&amp;D43&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="44" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E44" s="6" t="str">
-        <f>"[['"&amp;A44&amp;"'], ['"&amp;B44&amp;"'], '"&amp;D44&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="45" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E45" s="6" t="str">
-        <f>"[['"&amp;A45&amp;"'], ['"&amp;B45&amp;"'], '"&amp;D45&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="46" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E46" s="6" t="str">
-        <f>"[['"&amp;A46&amp;"'], ['"&amp;B46&amp;"'], '"&amp;D46&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="47" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E47" s="6" t="str">
-        <f>"[['"&amp;A47&amp;"'], ['"&amp;B47&amp;"'], '"&amp;D47&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="48" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E48" s="6" t="str">
-        <f>"[['"&amp;A48&amp;"'], ['"&amp;B48&amp;"'], '"&amp;D48&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="6" t="str">
-        <f>"[['"&amp;A49&amp;"'], ['"&amp;B49&amp;"'], '"&amp;D49&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="6" t="str">
-        <f>"[['"&amp;A50&amp;"'], ['"&amp;B50&amp;"'], '"&amp;D50&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="6" t="str">
-        <f>"[['"&amp;A51&amp;"'], ['"&amp;B51&amp;"'], '"&amp;D51&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="6" t="str">
-        <f>"[['"&amp;A52&amp;"'], ['"&amp;B52&amp;"'], '"&amp;D52&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="6" t="str">
-        <f>"[['"&amp;A53&amp;"'], ['"&amp;B53&amp;"'], '"&amp;D53&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="6" t="str">
-        <f>"[['"&amp;A54&amp;"'], ['"&amp;B54&amp;"'], '"&amp;D54&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="6" t="str">
-        <f>"[['"&amp;A55&amp;"'], ['"&amp;B55&amp;"'], '"&amp;D55&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="6" t="str">
-        <f>"[['"&amp;A56&amp;"'], ['"&amp;B56&amp;"'], '"&amp;D56&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="6" t="str">
-        <f>"[['"&amp;A57&amp;"'], ['"&amp;B57&amp;"'], '"&amp;D57&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="6" t="str">
-        <f>"[['"&amp;A58&amp;"'], ['"&amp;B58&amp;"'], '"&amp;D58&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="6" t="str">
-        <f>"[['"&amp;A59&amp;"'], ['"&amp;B59&amp;"'], '"&amp;D59&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="6" t="str">
-        <f>"[['"&amp;A60&amp;"'], ['"&amp;B60&amp;"'], '"&amp;D60&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="6" t="str">
-        <f>"[['"&amp;A61&amp;"'], ['"&amp;B61&amp;"'], '"&amp;D61&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="6" t="str">
-        <f>"[['"&amp;A62&amp;"'], ['"&amp;B62&amp;"'], '"&amp;D62&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="6" t="str">
-        <f>"[['"&amp;A63&amp;"'], ['"&amp;B63&amp;"'], '"&amp;D63&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="6" t="str">
-        <f>"[['"&amp;A64&amp;"'], ['"&amp;B64&amp;"'], '"&amp;D64&amp;"', '3']"</f>
+        <f t="shared" si="1"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E65" s="6" t="str">
-        <f>"[['"&amp;A65&amp;"'], ['"&amp;B65&amp;"'], '"&amp;D65&amp;"', '3']"</f>
+        <f t="shared" ref="E65:E67" si="2">"[['"&amp;A65&amp;"'], ['"&amp;B65&amp;"'], '"&amp;D65&amp;"', '3']"</f>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E66" s="6" t="str">
-        <f>"[['"&amp;A66&amp;"'], ['"&amp;B66&amp;"'], '"&amp;D66&amp;"', '3']"</f>
+        <f t="shared" si="2"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E67" s="6" t="str">
-        <f>"[['"&amp;A67&amp;"'], ['"&amp;B67&amp;"'], '"&amp;D67&amp;"', '3']"</f>
+        <f t="shared" si="2"/>
         <v>[[''], [''], '', '3']</v>
       </c>
     </row>
@@ -63266,7 +63274,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O1:O23">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A32">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
new words and rules 3-6
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F1E469-5EDC-475B-A365-4A28DEF4D90D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0F3329-1B20-4ECF-94F8-139153F35FDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16629" uniqueCount="2857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16835" uniqueCount="2915">
   <si>
     <t>stage</t>
   </si>
@@ -8612,6 +8612,180 @@
   </si>
   <si>
     <t>передвижение</t>
+  </si>
+  <si>
+    <t>어서 오세요</t>
+  </si>
+  <si>
+    <t>티셔츠</t>
+  </si>
+  <si>
+    <t>색깔</t>
+  </si>
+  <si>
+    <t>원피스</t>
+  </si>
+  <si>
+    <t>블라우스</t>
+  </si>
+  <si>
+    <t>노트북</t>
+  </si>
+  <si>
+    <t>디자인</t>
+  </si>
+  <si>
+    <t>수선하다</t>
+  </si>
+  <si>
+    <t>그만</t>
+  </si>
+  <si>
+    <t>문제</t>
+  </si>
+  <si>
+    <t>간단하다</t>
+  </si>
+  <si>
+    <t>치수</t>
+  </si>
+  <si>
+    <t>무늬</t>
+  </si>
+  <si>
+    <t>빗소리</t>
+  </si>
+  <si>
+    <t>큼일 나다</t>
+  </si>
+  <si>
+    <t>고르다</t>
+  </si>
+  <si>
+    <t>움직이다</t>
+  </si>
+  <si>
+    <t>소개팅</t>
+  </si>
+  <si>
+    <t>면접시험</t>
+  </si>
+  <si>
+    <t>자르다</t>
+  </si>
+  <si>
+    <t>느낌</t>
+  </si>
+  <si>
+    <t>회원</t>
+  </si>
+  <si>
+    <t>할인</t>
+  </si>
+  <si>
+    <t>부</t>
+  </si>
+  <si>
+    <t>단체</t>
+  </si>
+  <si>
+    <t>모든</t>
+  </si>
+  <si>
+    <t>평소</t>
+  </si>
+  <si>
+    <t>футболка</t>
+  </si>
+  <si>
+    <t>блузка</t>
+  </si>
+  <si>
+    <t>ноутбук</t>
+  </si>
+  <si>
+    <t>дизайн</t>
+  </si>
+  <si>
+    <t>размер</t>
+  </si>
+  <si>
+    <t>чувство</t>
+  </si>
+  <si>
+    <t>группа</t>
+  </si>
+  <si>
+    <t>добро пожаловать</t>
+  </si>
+  <si>
+    <t>платье</t>
+  </si>
+  <si>
+    <t>저</t>
+  </si>
+  <si>
+    <t>길이</t>
+  </si>
+  <si>
+    <t>длина</t>
+  </si>
+  <si>
+    <t>ремонтировать одежду</t>
+  </si>
+  <si>
+    <t>остановиться / прекратить</t>
+  </si>
+  <si>
+    <t>проблема / задача</t>
+  </si>
+  <si>
+    <t>легкий / не сложный</t>
+  </si>
+  <si>
+    <t>шаблон / узоры</t>
+  </si>
+  <si>
+    <t>звук дождя</t>
+  </si>
+  <si>
+    <t>что-то плохое случилось</t>
+  </si>
+  <si>
+    <t>выбирать из множества</t>
+  </si>
+  <si>
+    <t>шаг / двигаться</t>
+  </si>
+  <si>
+    <t>свидание в слепую</t>
+  </si>
+  <si>
+    <t>интервью / экзамен / собеседование</t>
+  </si>
+  <si>
+    <t>резать / отрезать</t>
+  </si>
+  <si>
+    <t>член / челн клуба / член организации</t>
+  </si>
+  <si>
+    <t>распродажа / скидки</t>
+  </si>
+  <si>
+    <t>богатство / отдел</t>
+  </si>
+  <si>
+    <t>каждый / все</t>
+  </si>
+  <si>
+    <t>обычно / как все</t>
+  </si>
+  <si>
+    <t>обращение перед диалогом</t>
+  </si>
+  <si>
+    <t>общение</t>
   </si>
 </sst>
 </file>
@@ -8694,7 +8868,17 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -9073,11 +9257,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:M739"/>
+  <dimension ref="A1:M768"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A746" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J769" sqref="J769"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27719,9 +27903,15 @@
         <v>1</v>
       </c>
       <c r="D688" t="s">
+        <v>332</v>
+      </c>
+      <c r="E688" t="s">
+        <v>574</v>
+      </c>
+      <c r="F688" t="s">
         <v>2812</v>
       </c>
-      <c r="E688" t="s">
+      <c r="G688" t="s">
         <v>2813</v>
       </c>
       <c r="J688" s="3" t="s">
@@ -27745,9 +27935,15 @@
         <v>2</v>
       </c>
       <c r="D689" t="s">
+        <v>332</v>
+      </c>
+      <c r="E689" t="s">
+        <v>574</v>
+      </c>
+      <c r="F689" t="s">
         <v>2812</v>
       </c>
-      <c r="E689" t="s">
+      <c r="G689" t="s">
         <v>2813</v>
       </c>
       <c r="J689" s="3" t="s">
@@ -27771,9 +27967,15 @@
         <v>3</v>
       </c>
       <c r="D690" t="s">
+        <v>332</v>
+      </c>
+      <c r="E690" t="s">
+        <v>574</v>
+      </c>
+      <c r="F690" t="s">
         <v>2812</v>
       </c>
-      <c r="E690" t="s">
+      <c r="G690" t="s">
         <v>2813</v>
       </c>
       <c r="J690" s="3" t="s">
@@ -27797,9 +27999,15 @@
         <v>4</v>
       </c>
       <c r="D691" t="s">
+        <v>332</v>
+      </c>
+      <c r="E691" t="s">
+        <v>574</v>
+      </c>
+      <c r="F691" t="s">
         <v>2812</v>
       </c>
-      <c r="E691" t="s">
+      <c r="G691" t="s">
         <v>2813</v>
       </c>
       <c r="J691" s="3" t="s">
@@ -27823,9 +28031,15 @@
         <v>5</v>
       </c>
       <c r="D692" t="s">
+        <v>332</v>
+      </c>
+      <c r="E692" t="s">
+        <v>574</v>
+      </c>
+      <c r="F692" t="s">
         <v>2812</v>
       </c>
-      <c r="E692" t="s">
+      <c r="G692" t="s">
         <v>2813</v>
       </c>
       <c r="J692" s="3" t="s">
@@ -27849,9 +28063,15 @@
         <v>6</v>
       </c>
       <c r="D693" t="s">
+        <v>332</v>
+      </c>
+      <c r="E693" t="s">
+        <v>574</v>
+      </c>
+      <c r="F693" t="s">
         <v>2812</v>
       </c>
-      <c r="E693" t="s">
+      <c r="G693" t="s">
         <v>2813</v>
       </c>
       <c r="J693" s="3" t="s">
@@ -27875,9 +28095,15 @@
         <v>7</v>
       </c>
       <c r="D694" t="s">
+        <v>332</v>
+      </c>
+      <c r="E694" t="s">
+        <v>574</v>
+      </c>
+      <c r="F694" t="s">
         <v>2812</v>
       </c>
-      <c r="E694" t="s">
+      <c r="G694" t="s">
         <v>2813</v>
       </c>
       <c r="J694" s="3" t="s">
@@ -27901,9 +28127,15 @@
         <v>8</v>
       </c>
       <c r="D695" t="s">
+        <v>332</v>
+      </c>
+      <c r="E695" t="s">
+        <v>574</v>
+      </c>
+      <c r="F695" t="s">
         <v>2812</v>
       </c>
-      <c r="E695" t="s">
+      <c r="G695" t="s">
         <v>2813</v>
       </c>
       <c r="J695" s="3" t="s">
@@ -27927,9 +28159,15 @@
         <v>9</v>
       </c>
       <c r="D696" t="s">
+        <v>332</v>
+      </c>
+      <c r="E696" t="s">
+        <v>574</v>
+      </c>
+      <c r="F696" t="s">
         <v>2812</v>
       </c>
-      <c r="E696" t="s">
+      <c r="G696" t="s">
         <v>2813</v>
       </c>
       <c r="J696" s="3" t="s">
@@ -27953,9 +28191,15 @@
         <v>10</v>
       </c>
       <c r="D697" t="s">
+        <v>332</v>
+      </c>
+      <c r="E697" t="s">
+        <v>574</v>
+      </c>
+      <c r="F697" t="s">
         <v>2812</v>
       </c>
-      <c r="E697" t="s">
+      <c r="G697" t="s">
         <v>2813</v>
       </c>
       <c r="J697" s="3" t="s">
@@ -27979,9 +28223,15 @@
         <v>11</v>
       </c>
       <c r="D698" t="s">
+        <v>332</v>
+      </c>
+      <c r="E698" t="s">
+        <v>574</v>
+      </c>
+      <c r="F698" t="s">
         <v>2812</v>
       </c>
-      <c r="E698" t="s">
+      <c r="G698" t="s">
         <v>2813</v>
       </c>
       <c r="J698" s="3" t="s">
@@ -28005,9 +28255,15 @@
         <v>12</v>
       </c>
       <c r="D699" t="s">
+        <v>332</v>
+      </c>
+      <c r="E699" t="s">
+        <v>574</v>
+      </c>
+      <c r="F699" t="s">
         <v>2812</v>
       </c>
-      <c r="E699" t="s">
+      <c r="G699" t="s">
         <v>2813</v>
       </c>
       <c r="J699" s="3" t="s">
@@ -28031,9 +28287,15 @@
         <v>13</v>
       </c>
       <c r="D700" t="s">
+        <v>332</v>
+      </c>
+      <c r="E700" t="s">
+        <v>574</v>
+      </c>
+      <c r="F700" t="s">
         <v>2812</v>
       </c>
-      <c r="E700" t="s">
+      <c r="G700" t="s">
         <v>2813</v>
       </c>
       <c r="J700" s="3" t="s">
@@ -28057,9 +28319,15 @@
         <v>14</v>
       </c>
       <c r="D701" t="s">
+        <v>332</v>
+      </c>
+      <c r="E701" t="s">
+        <v>574</v>
+      </c>
+      <c r="F701" t="s">
         <v>2812</v>
       </c>
-      <c r="E701" t="s">
+      <c r="G701" t="s">
         <v>2813</v>
       </c>
       <c r="J701" s="3" t="s">
@@ -28083,9 +28351,15 @@
         <v>15</v>
       </c>
       <c r="D702" t="s">
+        <v>332</v>
+      </c>
+      <c r="E702" t="s">
+        <v>574</v>
+      </c>
+      <c r="F702" t="s">
         <v>2812</v>
       </c>
-      <c r="E702" t="s">
+      <c r="G702" t="s">
         <v>2813</v>
       </c>
       <c r="J702" s="3" t="s">
@@ -28109,9 +28383,15 @@
         <v>16</v>
       </c>
       <c r="D703" t="s">
+        <v>332</v>
+      </c>
+      <c r="E703" t="s">
+        <v>574</v>
+      </c>
+      <c r="F703" t="s">
         <v>2812</v>
       </c>
-      <c r="E703" t="s">
+      <c r="G703" t="s">
         <v>2813</v>
       </c>
       <c r="J703" s="3" t="s">
@@ -28135,9 +28415,15 @@
         <v>17</v>
       </c>
       <c r="D704" t="s">
+        <v>332</v>
+      </c>
+      <c r="E704" t="s">
+        <v>574</v>
+      </c>
+      <c r="F704" t="s">
         <v>2812</v>
       </c>
-      <c r="E704" t="s">
+      <c r="G704" t="s">
         <v>2813</v>
       </c>
       <c r="J704" s="3" t="s">
@@ -28161,9 +28447,15 @@
         <v>18</v>
       </c>
       <c r="D705" t="s">
+        <v>332</v>
+      </c>
+      <c r="E705" t="s">
+        <v>574</v>
+      </c>
+      <c r="F705" t="s">
         <v>2812</v>
       </c>
-      <c r="E705" t="s">
+      <c r="G705" t="s">
         <v>2813</v>
       </c>
       <c r="J705" s="3" t="s">
@@ -28187,9 +28479,15 @@
         <v>19</v>
       </c>
       <c r="D706" t="s">
+        <v>332</v>
+      </c>
+      <c r="E706" t="s">
+        <v>574</v>
+      </c>
+      <c r="F706" t="s">
         <v>2812</v>
       </c>
-      <c r="E706" t="s">
+      <c r="G706" t="s">
         <v>2813</v>
       </c>
       <c r="J706" s="3" t="s">
@@ -28213,9 +28511,15 @@
         <v>20</v>
       </c>
       <c r="D707" t="s">
+        <v>332</v>
+      </c>
+      <c r="E707" t="s">
+        <v>574</v>
+      </c>
+      <c r="F707" t="s">
         <v>2812</v>
       </c>
-      <c r="E707" t="s">
+      <c r="G707" t="s">
         <v>2813</v>
       </c>
       <c r="J707" s="3" t="s">
@@ -28239,9 +28543,15 @@
         <v>21</v>
       </c>
       <c r="D708" t="s">
+        <v>332</v>
+      </c>
+      <c r="E708" t="s">
+        <v>574</v>
+      </c>
+      <c r="F708" t="s">
         <v>2812</v>
       </c>
-      <c r="E708" t="s">
+      <c r="G708" t="s">
         <v>2813</v>
       </c>
       <c r="J708" s="3" t="s">
@@ -28265,9 +28575,15 @@
         <v>22</v>
       </c>
       <c r="D709" t="s">
+        <v>332</v>
+      </c>
+      <c r="E709" t="s">
+        <v>574</v>
+      </c>
+      <c r="F709" t="s">
         <v>2812</v>
       </c>
-      <c r="E709" t="s">
+      <c r="G709" t="s">
         <v>2813</v>
       </c>
       <c r="J709" s="3" t="s">
@@ -28291,9 +28607,15 @@
         <v>23</v>
       </c>
       <c r="D710" t="s">
+        <v>332</v>
+      </c>
+      <c r="E710" t="s">
+        <v>574</v>
+      </c>
+      <c r="F710" t="s">
         <v>2812</v>
       </c>
-      <c r="E710" t="s">
+      <c r="G710" t="s">
         <v>2813</v>
       </c>
       <c r="J710" s="3" t="s">
@@ -28317,9 +28639,15 @@
         <v>24</v>
       </c>
       <c r="D711" t="s">
+        <v>332</v>
+      </c>
+      <c r="E711" t="s">
+        <v>574</v>
+      </c>
+      <c r="F711" t="s">
         <v>2812</v>
       </c>
-      <c r="E711" t="s">
+      <c r="G711" t="s">
         <v>2813</v>
       </c>
       <c r="J711" s="3" t="s">
@@ -28343,9 +28671,15 @@
         <v>25</v>
       </c>
       <c r="D712" t="s">
+        <v>332</v>
+      </c>
+      <c r="E712" t="s">
+        <v>574</v>
+      </c>
+      <c r="F712" t="s">
         <v>2812</v>
       </c>
-      <c r="E712" t="s">
+      <c r="G712" t="s">
         <v>2813</v>
       </c>
       <c r="J712" s="3" t="s">
@@ -28369,9 +28703,15 @@
         <v>26</v>
       </c>
       <c r="D713" t="s">
+        <v>332</v>
+      </c>
+      <c r="E713" t="s">
+        <v>574</v>
+      </c>
+      <c r="F713" t="s">
         <v>2812</v>
       </c>
-      <c r="E713" t="s">
+      <c r="G713" t="s">
         <v>2813</v>
       </c>
       <c r="J713" s="3" t="s">
@@ -28395,9 +28735,15 @@
         <v>27</v>
       </c>
       <c r="D714" t="s">
+        <v>332</v>
+      </c>
+      <c r="E714" t="s">
+        <v>574</v>
+      </c>
+      <c r="F714" t="s">
         <v>2812</v>
       </c>
-      <c r="E714" t="s">
+      <c r="G714" t="s">
         <v>2813</v>
       </c>
       <c r="J714" s="3" t="s">
@@ -28421,9 +28767,15 @@
         <v>28</v>
       </c>
       <c r="D715" t="s">
+        <v>332</v>
+      </c>
+      <c r="E715" t="s">
+        <v>574</v>
+      </c>
+      <c r="F715" t="s">
         <v>2812</v>
       </c>
-      <c r="E715" t="s">
+      <c r="G715" t="s">
         <v>2813</v>
       </c>
       <c r="J715" s="3" t="s">
@@ -28447,9 +28799,15 @@
         <v>29</v>
       </c>
       <c r="D716" t="s">
+        <v>332</v>
+      </c>
+      <c r="E716" t="s">
+        <v>574</v>
+      </c>
+      <c r="F716" t="s">
         <v>2812</v>
       </c>
-      <c r="E716" t="s">
+      <c r="G716" t="s">
         <v>2813</v>
       </c>
       <c r="J716" s="3" t="s">
@@ -28473,9 +28831,15 @@
         <v>30</v>
       </c>
       <c r="D717" t="s">
+        <v>332</v>
+      </c>
+      <c r="E717" t="s">
+        <v>574</v>
+      </c>
+      <c r="F717" t="s">
         <v>2812</v>
       </c>
-      <c r="E717" t="s">
+      <c r="G717" t="s">
         <v>2813</v>
       </c>
       <c r="J717" s="3" t="s">
@@ -28499,9 +28863,15 @@
         <v>2810</v>
       </c>
       <c r="D718" t="s">
+        <v>332</v>
+      </c>
+      <c r="E718" t="s">
+        <v>574</v>
+      </c>
+      <c r="F718" t="s">
         <v>2812</v>
       </c>
-      <c r="E718" t="s">
+      <c r="G718" t="s">
         <v>2813</v>
       </c>
       <c r="J718" t="s">
@@ -29099,10 +29469,764 @@
         <v>756</v>
       </c>
     </row>
+    <row r="740" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A740" t="s">
+        <v>2857</v>
+      </c>
+      <c r="B740" t="s">
+        <v>2891</v>
+      </c>
+      <c r="D740" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E740" t="s">
+        <v>577</v>
+      </c>
+      <c r="J740" s="3" t="s">
+        <v>2780</v>
+      </c>
+      <c r="K740">
+        <v>3</v>
+      </c>
+      <c r="L740">
+        <v>6</v>
+      </c>
+      <c r="M740" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="741" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A741" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B741" t="s">
+        <v>2884</v>
+      </c>
+      <c r="D741" t="s">
+        <v>127</v>
+      </c>
+      <c r="E741" t="s">
+        <v>569</v>
+      </c>
+      <c r="J741" t="s">
+        <v>64</v>
+      </c>
+      <c r="K741">
+        <v>3</v>
+      </c>
+      <c r="L741">
+        <v>6</v>
+      </c>
+      <c r="M741" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="742" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A742" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B742" t="s">
+        <v>781</v>
+      </c>
+      <c r="D742" t="s">
+        <v>780</v>
+      </c>
+      <c r="E742" t="s">
+        <v>781</v>
+      </c>
+      <c r="J742" t="s">
+        <v>64</v>
+      </c>
+      <c r="K742">
+        <v>3</v>
+      </c>
+      <c r="L742">
+        <v>6</v>
+      </c>
+      <c r="M742" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="743" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A743" t="s">
+        <v>2860</v>
+      </c>
+      <c r="B743" t="s">
+        <v>2892</v>
+      </c>
+      <c r="D743" t="s">
+        <v>127</v>
+      </c>
+      <c r="E743" t="s">
+        <v>569</v>
+      </c>
+      <c r="J743" t="s">
+        <v>64</v>
+      </c>
+      <c r="K743">
+        <v>3</v>
+      </c>
+      <c r="L743">
+        <v>6</v>
+      </c>
+      <c r="M743" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="744" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A744" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B744" t="s">
+        <v>2885</v>
+      </c>
+      <c r="D744" t="s">
+        <v>127</v>
+      </c>
+      <c r="E744" t="s">
+        <v>569</v>
+      </c>
+      <c r="J744" t="s">
+        <v>64</v>
+      </c>
+      <c r="K744">
+        <v>3</v>
+      </c>
+      <c r="L744">
+        <v>6</v>
+      </c>
+      <c r="M744" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="745" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A745" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B745" t="s">
+        <v>2886</v>
+      </c>
+      <c r="D745" t="s">
+        <v>952</v>
+      </c>
+      <c r="E745" t="s">
+        <v>951</v>
+      </c>
+      <c r="J745" t="s">
+        <v>64</v>
+      </c>
+      <c r="K745">
+        <v>3</v>
+      </c>
+      <c r="L745">
+        <v>6</v>
+      </c>
+      <c r="M745" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="746" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A746" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B746" t="s">
+        <v>2887</v>
+      </c>
+      <c r="D746" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E746" t="s">
+        <v>577</v>
+      </c>
+      <c r="J746" t="s">
+        <v>64</v>
+      </c>
+      <c r="K746">
+        <v>3</v>
+      </c>
+      <c r="L746">
+        <v>6</v>
+      </c>
+      <c r="M746" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="747" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A747" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B747" t="s">
+        <v>2913</v>
+      </c>
+      <c r="D747" t="s">
+        <v>755</v>
+      </c>
+      <c r="E747" t="s">
+        <v>2914</v>
+      </c>
+      <c r="J747" t="s">
+        <v>55</v>
+      </c>
+      <c r="K747">
+        <v>3</v>
+      </c>
+      <c r="L747">
+        <v>6</v>
+      </c>
+      <c r="M747" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="748" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A748" t="s">
+        <v>2894</v>
+      </c>
+      <c r="B748" t="s">
+        <v>2895</v>
+      </c>
+      <c r="D748" t="s">
+        <v>630</v>
+      </c>
+      <c r="E748" t="s">
+        <v>631</v>
+      </c>
+      <c r="J748" t="s">
+        <v>64</v>
+      </c>
+      <c r="K748">
+        <v>3</v>
+      </c>
+      <c r="L748">
+        <v>6</v>
+      </c>
+      <c r="M748" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="749" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A749" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B749" t="s">
+        <v>2896</v>
+      </c>
+      <c r="D749" t="s">
+        <v>127</v>
+      </c>
+      <c r="E749" t="s">
+        <v>569</v>
+      </c>
+      <c r="J749" t="s">
+        <v>55</v>
+      </c>
+      <c r="K749">
+        <v>3</v>
+      </c>
+      <c r="L749">
+        <v>6</v>
+      </c>
+      <c r="M749" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="750" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A750" t="s">
+        <v>2865</v>
+      </c>
+      <c r="B750" t="s">
+        <v>2897</v>
+      </c>
+      <c r="D750" t="s">
+        <v>54</v>
+      </c>
+      <c r="E750" t="s">
+        <v>566</v>
+      </c>
+      <c r="J750" t="s">
+        <v>55</v>
+      </c>
+      <c r="K750">
+        <v>3</v>
+      </c>
+      <c r="L750">
+        <v>6</v>
+      </c>
+      <c r="M750" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="751" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A751" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B751" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D751" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E751" t="s">
+        <v>577</v>
+      </c>
+      <c r="J751" t="s">
+        <v>64</v>
+      </c>
+      <c r="K751">
+        <v>3</v>
+      </c>
+      <c r="L751">
+        <v>6</v>
+      </c>
+      <c r="M751" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="752" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A752" t="s">
+        <v>2867</v>
+      </c>
+      <c r="B752" t="s">
+        <v>2899</v>
+      </c>
+      <c r="D752" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E752" t="s">
+        <v>577</v>
+      </c>
+      <c r="J752" t="s">
+        <v>301</v>
+      </c>
+      <c r="K752">
+        <v>3</v>
+      </c>
+      <c r="L752">
+        <v>6</v>
+      </c>
+      <c r="M752" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="753" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A753" t="s">
+        <v>2868</v>
+      </c>
+      <c r="B753" t="s">
+        <v>2888</v>
+      </c>
+      <c r="D753" t="s">
+        <v>127</v>
+      </c>
+      <c r="E753" t="s">
+        <v>569</v>
+      </c>
+      <c r="J753" t="s">
+        <v>64</v>
+      </c>
+      <c r="K753">
+        <v>3</v>
+      </c>
+      <c r="L753">
+        <v>6</v>
+      </c>
+      <c r="M753" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="754" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A754" t="s">
+        <v>2869</v>
+      </c>
+      <c r="B754" t="s">
+        <v>2900</v>
+      </c>
+      <c r="D754" t="s">
+        <v>127</v>
+      </c>
+      <c r="E754" t="s">
+        <v>569</v>
+      </c>
+      <c r="J754" t="s">
+        <v>64</v>
+      </c>
+      <c r="K754">
+        <v>3</v>
+      </c>
+      <c r="L754">
+        <v>6</v>
+      </c>
+      <c r="M754" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="755" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A755" t="s">
+        <v>2870</v>
+      </c>
+      <c r="B755" t="s">
+        <v>2901</v>
+      </c>
+      <c r="D755" t="s">
+        <v>365</v>
+      </c>
+      <c r="E755" t="s">
+        <v>575</v>
+      </c>
+      <c r="J755" t="s">
+        <v>64</v>
+      </c>
+      <c r="K755">
+        <v>3</v>
+      </c>
+      <c r="L755">
+        <v>6</v>
+      </c>
+      <c r="M755" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="756" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A756" t="s">
+        <v>2871</v>
+      </c>
+      <c r="B756" t="s">
+        <v>2902</v>
+      </c>
+      <c r="D756" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E756" t="s">
+        <v>577</v>
+      </c>
+      <c r="J756" t="s">
+        <v>64</v>
+      </c>
+      <c r="K756">
+        <v>3</v>
+      </c>
+      <c r="L756">
+        <v>6</v>
+      </c>
+      <c r="M756" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="757" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A757" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B757" t="s">
+        <v>2903</v>
+      </c>
+      <c r="D757" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E757" t="s">
+        <v>577</v>
+      </c>
+      <c r="J757" t="s">
+        <v>55</v>
+      </c>
+      <c r="K757">
+        <v>3</v>
+      </c>
+      <c r="L757">
+        <v>6</v>
+      </c>
+      <c r="M757" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="758" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A758" t="s">
+        <v>2873</v>
+      </c>
+      <c r="B758" t="s">
+        <v>2904</v>
+      </c>
+      <c r="D758" t="s">
+        <v>54</v>
+      </c>
+      <c r="E758" t="s">
+        <v>566</v>
+      </c>
+      <c r="J758" t="s">
+        <v>55</v>
+      </c>
+      <c r="K758">
+        <v>3</v>
+      </c>
+      <c r="L758">
+        <v>6</v>
+      </c>
+      <c r="M758" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="759" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A759" t="s">
+        <v>2874</v>
+      </c>
+      <c r="B759" t="s">
+        <v>2905</v>
+      </c>
+      <c r="D759" t="s">
+        <v>2741</v>
+      </c>
+      <c r="E759" t="s">
+        <v>2740</v>
+      </c>
+      <c r="J759" t="s">
+        <v>64</v>
+      </c>
+      <c r="K759">
+        <v>3</v>
+      </c>
+      <c r="L759">
+        <v>6</v>
+      </c>
+      <c r="M759" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="760" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A760" t="s">
+        <v>2875</v>
+      </c>
+      <c r="B760" t="s">
+        <v>2906</v>
+      </c>
+      <c r="D760" t="s">
+        <v>2395</v>
+      </c>
+      <c r="E760" t="s">
+        <v>2394</v>
+      </c>
+      <c r="J760" t="s">
+        <v>64</v>
+      </c>
+      <c r="K760">
+        <v>3</v>
+      </c>
+      <c r="L760">
+        <v>6</v>
+      </c>
+      <c r="M760" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="761" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A761" t="s">
+        <v>2876</v>
+      </c>
+      <c r="B761" t="s">
+        <v>2907</v>
+      </c>
+      <c r="D761" t="s">
+        <v>54</v>
+      </c>
+      <c r="E761" t="s">
+        <v>566</v>
+      </c>
+      <c r="J761" t="s">
+        <v>55</v>
+      </c>
+      <c r="K761">
+        <v>3</v>
+      </c>
+      <c r="L761">
+        <v>6</v>
+      </c>
+      <c r="M761" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="762" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A762" t="s">
+        <v>2877</v>
+      </c>
+      <c r="B762" t="s">
+        <v>2889</v>
+      </c>
+      <c r="D762" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E762" t="s">
+        <v>577</v>
+      </c>
+      <c r="J762" t="s">
+        <v>64</v>
+      </c>
+      <c r="K762">
+        <v>3</v>
+      </c>
+      <c r="L762">
+        <v>6</v>
+      </c>
+      <c r="M762" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="763" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A763" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B763" t="s">
+        <v>2908</v>
+      </c>
+      <c r="D763" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E763" t="s">
+        <v>577</v>
+      </c>
+      <c r="J763" t="s">
+        <v>64</v>
+      </c>
+      <c r="K763">
+        <v>3</v>
+      </c>
+      <c r="L763">
+        <v>6</v>
+      </c>
+      <c r="M763" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="764" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A764" t="s">
+        <v>2879</v>
+      </c>
+      <c r="B764" t="s">
+        <v>2909</v>
+      </c>
+      <c r="D764" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E764" t="s">
+        <v>577</v>
+      </c>
+      <c r="J764" t="s">
+        <v>64</v>
+      </c>
+      <c r="K764">
+        <v>3</v>
+      </c>
+      <c r="L764">
+        <v>6</v>
+      </c>
+      <c r="M764" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="765" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A765" t="s">
+        <v>2880</v>
+      </c>
+      <c r="B765" t="s">
+        <v>2910</v>
+      </c>
+      <c r="D765" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E765" t="s">
+        <v>577</v>
+      </c>
+      <c r="J765" t="s">
+        <v>64</v>
+      </c>
+      <c r="K765">
+        <v>3</v>
+      </c>
+      <c r="L765">
+        <v>6</v>
+      </c>
+      <c r="M765" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="766" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A766" t="s">
+        <v>2881</v>
+      </c>
+      <c r="B766" t="s">
+        <v>2890</v>
+      </c>
+      <c r="D766" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E766" t="s">
+        <v>577</v>
+      </c>
+      <c r="J766" t="s">
+        <v>64</v>
+      </c>
+      <c r="K766">
+        <v>3</v>
+      </c>
+      <c r="L766">
+        <v>6</v>
+      </c>
+      <c r="M766" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="767" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A767" t="s">
+        <v>2882</v>
+      </c>
+      <c r="B767" t="s">
+        <v>2911</v>
+      </c>
+      <c r="D767" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E767" t="s">
+        <v>577</v>
+      </c>
+      <c r="J767" t="s">
+        <v>64</v>
+      </c>
+      <c r="K767">
+        <v>3</v>
+      </c>
+      <c r="L767">
+        <v>6</v>
+      </c>
+      <c r="M767" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="768" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A768" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B768" t="s">
+        <v>2912</v>
+      </c>
+      <c r="D768" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E768" t="s">
+        <v>577</v>
+      </c>
+      <c r="J768" t="s">
+        <v>302</v>
+      </c>
+      <c r="K768">
+        <v>3</v>
+      </c>
+      <c r="L768">
+        <v>6</v>
+      </c>
+      <c r="M768" t="s">
+        <v>756</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M686" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}"/>
-  <conditionalFormatting sqref="A1:A538 A540:A616 A620:A1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+  <conditionalFormatting sqref="A1:A538 A540:A616 A620:A739 A741:A1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -30497,7 +31621,7 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A67">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46368,7 +47492,7 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A614">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49471,11 +50595,11 @@
   </sheetData>
   <autoFilter ref="A1:A616" xr:uid="{CA85B85C-B632-4DE2-B59B-FD77C3B41E34}">
     <filterColumn colId="0">
-      <colorFilter dxfId="6"/>
+      <colorFilter dxfId="7"/>
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -63616,8 +64740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D369D01-9764-417F-BDC6-1E0EEA4F2B74}">
   <dimension ref="A1:S106"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:A106"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63628,18 +64752,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>2624</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2671</v>
+      <c r="A1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>568</v>
+        <v>2813</v>
       </c>
       <c r="E1" s="6" t="str">
         <f t="shared" ref="E1:E32" si="0">"[['"&amp;A1&amp;"'], ['"&amp;B1&amp;"'], '"&amp;D1&amp;"', '3']"</f>
-        <v>[['세탁소'], ['прачечная / химчистка'], 'место', '3']</v>
+        <v>[['하루'], ['1'], 'день месяца', '3']</v>
       </c>
       <c r="O1" t="s">
         <v>2521</v>
@@ -63655,18 +64779,18 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2641</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2677</v>
+      <c r="A2" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2394</v>
+        <v>2813</v>
       </c>
       <c r="E2" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['발표'], ['презентация / доклад'], 'профессия', '3']</v>
+        <v>[['이틀'], ['2'], 'день месяца', '3']</v>
       </c>
       <c r="O2" t="s">
         <v>2522</v>
@@ -63682,18 +64806,18 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2697</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2698</v>
+      <c r="A3" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>871</v>
+        <v>2813</v>
       </c>
       <c r="E3" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['걱정이다'], ['беспокоиться / беспокоиться о чем-то'], 'состояние', '3']</v>
+        <v>[['사흘'], ['3'], 'день месяца', '3']</v>
       </c>
       <c r="O3" t="s">
         <v>2523</v>
@@ -63709,18 +64833,18 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2692</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2678</v>
+      <c r="A4" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>871</v>
+        <v>2813</v>
       </c>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['걱정되다'], ['беспокоиться / волноваться'], 'состояние', '3']</v>
+        <v>[['나흘'], ['4'], 'день месяца', '3']</v>
       </c>
       <c r="O4" t="s">
         <v>2524</v>
@@ -63736,18 +64860,18 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>2642</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2679</v>
+      <c r="A5" t="s">
+        <v>2784</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>587</v>
+        <v>2813</v>
       </c>
       <c r="E5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['지저분하다'], ['грязный / неряшливый'], 'люди', '3']</v>
+        <v>[['닷새'], ['5'], 'день месяца', '3']</v>
       </c>
       <c r="O5" t="s">
         <v>2525</v>
@@ -63763,18 +64887,18 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>2643</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2680</v>
+      <c r="A6" t="s">
+        <v>2811</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>566</v>
+        <v>2813</v>
       </c>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['끝내다'], ['заканчивать / завершать'], 'действие', '3']</v>
+        <v>[['엿새'], ['6'], 'день месяца', '3']</v>
       </c>
       <c r="O6" t="s">
         <v>2526</v>
@@ -63790,18 +64914,18 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>2644</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2681</v>
+      <c r="A7" t="s">
+        <v>2785</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['여러 가지'], ['различный / разнообразный'], 'другое', '3']</v>
+        <v>[['이레'], ['7'], 'день месяца', '3']</v>
       </c>
       <c r="O7" t="s">
         <v>2527</v>
@@ -63817,18 +64941,18 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2645</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2682</v>
+      <c r="A8" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>574</v>
+        <v>2813</v>
       </c>
       <c r="E8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['걸리다'], ['длиться (о времени) / занимать времени'], 'время', '3']</v>
+        <v>[['여드레'], ['8'], 'день месяца', '3']</v>
       </c>
       <c r="J8" t="s">
         <v>2476</v>
@@ -63853,18 +64977,18 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>2646</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2647</v>
+      <c r="A9" t="s">
+        <v>2787</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>568</v>
+        <v>2813</v>
       </c>
       <c r="E9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['부엌'], ['кухня (помещение)'], 'место', '3']</v>
+        <v>[['아흐레'], ['9'], 'день месяца', '3']</v>
       </c>
       <c r="J9" t="s">
         <v>2477</v>
@@ -63889,18 +65013,18 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>2648</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2683</v>
+      <c r="A10" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>574</v>
+        <v>2813</v>
       </c>
       <c r="E10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['아까'], ['ранее / недавно / только что'], 'время', '3']</v>
+        <v>[['열흘'], ['10'], 'день месяца', '3']</v>
       </c>
       <c r="J10" t="s">
         <v>2478</v>
@@ -63925,18 +65049,18 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>2649</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2650</v>
+      <c r="A11" t="s">
+        <v>2789</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>569</v>
+        <v>2813</v>
       </c>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['갈아입다'], ['переодеваться'], 'одежда', '3']</v>
+        <v>[['열하루'], ['11'], 'день месяца', '3']</v>
       </c>
       <c r="J11" t="s">
         <v>2479</v>
@@ -63961,18 +65085,18 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>2651</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2693</v>
+      <c r="A12" t="s">
+        <v>2790</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>566</v>
+        <v>2813</v>
       </c>
       <c r="E12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['무리'], ['сложно что-то сделать'], 'действие', '3']</v>
+        <v>[['열이틀'], ['12'], 'день месяца', '3']</v>
       </c>
       <c r="J12" t="s">
         <v>2480</v>
@@ -63997,18 +65121,18 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>2652</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2684</v>
+      <c r="A13" t="s">
+        <v>2791</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['싫다'], ['не хотеть / не нравиться'], 'другое', '3']</v>
+        <v>[['열사흘'], ['13'], 'день месяца', '3']</v>
       </c>
       <c r="J13" t="s">
         <v>2481</v>
@@ -64033,18 +65157,18 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>2653</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2685</v>
+      <c r="A14" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>574</v>
+        <v>2813</v>
       </c>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['일단'], ['сначала / сперва / в первую очередь'], 'время', '3']</v>
+        <v>[['열나흘'], ['14'], 'день месяца', '3']</v>
       </c>
       <c r="J14" t="s">
         <v>2482</v>
@@ -64069,18 +65193,18 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>2654</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>2694</v>
+      <c r="A15" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['또'], ['снова / опять / еще раз'], 'другое', '3']</v>
+        <v>[['열닷새'], ['15'], 'день месяца', '3']</v>
       </c>
       <c r="J15" t="s">
         <v>2483</v>
@@ -64105,18 +65229,18 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>2655</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>2686</v>
+      <c r="A16" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>574</v>
+        <v>2813</v>
       </c>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['천천히'], ['медленно / неторопливо / потихоньку'], 'время', '3']</v>
+        <v>[['열엿새'], ['16'], 'день месяца', '3']</v>
       </c>
       <c r="J16" t="s">
         <v>2484</v>
@@ -64141,18 +65265,18 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>2656</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>2687</v>
+      <c r="A17" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>574</v>
+        <v>2813</v>
       </c>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['새로'], ['вновь / заново'], 'время', '3']</v>
+        <v>[['열이레'], ['17'], 'день месяца', '3']</v>
       </c>
       <c r="J17" t="s">
         <v>2485</v>
@@ -64177,18 +65301,18 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>2657</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>2688</v>
+      <c r="A18" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>574</v>
+        <v>2813</v>
       </c>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['오래'], ['долго / давно'], 'время', '3']</v>
+        <v>[['열여드레'], ['18'], 'день месяца', '3']</v>
       </c>
       <c r="J18" t="s">
         <v>2487</v>
@@ -64213,18 +65337,18 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>2658</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2689</v>
+      <c r="A19" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>571</v>
+        <v>2813</v>
       </c>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['냄새'], ['запах / аромат / вонь'], 'продукты', '3']</v>
+        <v>[['열아흐레'], ['19'], 'день месяца', '3']</v>
       </c>
       <c r="J19" t="s">
         <v>2488</v>
@@ -64249,18 +65373,18 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>2659</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>2660</v>
+      <c r="A20" t="s">
+        <v>2799</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['서류'], ['документ'], 'другое', '3']</v>
+        <v>[['스무날'], ['20'], 'день месяца', '3']</v>
       </c>
       <c r="J20" t="s">
         <v>2489</v>
@@ -64285,18 +65409,18 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>2661</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2662</v>
+      <c r="A21" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>2695</v>
+        <v>2813</v>
       </c>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['외국어'], ['иностранный язык'], 'образование', '3']</v>
+        <v>[['스무하루'], ['21'], 'день месяца', '3']</v>
       </c>
       <c r="J21" t="s">
         <v>2490</v>
@@ -64321,18 +65445,18 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>2663</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>2664</v>
+      <c r="A22" t="s">
+        <v>2801</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>2695</v>
+        <v>2813</v>
       </c>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['한국어능력시험'], ['экзамен ТОПИК'], 'образование', '3']</v>
+        <v>[['스무이틀'], ['22'], 'день месяца', '3']</v>
       </c>
       <c r="J22" t="s">
         <v>2491</v>
@@ -64357,18 +65481,18 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>2665</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>2690</v>
+      <c r="A23" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B23">
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>2695</v>
+        <v>2813</v>
       </c>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['자격증'], ['диплом / сертификат / лицензия'], 'образование', '3']</v>
+        <v>[['스무사흘'], ['23'], 'день месяца', '3']</v>
       </c>
       <c r="O23" t="s">
         <v>2542</v>
@@ -64385,107 +65509,107 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2701</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2736</v>
+        <v>2803</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['계획'], ['планы / дела / проект'], 'другое', '3']</v>
+        <v>[['스무나흘'], ['24'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2706</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2707</v>
+        <v>2804</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['내려가다'], ['спускаться'], 'другое', '3']</v>
+        <v>[['스무닷새'], ['25'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>2434</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2728</v>
+        <v>2805</v>
+      </c>
+      <c r="B26">
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>566</v>
+        <v>2813</v>
       </c>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['돕다'], ['помогать / оказывать помощь'], 'действие', '3']</v>
+        <v>[['스무엿새'], ['26'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>2742</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2729</v>
+        <v>2806</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['밀리다'], ['скапливаться / накапливаться'], 'другое', '3']</v>
+        <v>[['스무이레'], ['27'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2711</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2730</v>
+        <v>2807</v>
+      </c>
+      <c r="B28">
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['방문하다'], ['посетить / прибыть с визитом / навещать'], 'другое', '3']</v>
+        <v>[['스무여드레'], ['28'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>2712</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2731</v>
+        <v>2808</v>
+      </c>
+      <c r="B29">
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>2394</v>
+        <v>2813</v>
       </c>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['봉사'], ['волонтерство / обслуживание'], 'профессия', '3']</v>
+        <v>[['스무아'], ['29'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>2716</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2732</v>
+        <v>2809</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>577</v>
+        <v>2813</v>
       </c>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>[['실컷'], ['вдоволь / сколько угодно'], 'другое', '3']</v>
+        <v>[['그믐'], ['30'], 'день месяца', '3']</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -64890,9 +66014,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O1:O23">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A32">
+  <conditionalFormatting sqref="A31:A32">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A30">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new rulles and words 4-4 and 4-11
</commit_message>
<xml_diff>
--- a/static/word_db.xlsx
+++ b/static/word_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\личное\korean\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781FBFBC-EFAA-4BB7-9171-E7F330559DBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A6AB6B-55D5-4DD2-8CAA-39CD4901DC72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F542CF1A-05FA-47C0-8419-078B32C6E1FC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12141" uniqueCount="3290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12755" uniqueCount="3451">
   <si>
     <t>stage</t>
   </si>
@@ -9904,6 +9904,489 @@
   </si>
   <si>
     <t>встретимся позже</t>
+  </si>
+  <si>
+    <t>그럴게요</t>
+  </si>
+  <si>
+    <t>동료</t>
+  </si>
+  <si>
+    <t>중고</t>
+  </si>
+  <si>
+    <t>어쩌지요</t>
+  </si>
+  <si>
+    <t>기회가 되다</t>
+  </si>
+  <si>
+    <t>안 좋은 일</t>
+  </si>
+  <si>
+    <t>왜 그렇게</t>
+  </si>
+  <si>
+    <t>섭섭하다</t>
+  </si>
+  <si>
+    <t>뵙다</t>
+  </si>
+  <si>
+    <t>잡히다</t>
+  </si>
+  <si>
+    <t>도둑</t>
+  </si>
+  <si>
+    <t>채팅</t>
+  </si>
+  <si>
+    <t>일정</t>
+  </si>
+  <si>
+    <t>화인</t>
+  </si>
+  <si>
+    <t>정성껏</t>
+  </si>
+  <si>
+    <t>때</t>
+  </si>
+  <si>
+    <t>신경을 쓰다</t>
+  </si>
+  <si>
+    <t>이야기를 나누다</t>
+  </si>
+  <si>
+    <t>경우</t>
+  </si>
+  <si>
+    <t>드물다</t>
+  </si>
+  <si>
+    <t>제목</t>
+  </si>
+  <si>
+    <t>감독</t>
+  </si>
+  <si>
+    <t>заголовок / название фильма</t>
+  </si>
+  <si>
+    <t>줄거리</t>
+  </si>
+  <si>
+    <t>배경</t>
+  </si>
+  <si>
+    <t>연기자</t>
+  </si>
+  <si>
+    <t>주인공</t>
+  </si>
+  <si>
+    <t>시청자</t>
+  </si>
+  <si>
+    <t>관객</t>
+  </si>
+  <si>
+    <t>영화 감상</t>
+  </si>
+  <si>
+    <t>영화 음악</t>
+  </si>
+  <si>
+    <t>영화와 드라마</t>
+  </si>
+  <si>
+    <t>Кино и дорамы</t>
+  </si>
+  <si>
+    <t>сюжет / ход развития событий</t>
+  </si>
+  <si>
+    <t>фон / задний план / разворачиваются события</t>
+  </si>
+  <si>
+    <t>актер / актриса</t>
+  </si>
+  <si>
+    <t>персонаж / главный персонаж</t>
+  </si>
+  <si>
+    <t>исполнитель / исполнитель роли</t>
+  </si>
+  <si>
+    <t>телезритель</t>
+  </si>
+  <si>
+    <t>зрители в кино</t>
+  </si>
+  <si>
+    <t>просмотр фильма с наслаждением</t>
+  </si>
+  <si>
+    <t>прослушивание музыки с наслаждением</t>
+  </si>
+  <si>
+    <t>감동적이다</t>
+  </si>
+  <si>
+    <t>흥미롭다</t>
+  </si>
+  <si>
+    <t>영상이 아름답다</t>
+  </si>
+  <si>
+    <t>인상적이다</t>
+  </si>
+  <si>
+    <t>신나다</t>
+  </si>
+  <si>
+    <t>연기를 잘하다</t>
+  </si>
+  <si>
+    <t>기억에 오래 남다</t>
+  </si>
+  <si>
+    <t>трогательный / задевающий / пронзительный</t>
+  </si>
+  <si>
+    <t>впечатление / впечатляющий</t>
+  </si>
+  <si>
+    <t>интересный</t>
+  </si>
+  <si>
+    <t>веселый / духоподъемный</t>
+  </si>
+  <si>
+    <t>прекрасное видео</t>
+  </si>
+  <si>
+    <t>хорошо играет</t>
+  </si>
+  <si>
+    <t>запоминающееся</t>
+  </si>
+  <si>
+    <t>я сделаю это</t>
+  </si>
+  <si>
+    <t>дряхлый / подержанный / БУ</t>
+  </si>
+  <si>
+    <t>коллега / сотрудник / сослуживец</t>
+  </si>
+  <si>
+    <t>есть шанс / возможность</t>
+  </si>
+  <si>
+    <t>что делать / как быть / растерянность</t>
+  </si>
+  <si>
+    <t>плохо / что-то нехорошее</t>
+  </si>
+  <si>
+    <t>почему так?</t>
+  </si>
+  <si>
+    <t>грустно / печально</t>
+  </si>
+  <si>
+    <t>встречать / вежливый аналог 만나다</t>
+  </si>
+  <si>
+    <t>взят / быть взятым</t>
+  </si>
+  <si>
+    <t>вор / кража</t>
+  </si>
+  <si>
+    <t>чат</t>
+  </si>
+  <si>
+    <t>расписание / распорядок / график / план</t>
+  </si>
+  <si>
+    <t>подтвердить / удостовериться</t>
+  </si>
+  <si>
+    <t>искренне / из всех сил</t>
+  </si>
+  <si>
+    <t>заботиться / уделять внимание</t>
+  </si>
+  <si>
+    <t>беседовать</t>
+  </si>
+  <si>
+    <t>редкий</t>
+  </si>
+  <si>
+    <t>случай / ситуация</t>
+  </si>
+  <si>
+    <t>момент / отрезок времени</t>
+  </si>
+  <si>
+    <t>встреча', 'сбор', 'тусовка</t>
+  </si>
+  <si>
+    <t>совместный прием пищи', 'вместе есть</t>
+  </si>
+  <si>
+    <t>угощать', 'угощать едой</t>
+  </si>
+  <si>
+    <t>звать', 'петь</t>
+  </si>
+  <si>
+    <t>не получится прийти', 'не думаю, что не смогу</t>
+  </si>
+  <si>
+    <t>жалко, но ничего не поделаешь', 'знаю, но не могу сделать</t>
+  </si>
+  <si>
+    <t>спасибо, что пришли', 'вы должно быть заняты, спасибо, что пришли</t>
+  </si>
+  <si>
+    <t>коллега', 'сотрудник', 'сослуживец</t>
+  </si>
+  <si>
+    <t>дряхлый', 'подержанный', 'БУ</t>
+  </si>
+  <si>
+    <t>что делать', 'как быть', 'растерянность</t>
+  </si>
+  <si>
+    <t>есть шанс', 'возможность</t>
+  </si>
+  <si>
+    <t>плохо', 'что-то нехорошее</t>
+  </si>
+  <si>
+    <t>грустно', 'печально</t>
+  </si>
+  <si>
+    <t>встречать', 'вежливый аналог 만나다</t>
+  </si>
+  <si>
+    <t>взят', 'быть взятым</t>
+  </si>
+  <si>
+    <t>вор', 'кража</t>
+  </si>
+  <si>
+    <t>расписание', 'распорядок', 'график', 'план</t>
+  </si>
+  <si>
+    <t>подтвердить', 'удостовериться</t>
+  </si>
+  <si>
+    <t>искренне', 'из всех сил</t>
+  </si>
+  <si>
+    <t>момент', 'отрезок времени</t>
+  </si>
+  <si>
+    <t>заботиться', 'уделять внимание</t>
+  </si>
+  <si>
+    <t>случай', 'ситуация</t>
+  </si>
+  <si>
+    <t>заголовок', 'название фильма</t>
+  </si>
+  <si>
+    <t>сюжет', 'ход развития событий</t>
+  </si>
+  <si>
+    <t>фон', 'задний план', 'разворачиваются события</t>
+  </si>
+  <si>
+    <t>актер', 'актриса</t>
+  </si>
+  <si>
+    <t>исполнитель', 'исполнитель роли</t>
+  </si>
+  <si>
+    <t>персонаж', 'главный персонаж</t>
+  </si>
+  <si>
+    <t>трогательный', 'задевающий', 'пронзительный</t>
+  </si>
+  <si>
+    <t>впечатление', 'впечатляющий</t>
+  </si>
+  <si>
+    <t>веселый', 'духоподъемный</t>
+  </si>
+  <si>
+    <t>건강을 유지하다</t>
+  </si>
+  <si>
+    <t>나쁜 습관을 고치다</t>
+  </si>
+  <si>
+    <t>좋은 성적을 받다</t>
+  </si>
+  <si>
+    <t>규칙적으로 생활하다</t>
+  </si>
+  <si>
+    <t>실력을 높이다</t>
+  </si>
+  <si>
+    <t>돈을 모으다</t>
+  </si>
+  <si>
+    <t>결심</t>
+  </si>
+  <si>
+    <t>решительность</t>
+  </si>
+  <si>
+    <t>избавиться от плохой привычки</t>
+  </si>
+  <si>
+    <t>правильно жить</t>
+  </si>
+  <si>
+    <t>копить деньги</t>
+  </si>
+  <si>
+    <t>уровень знаний / повышать навыки</t>
+  </si>
+  <si>
+    <t>хорошие результаты</t>
+  </si>
+  <si>
+    <t>꾸준히 운동하다</t>
+  </si>
+  <si>
+    <t>커피를 줄이다</t>
+  </si>
+  <si>
+    <t>독서를 하다</t>
+  </si>
+  <si>
+    <t>할 일을 미루지 않다</t>
+  </si>
+  <si>
+    <t>술을 끊다</t>
+  </si>
+  <si>
+    <t>담배를 끊다</t>
+  </si>
+  <si>
+    <t>неуклонно</t>
+  </si>
+  <si>
+    <t>пить меньше кофе</t>
+  </si>
+  <si>
+    <t>채소를 많이 먹다</t>
+  </si>
+  <si>
+    <t>читать</t>
+  </si>
+  <si>
+    <t>не откладывать дела на потом</t>
+  </si>
+  <si>
+    <t>бросить пить</t>
+  </si>
+  <si>
+    <t>бросить курить</t>
+  </si>
+  <si>
+    <t>есть много овощей</t>
+  </si>
+  <si>
+    <t>최고</t>
+  </si>
+  <si>
+    <t>한</t>
+  </si>
+  <si>
+    <t>판사</t>
+  </si>
+  <si>
+    <t>목록</t>
+  </si>
+  <si>
+    <t>계획표</t>
+  </si>
+  <si>
+    <t>환경</t>
+  </si>
+  <si>
+    <t>적금 통장</t>
+  </si>
+  <si>
+    <t>잊다</t>
+  </si>
+  <si>
+    <t>대화하다</t>
+  </si>
+  <si>
+    <t>웬일</t>
+  </si>
+  <si>
+    <t>딱</t>
+  </si>
+  <si>
+    <t>복숭아</t>
+  </si>
+  <si>
+    <t>몰표</t>
+  </si>
+  <si>
+    <t>배낭여행</t>
+  </si>
+  <si>
+    <t>비용</t>
+  </si>
+  <si>
+    <t>새해</t>
+  </si>
+  <si>
+    <t>문화생활</t>
+  </si>
+  <si>
+    <t>잠이 많다</t>
+  </si>
+  <si>
+    <t>아침잠</t>
+  </si>
+  <si>
+    <t>알차다</t>
+  </si>
+  <si>
+    <t>평균</t>
+  </si>
+  <si>
+    <t>용돈</t>
+  </si>
+  <si>
+    <t>줄이다</t>
+  </si>
+  <si>
+    <t>여행비</t>
+  </si>
+  <si>
+    <t>쓸데없다</t>
+  </si>
+  <si>
+    <t>절대로</t>
+  </si>
+  <si>
+    <t>마련하다</t>
   </si>
 </sst>
 </file>
@@ -9975,7 +10458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -9992,11 +10475,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -10357,11 +10861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9B2CAE-2EA5-4110-8EF6-0CACBAA50220}">
-  <dimension ref="A1:O1191"/>
+  <dimension ref="A1:O1286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1186" sqref="B1186"/>
+      <pane ySplit="1" topLeftCell="A1223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1225" sqref="A1225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51209,14 +51713,1687 @@
         <v>2831</v>
       </c>
     </row>
+    <row r="1192" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1192" s="10" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B1192" t="s">
+        <v>3346</v>
+      </c>
+      <c r="D1192" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1192" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1192,helper!$A$1:$A$41,0))</f>
+        <v>действие</v>
+      </c>
+      <c r="K1192">
+        <v>4</v>
+      </c>
+      <c r="L1192">
+        <v>3</v>
+      </c>
+      <c r="M1192" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1192" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1192" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1193" s="10" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B1193" t="s">
+        <v>3348</v>
+      </c>
+      <c r="D1193" t="s">
+        <v>579</v>
+      </c>
+      <c r="E1193" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1193,helper!$A$1:$A$41,0))</f>
+        <v>люди</v>
+      </c>
+      <c r="K1193">
+        <v>4</v>
+      </c>
+      <c r="L1193">
+        <v>3</v>
+      </c>
+      <c r="M1193" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1193" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1193" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1194" s="10" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B1194" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D1194" t="s">
+        <v>859</v>
+      </c>
+      <c r="E1194" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1194,helper!$A$1:$A$41,0))</f>
+        <v>состояние</v>
+      </c>
+      <c r="K1194">
+        <v>4</v>
+      </c>
+      <c r="L1194">
+        <v>3</v>
+      </c>
+      <c r="M1194" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1194" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1194" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1195" s="10" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>3350</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1195" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1195,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1195">
+        <v>4</v>
+      </c>
+      <c r="L1195">
+        <v>3</v>
+      </c>
+      <c r="M1195" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1195" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1195" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1196" s="10" t="s">
+        <v>3294</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>3349</v>
+      </c>
+      <c r="D1196" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1196" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1196,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1196">
+        <v>4</v>
+      </c>
+      <c r="L1196">
+        <v>3</v>
+      </c>
+      <c r="M1196" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1196" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1196" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1197" s="10" t="s">
+        <v>3295</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>3351</v>
+      </c>
+      <c r="D1197" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1197" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1197,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1197">
+        <v>4</v>
+      </c>
+      <c r="L1197">
+        <v>3</v>
+      </c>
+      <c r="M1197" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1197" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1197" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1198" s="10" t="s">
+        <v>3296</v>
+      </c>
+      <c r="B1198" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D1198" t="s">
+        <v>744</v>
+      </c>
+      <c r="E1198" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1198,helper!$A$1:$A$41,0))</f>
+        <v>общение</v>
+      </c>
+      <c r="K1198">
+        <v>4</v>
+      </c>
+      <c r="L1198">
+        <v>3</v>
+      </c>
+      <c r="M1198" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1198" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1198" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1199" s="10" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B1199" t="s">
+        <v>3353</v>
+      </c>
+      <c r="D1199" t="s">
+        <v>859</v>
+      </c>
+      <c r="E1199" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1199,helper!$A$1:$A$41,0))</f>
+        <v>состояние</v>
+      </c>
+      <c r="K1199">
+        <v>4</v>
+      </c>
+      <c r="L1199">
+        <v>3</v>
+      </c>
+      <c r="M1199" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1199" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1199" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1200" s="10" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B1200" t="s">
+        <v>3354</v>
+      </c>
+      <c r="D1200" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1200" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1200,helper!$A$1:$A$41,0))</f>
+        <v>действие</v>
+      </c>
+      <c r="K1200">
+        <v>4</v>
+      </c>
+      <c r="L1200">
+        <v>3</v>
+      </c>
+      <c r="M1200" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1200" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1200" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1201" s="10" t="s">
+        <v>3299</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>3355</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1201" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1201,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1201">
+        <v>4</v>
+      </c>
+      <c r="L1201">
+        <v>3</v>
+      </c>
+      <c r="M1201" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1201" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1201" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1202" s="10" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>3356</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>579</v>
+      </c>
+      <c r="E1202" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1202,helper!$A$1:$A$41,0))</f>
+        <v>люди</v>
+      </c>
+      <c r="K1202">
+        <v>4</v>
+      </c>
+      <c r="L1202">
+        <v>3</v>
+      </c>
+      <c r="M1202" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1202" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1202" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1203" s="10" t="s">
+        <v>3301</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D1203" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1203" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1203,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1203">
+        <v>4</v>
+      </c>
+      <c r="L1203">
+        <v>3</v>
+      </c>
+      <c r="M1203" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1203" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1203" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1204" s="10" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>3358</v>
+      </c>
+      <c r="D1204" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1204" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1204,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1204">
+        <v>4</v>
+      </c>
+      <c r="L1204">
+        <v>3</v>
+      </c>
+      <c r="M1204" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1204" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1204" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1205" s="10" t="s">
+        <v>3303</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>3359</v>
+      </c>
+      <c r="D1205" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1205" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1205,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1205">
+        <v>4</v>
+      </c>
+      <c r="L1205">
+        <v>3</v>
+      </c>
+      <c r="M1205" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1205" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1205" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1206" s="10" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>3360</v>
+      </c>
+      <c r="D1206" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1206" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1206,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1206">
+        <v>4</v>
+      </c>
+      <c r="L1206">
+        <v>3</v>
+      </c>
+      <c r="M1206" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1206" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1206" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1207" s="10" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>3365</v>
+      </c>
+      <c r="D1207" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1207" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1207,helper!$A$1:$A$41,0))</f>
+        <v>время</v>
+      </c>
+      <c r="K1207">
+        <v>4</v>
+      </c>
+      <c r="L1207">
+        <v>3</v>
+      </c>
+      <c r="M1207" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1207" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1207" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1208" s="10" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>3361</v>
+      </c>
+      <c r="D1208" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1208" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1208,helper!$A$1:$A$41,0))</f>
+        <v>действие</v>
+      </c>
+      <c r="K1208">
+        <v>4</v>
+      </c>
+      <c r="L1208">
+        <v>3</v>
+      </c>
+      <c r="M1208" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1208" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1208" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1209" s="10" t="s">
+        <v>3307</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>3362</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>744</v>
+      </c>
+      <c r="E1209" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1209,helper!$A$1:$A$41,0))</f>
+        <v>общение</v>
+      </c>
+      <c r="K1209">
+        <v>4</v>
+      </c>
+      <c r="L1209">
+        <v>3</v>
+      </c>
+      <c r="M1209" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1209" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1209" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1210" s="10" t="s">
+        <v>3308</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>3364</v>
+      </c>
+      <c r="D1210" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1210" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1210,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1210">
+        <v>4</v>
+      </c>
+      <c r="L1210">
+        <v>3</v>
+      </c>
+      <c r="M1210" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1210" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1210" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1211" s="10" t="s">
+        <v>3309</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>3363</v>
+      </c>
+      <c r="D1211" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1211" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1211,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1211">
+        <v>4</v>
+      </c>
+      <c r="L1211">
+        <v>3</v>
+      </c>
+      <c r="M1211" t="s">
+        <v>3253</v>
+      </c>
+      <c r="N1211" t="s">
+        <v>935</v>
+      </c>
+      <c r="O1211" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1212" s="10" t="s">
+        <v>3397</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>2711</v>
+      </c>
+      <c r="D1212" t="s">
+        <v>859</v>
+      </c>
+      <c r="E1212" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1212,helper!$A$1:$A$41,0))</f>
+        <v>состояние</v>
+      </c>
+      <c r="K1212">
+        <v>4</v>
+      </c>
+      <c r="L1212">
+        <v>4</v>
+      </c>
+      <c r="M1212" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1212" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1212" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1213" s="10" t="s">
+        <v>3398</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>3405</v>
+      </c>
+      <c r="D1213" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1213" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1213,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1213">
+        <v>4</v>
+      </c>
+      <c r="L1213">
+        <v>4</v>
+      </c>
+      <c r="M1213" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1213" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1213" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1214" s="10" t="s">
+        <v>3400</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>3406</v>
+      </c>
+      <c r="D1214" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1214" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1214,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1214">
+        <v>4</v>
+      </c>
+      <c r="L1214">
+        <v>4</v>
+      </c>
+      <c r="M1214" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1214" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1214" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1215" s="10" t="s">
+        <v>3399</v>
+      </c>
+      <c r="B1215" t="s">
+        <v>3409</v>
+      </c>
+      <c r="D1215" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E1215" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1215,helper!$A$1:$A$41,0))</f>
+        <v>образование</v>
+      </c>
+      <c r="K1215">
+        <v>4</v>
+      </c>
+      <c r="L1215">
+        <v>4</v>
+      </c>
+      <c r="M1215" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1215" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1215" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1216" s="10" t="s">
+        <v>3401</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>3408</v>
+      </c>
+      <c r="D1216" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E1216" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1216,helper!$A$1:$A$41,0))</f>
+        <v>образование</v>
+      </c>
+      <c r="K1216">
+        <v>4</v>
+      </c>
+      <c r="L1216">
+        <v>4</v>
+      </c>
+      <c r="M1216" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1216" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1216" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1217" s="10" t="s">
+        <v>3402</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>3407</v>
+      </c>
+      <c r="D1217" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1217" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1217,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1217">
+        <v>4</v>
+      </c>
+      <c r="L1217">
+        <v>4</v>
+      </c>
+      <c r="M1217" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1217" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1217" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1218" s="10" t="s">
+        <v>3410</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>3416</v>
+      </c>
+      <c r="D1218" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1218" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1218,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1218">
+        <v>4</v>
+      </c>
+      <c r="L1218">
+        <v>4</v>
+      </c>
+      <c r="M1218" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1218" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1218" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1219" s="10" t="s">
+        <v>3411</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>3417</v>
+      </c>
+      <c r="D1219" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1219" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1219,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1219">
+        <v>4</v>
+      </c>
+      <c r="L1219">
+        <v>4</v>
+      </c>
+      <c r="M1219" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1219" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1219" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1220" s="10" t="s">
+        <v>3412</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>3419</v>
+      </c>
+      <c r="D1220" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1220" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1220,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1220">
+        <v>4</v>
+      </c>
+      <c r="L1220">
+        <v>4</v>
+      </c>
+      <c r="M1220" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1220" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1220" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1221" s="10" t="s">
+        <v>3413</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>3420</v>
+      </c>
+      <c r="D1221" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1221" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1221,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1221">
+        <v>4</v>
+      </c>
+      <c r="L1221">
+        <v>4</v>
+      </c>
+      <c r="M1221" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1221" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1221" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1222" s="10" t="s">
+        <v>3414</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>3421</v>
+      </c>
+      <c r="D1222" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1222" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1222,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1222">
+        <v>4</v>
+      </c>
+      <c r="L1222">
+        <v>4</v>
+      </c>
+      <c r="M1222" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1222" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1222" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1223" s="10" t="s">
+        <v>3415</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>3422</v>
+      </c>
+      <c r="D1223" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1223" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1223,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1223">
+        <v>4</v>
+      </c>
+      <c r="L1223">
+        <v>4</v>
+      </c>
+      <c r="M1223" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1223" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1223" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1224" s="10" t="s">
+        <v>3418</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>3423</v>
+      </c>
+      <c r="D1224" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1224" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1224,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1224">
+        <v>4</v>
+      </c>
+      <c r="L1224">
+        <v>4</v>
+      </c>
+      <c r="M1224" t="s">
+        <v>3403</v>
+      </c>
+      <c r="N1224" t="s">
+        <v>3404</v>
+      </c>
+      <c r="O1224" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1225" s="10" t="s">
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1226" s="10" t="s">
+        <v>3425</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1227" s="10" t="s">
+        <v>3403</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1228" s="10" t="s">
+        <v>3426</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1229" s="10" t="s">
+        <v>3427</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1230" s="10" t="s">
+        <v>3428</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1231" s="10" t="s">
+        <v>3429</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1232" s="10" t="s">
+        <v>3430</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1233" s="10" t="s">
+        <v>3431</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1234" s="10" t="s">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1235" s="10" t="s">
+        <v>3433</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1236" s="10" t="s">
+        <v>3434</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1237" s="10" t="s">
+        <v>3435</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1238" s="10" t="s">
+        <v>3436</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1239" s="10" t="s">
+        <v>3437</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1240" s="10" t="s">
+        <v>3438</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1241" s="10" t="s">
+        <v>3439</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1242" s="10" t="s">
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1243" s="10" t="s">
+        <v>3441</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1244" s="10" t="s">
+        <v>3442</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1245" s="10" t="s">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1246" s="10" t="s">
+        <v>3444</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1247" s="10" t="s">
+        <v>3445</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1248" s="10" t="s">
+        <v>3446</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1249" s="10" t="s">
+        <v>3447</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1250" s="10" t="s">
+        <v>3448</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1251" s="10" t="s">
+        <v>3449</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1252" s="10" t="s">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1269" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>3312</v>
+      </c>
+      <c r="D1269" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1269" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1269,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1269">
+        <v>4</v>
+      </c>
+      <c r="L1269">
+        <v>11</v>
+      </c>
+      <c r="M1269" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1269" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1269" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1270" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>3323</v>
+      </c>
+      <c r="D1270" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1270" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1270,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1270">
+        <v>4</v>
+      </c>
+      <c r="L1270">
+        <v>11</v>
+      </c>
+      <c r="M1270" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1270" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1270" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1271" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>3324</v>
+      </c>
+      <c r="D1271" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1271" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1271,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1271">
+        <v>4</v>
+      </c>
+      <c r="L1271">
+        <v>11</v>
+      </c>
+      <c r="M1271" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1271" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1271" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1272" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>3064</v>
+      </c>
+      <c r="D1272" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E1272" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1272,helper!$A$1:$A$41,0))</f>
+        <v>профессия</v>
+      </c>
+      <c r="K1272">
+        <v>4</v>
+      </c>
+      <c r="L1272">
+        <v>11</v>
+      </c>
+      <c r="M1272" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1272" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1272" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1273" t="s">
+        <v>429</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>3325</v>
+      </c>
+      <c r="D1273" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E1273" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1273,helper!$A$1:$A$41,0))</f>
+        <v>профессия</v>
+      </c>
+      <c r="K1273">
+        <v>4</v>
+      </c>
+      <c r="L1273">
+        <v>11</v>
+      </c>
+      <c r="M1273" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1273" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1273" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1274" t="s">
+        <v>3315</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>3327</v>
+      </c>
+      <c r="D1274" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E1274" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1274,helper!$A$1:$A$41,0))</f>
+        <v>профессия</v>
+      </c>
+      <c r="K1274">
+        <v>4</v>
+      </c>
+      <c r="L1274">
+        <v>11</v>
+      </c>
+      <c r="M1274" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1274" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1274" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1275" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>3326</v>
+      </c>
+      <c r="D1275" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E1275" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1275,helper!$A$1:$A$41,0))</f>
+        <v>профессия</v>
+      </c>
+      <c r="K1275">
+        <v>4</v>
+      </c>
+      <c r="L1275">
+        <v>11</v>
+      </c>
+      <c r="M1275" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1275" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1275" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1276" t="s">
+        <v>3317</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>3328</v>
+      </c>
+      <c r="D1276" t="s">
+        <v>579</v>
+      </c>
+      <c r="E1276" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1276,helper!$A$1:$A$41,0))</f>
+        <v>люди</v>
+      </c>
+      <c r="K1276">
+        <v>4</v>
+      </c>
+      <c r="L1276">
+        <v>11</v>
+      </c>
+      <c r="M1276" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1276" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1276" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1277" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>3329</v>
+      </c>
+      <c r="D1277" t="s">
+        <v>579</v>
+      </c>
+      <c r="E1277" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1277,helper!$A$1:$A$41,0))</f>
+        <v>люди</v>
+      </c>
+      <c r="K1277">
+        <v>4</v>
+      </c>
+      <c r="L1277">
+        <v>11</v>
+      </c>
+      <c r="M1277" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1277" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1277" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1278" t="s">
+        <v>3319</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>3330</v>
+      </c>
+      <c r="D1278" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E1278" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1278,helper!$A$1:$A$41,0))</f>
+        <v>досуг</v>
+      </c>
+      <c r="K1278">
+        <v>4</v>
+      </c>
+      <c r="L1278">
+        <v>11</v>
+      </c>
+      <c r="M1278" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1278" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1278" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1279" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>3331</v>
+      </c>
+      <c r="D1279" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E1279" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1279,helper!$A$1:$A$41,0))</f>
+        <v>досуг</v>
+      </c>
+      <c r="K1279">
+        <v>4</v>
+      </c>
+      <c r="L1279">
+        <v>11</v>
+      </c>
+      <c r="M1279" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1279" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1279" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1280" t="s">
+        <v>3332</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>3339</v>
+      </c>
+      <c r="D1280" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1280" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1280,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1280">
+        <v>4</v>
+      </c>
+      <c r="L1280">
+        <v>11</v>
+      </c>
+      <c r="M1280" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1280" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1280" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1281" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>3340</v>
+      </c>
+      <c r="D1281" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1281" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1281,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1281">
+        <v>4</v>
+      </c>
+      <c r="L1281">
+        <v>11</v>
+      </c>
+      <c r="M1281" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1281" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1281" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1282" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>3341</v>
+      </c>
+      <c r="D1282" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1282" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1282,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1282">
+        <v>4</v>
+      </c>
+      <c r="L1282">
+        <v>11</v>
+      </c>
+      <c r="M1282" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1282" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1282" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1283" t="s">
+        <v>3336</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>3342</v>
+      </c>
+      <c r="D1283" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1283" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1283,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1283">
+        <v>4</v>
+      </c>
+      <c r="L1283">
+        <v>11</v>
+      </c>
+      <c r="M1283" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1283" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1283" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1284" t="s">
+        <v>3337</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>3344</v>
+      </c>
+      <c r="D1284" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1284" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1284,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1284">
+        <v>4</v>
+      </c>
+      <c r="L1284">
+        <v>11</v>
+      </c>
+      <c r="M1284" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1284" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1284" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1285" t="s">
+        <v>3334</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>3343</v>
+      </c>
+      <c r="D1285" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1285" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1285,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1285">
+        <v>4</v>
+      </c>
+      <c r="L1285">
+        <v>11</v>
+      </c>
+      <c r="M1285" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1285" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1285" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1286" t="s">
+        <v>3338</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>3345</v>
+      </c>
+      <c r="D1286" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1286" t="str">
+        <f>INDEX(helper!$B$1:$B$41,MATCH(Лист1!D1286,helper!$A$1:$A$41,0))</f>
+        <v>другое</v>
+      </c>
+      <c r="K1286">
+        <v>4</v>
+      </c>
+      <c r="L1286">
+        <v>11</v>
+      </c>
+      <c r="M1286" t="s">
+        <v>3321</v>
+      </c>
+      <c r="N1286" t="s">
+        <v>3322</v>
+      </c>
+      <c r="O1286" t="s">
+        <v>827</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O773" xr:uid="{D39886AE-5543-4E07-A729-AC3EEF5E2C50}">
     <sortState ref="A2:O773">
       <sortCondition ref="K1:K773"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A1100 A1038:A1042 A992 A921 A805:A814 A544:A620 A1:A542 A624:A744 A746:A767 A769:A782 A844:A875 A994 A996:A997 A1003 A1005 A1009 A1036 A1107:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+  <conditionalFormatting sqref="A1100 A1038:A1042 A992 A921 A805:A814 A544:A620 A1:A542 A624:A744 A746:A767 A769:A782 A844:A875 A994 A996:A997 A1003 A1005 A1009 A1036 A1107:A1224 A1228:A1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -70762,16 +72939,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8666763D-5C16-4B35-A3B1-FA00CC1306A3}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I32"/>
+    <sheetView topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -70800,7 +72977,7 @@
         <v>745</v>
       </c>
       <c r="I1" s="6" t="str">
-        <f t="shared" ref="I1:I32" si="0">"[['"&amp;A1&amp;"'], ['"&amp;B1&amp;"'], '"&amp;C1&amp;"', '3'"&amp;", ['"&amp;E1&amp;" "&amp;F1&amp;"', '"&amp;E1&amp;" "&amp;G1&amp;"']]"</f>
+        <f t="shared" ref="I1:I64" si="0">"[['"&amp;A1&amp;"'], ['"&amp;B1&amp;"'], '"&amp;C1&amp;"', '3'"&amp;", ['"&amp;E1&amp;" "&amp;F1&amp;"', '"&amp;E1&amp;" "&amp;G1&amp;"']]"</f>
         <v>[['외국에서 생활하다'], ['уклад жизни за границей'], 'релокация', '3', ['2 외국 생활', '2 жизнь за границей']]</v>
       </c>
     </row>
@@ -71678,110 +73855,1542 @@
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>3254</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3262</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G33" t="s">
+        <v>935</v>
+      </c>
+      <c r="I33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['초대하다'], ['приглашать'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3255</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3263</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G34" t="s">
+        <v>935</v>
+      </c>
+      <c r="I34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['초대를 받다'], ['принять приглашение'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>3256</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3366</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G35" t="s">
+        <v>935</v>
+      </c>
+      <c r="I35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['모임을 가지다'], ['встреча', 'сбор', 'тусовка'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3257</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3367</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G36" t="s">
+        <v>935</v>
+      </c>
+      <c r="I36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['식사를 함께 하다'], ['совместный прием пищи', 'вместе есть'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>3261</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3368</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G37" t="s">
+        <v>935</v>
+      </c>
+      <c r="I37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['음식을 대접하다'], ['угощать', 'угощать едой'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>3258</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3369</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G38" t="s">
+        <v>935</v>
+      </c>
+      <c r="I38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['부르다'], ['звать', 'петь'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>3259</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3269</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G39" t="s">
+        <v>935</v>
+      </c>
+      <c r="I39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['파티를 하다'], ['организовать вечеринку'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3267</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G40" t="s">
+        <v>935</v>
+      </c>
+      <c r="I40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['파티를 열다'], ['открывать вечеринку'], 'досуг', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>3270</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3280</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G41" t="s">
+        <v>935</v>
+      </c>
+      <c r="I41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['초대해 줘서 고마워요'], ['спасибо за приглашение'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>3271</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3370</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G42" t="s">
+        <v>935</v>
+      </c>
+      <c r="I42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['저는 못 갈 것 같아요'], ['не получится прийти', 'не думаю, что не смогу'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3283</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G43" t="s">
+        <v>935</v>
+      </c>
+      <c r="I43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['일정 확인해 보고 다시 연락드릴게요'], ['проверю график и перезвоню'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>3273</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G44" t="s">
+        <v>935</v>
+      </c>
+      <c r="I44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['아귑지만 어쩔 수 없네요'], ['жалко, но ничего не поделаешь', 'знаю, но не могу сделать'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>3274</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3282</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G45" t="s">
+        <v>935</v>
+      </c>
+      <c r="I45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['꼭 갈게요'], ['я обязательно пойду'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>3275</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3285</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G46" t="s">
+        <v>935</v>
+      </c>
+      <c r="I46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['꼭 참석할게요'], ['я обязательно поучаствую'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C47" s="3"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>3276</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3286</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G47" t="s">
+        <v>935</v>
+      </c>
+      <c r="I47" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['일이 있어서 참석하기 어려워요'], ['у меня дела, поэтому скорее всего не приду'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C48" s="3"/>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>3277</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3372</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G48" t="s">
+        <v>935</v>
+      </c>
+      <c r="I48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['바쁘실 텐데 와 주셔서 감사해요'], ['спасибо, что пришли', 'вы должно быть заняты, спасибо, что пришли'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C49" s="3"/>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>3278</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3288</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G49" t="s">
+        <v>935</v>
+      </c>
+      <c r="I49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['다음에 봐요'], ['увидимся позже'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C50" s="3"/>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>3279</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3289</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G50" t="s">
+        <v>935</v>
+      </c>
+      <c r="I50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['다음에 만나요'], ['встретимся позже'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C51" s="3"/>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C51" t="s">
+        <v>557</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G51" t="s">
+        <v>935</v>
+      </c>
+      <c r="I51" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['그럴게요'], ['я сделаю это'], 'действие', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C52" s="3"/>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3373</v>
+      </c>
+      <c r="C52" t="s">
+        <v>578</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G52" t="s">
+        <v>935</v>
+      </c>
+      <c r="I52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['동료'], ['коллега', 'сотрудник', 'сослуживец'], 'люди', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C53" s="3"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3374</v>
+      </c>
+      <c r="C53" t="s">
+        <v>860</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G53" t="s">
+        <v>935</v>
+      </c>
+      <c r="I53" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['중고'], ['дряхлый', 'подержанный', 'БУ'], 'состояние', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C54" s="3"/>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3375</v>
+      </c>
+      <c r="C54" t="s">
+        <v>568</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G54" t="s">
+        <v>935</v>
+      </c>
+      <c r="I54" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['어쩌지요'], ['что делать', 'как быть', 'растерянность'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
       <c r="J54" s="3"/>
     </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>3294</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3376</v>
+      </c>
+      <c r="C55" t="s">
+        <v>568</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G55" t="s">
+        <v>935</v>
+      </c>
+      <c r="I55" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['기회가 되다'], ['есть шанс', 'возможность'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="10" t="s">
+        <v>3295</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C56" t="s">
+        <v>568</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G56" t="s">
+        <v>935</v>
+      </c>
+      <c r="I56" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['안 좋은 일'], ['плохо', 'что-то нехорошее'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>3296</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3352</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G57" t="s">
+        <v>935</v>
+      </c>
+      <c r="I57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['왜 그렇게'], ['почему так?'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3378</v>
+      </c>
+      <c r="C58" t="s">
+        <v>860</v>
+      </c>
+      <c r="D58">
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G58" t="s">
+        <v>935</v>
+      </c>
+      <c r="I58" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['섭섭하다'], ['грустно', 'печально'], 'состояние', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3379</v>
+      </c>
+      <c r="C59" t="s">
+        <v>557</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="F59" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G59" t="s">
+        <v>935</v>
+      </c>
+      <c r="I59" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['뵙다'], ['встречать', 'вежливый аналог 만나다'], 'действие', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>3299</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3380</v>
+      </c>
+      <c r="C60" t="s">
+        <v>568</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G60" t="s">
+        <v>935</v>
+      </c>
+      <c r="I60" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['잡히다'], ['взят', 'быть взятым'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C61" t="s">
+        <v>578</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G61" t="s">
+        <v>935</v>
+      </c>
+      <c r="I61" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['도둑'], ['вор', 'кража'], 'люди', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>3301</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3357</v>
+      </c>
+      <c r="C62" t="s">
+        <v>568</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G62" t="s">
+        <v>935</v>
+      </c>
+      <c r="I62" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['채팅'], ['чат'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B63" t="s">
+        <v>3382</v>
+      </c>
+      <c r="C63" t="s">
+        <v>568</v>
+      </c>
+      <c r="D63">
+        <v>4</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G63" t="s">
+        <v>935</v>
+      </c>
+      <c r="I63" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['일정'], ['расписание', 'распорядок', 'график', 'план'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
+        <v>3303</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3383</v>
+      </c>
+      <c r="C64" t="s">
+        <v>568</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G64" t="s">
+        <v>935</v>
+      </c>
+      <c r="I64" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>[['화인'], ['подтвердить', 'удостовериться'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="10" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3384</v>
+      </c>
+      <c r="C65" t="s">
+        <v>568</v>
+      </c>
+      <c r="D65">
+        <v>4</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G65" t="s">
+        <v>935</v>
+      </c>
+      <c r="I65" s="6" t="str">
+        <f t="shared" ref="I65:I88" si="1">"[['"&amp;A65&amp;"'], ['"&amp;B65&amp;"'], '"&amp;C65&amp;"', '3'"&amp;", ['"&amp;E65&amp;" "&amp;F65&amp;"', '"&amp;E65&amp;" "&amp;G65&amp;"']]"</f>
+        <v>[['정성껏'], ['искренне', 'из всех сил'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="10" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B66" t="s">
+        <v>3385</v>
+      </c>
+      <c r="C66" t="s">
+        <v>565</v>
+      </c>
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G66" t="s">
+        <v>935</v>
+      </c>
+      <c r="I66" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['때'], ['момент', 'отрезок времени'], 'время', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="10" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3386</v>
+      </c>
+      <c r="C67" t="s">
+        <v>557</v>
+      </c>
+      <c r="D67">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G67" t="s">
+        <v>935</v>
+      </c>
+      <c r="I67" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['신경을 쓰다'], ['заботиться', 'уделять внимание'], 'действие', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="s">
+        <v>3307</v>
+      </c>
+      <c r="B68" t="s">
+        <v>3362</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G68" t="s">
+        <v>935</v>
+      </c>
+      <c r="I68" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['이야기를 나누다'], ['беседовать'], 'общение', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
+        <v>3308</v>
+      </c>
+      <c r="B69" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C69" t="s">
+        <v>568</v>
+      </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G69" t="s">
+        <v>935</v>
+      </c>
+      <c r="I69" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['경우'], ['случай', 'ситуация'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="10" t="s">
+        <v>3309</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3363</v>
+      </c>
+      <c r="C70" t="s">
+        <v>568</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70" t="s">
+        <v>3253</v>
+      </c>
+      <c r="G70" t="s">
+        <v>935</v>
+      </c>
+      <c r="I70" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['드물다'], ['редкий'], 'другое', '3', ['3 초대', '3 приглашение']]</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3388</v>
+      </c>
+      <c r="C71" t="s">
+        <v>568</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+      <c r="E71">
+        <v>11</v>
+      </c>
+      <c r="F71" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G71" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I71" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['제목'], ['заголовок', 'название фильма'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3389</v>
+      </c>
+      <c r="C72" t="s">
+        <v>568</v>
+      </c>
+      <c r="D72">
+        <v>4</v>
+      </c>
+      <c r="E72">
+        <v>11</v>
+      </c>
+      <c r="F72" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G72" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I72" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['줄거리'], ['сюжет', 'ход развития событий'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B73" t="s">
+        <v>3390</v>
+      </c>
+      <c r="C73" t="s">
+        <v>568</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+      <c r="E73">
+        <v>11</v>
+      </c>
+      <c r="F73" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G73" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I73" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['배경'], ['фон', 'задний план', 'разворачиваются события'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3064</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <v>11</v>
+      </c>
+      <c r="F74" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G74" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I74" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['감독'], ['режисер'], 'профессия', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>429</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>11</v>
+      </c>
+      <c r="F75" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G75" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I75" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['배우'], ['актер', 'актриса'], 'профессия', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>3315</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3392</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>11</v>
+      </c>
+      <c r="F76" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G76" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I76" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['연기자'], ['исполнитель', 'исполнитель роли'], 'профессия', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3393</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D77">
+        <v>4</v>
+      </c>
+      <c r="E77">
+        <v>11</v>
+      </c>
+      <c r="F77" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G77" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I77" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['주인공'], ['персонаж', 'главный персонаж'], 'профессия', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>3317</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3328</v>
+      </c>
+      <c r="C78" t="s">
+        <v>578</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G78" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I78" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['시청자'], ['телезритель'], 'люди', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B79" t="s">
+        <v>3329</v>
+      </c>
+      <c r="C79" t="s">
+        <v>578</v>
+      </c>
+      <c r="D79">
+        <v>4</v>
+      </c>
+      <c r="E79">
+        <v>11</v>
+      </c>
+      <c r="F79" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G79" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I79" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['관객'], ['зрители в кино'], 'люди', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>3319</v>
+      </c>
+      <c r="B80" t="s">
+        <v>3330</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80">
+        <v>11</v>
+      </c>
+      <c r="F80" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G80" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I80" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['영화 감상'], ['просмотр фильма с наслаждением'], 'досуг', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B81" t="s">
+        <v>3331</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G81" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I81" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['영화 음악'], ['прослушивание музыки с наслаждением'], 'досуг', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>3332</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3394</v>
+      </c>
+      <c r="C82" t="s">
+        <v>568</v>
+      </c>
+      <c r="D82">
+        <v>4</v>
+      </c>
+      <c r="E82">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G82" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I82" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['감동적이다'], ['трогательный', 'задевающий', 'пронзительный'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3395</v>
+      </c>
+      <c r="C83" t="s">
+        <v>568</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G83" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I83" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['인상적이다'], ['впечатление', 'впечатляющий'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3341</v>
+      </c>
+      <c r="C84" t="s">
+        <v>568</v>
+      </c>
+      <c r="D84">
+        <v>4</v>
+      </c>
+      <c r="E84">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G84" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I84" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['흥미롭다'], ['интересный'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>3336</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3396</v>
+      </c>
+      <c r="C85" t="s">
+        <v>568</v>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <v>11</v>
+      </c>
+      <c r="F85" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G85" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I85" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['신나다'], ['веселый', 'духоподъемный'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>3337</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3344</v>
+      </c>
+      <c r="C86" t="s">
+        <v>568</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86">
+        <v>11</v>
+      </c>
+      <c r="F86" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G86" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I86" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['연기를 잘하다'], ['хорошо играет'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>3334</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3343</v>
+      </c>
+      <c r="C87" t="s">
+        <v>568</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87">
+        <v>11</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G87" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I87" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['영상이 아름답다'], ['прекрасное видео'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>3338</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3345</v>
+      </c>
+      <c r="C88" t="s">
+        <v>568</v>
+      </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88">
+        <v>11</v>
+      </c>
+      <c r="F88" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G88" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I88" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>[['기억에 오래 남다'], ['запоминающееся'], 'другое', '3', ['11 영화와 드라마', '11 Кино и дорамы']]</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A32">
+  <conditionalFormatting sqref="A1:A88">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>